<commit_message>
what is going on...
</commit_message>
<xml_diff>
--- a/курсач медведь.xlsx
+++ b/курсач медведь.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megas\OneDrive\Рабочий стол\Projects\Java-English-Study\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="720" yWindow="135" windowWidth="27480" windowHeight="12600" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Ведомость электропотребителей" sheetId="1" r:id="rId1"/>
@@ -17,7 +12,7 @@
     <sheet name="Расчет освещения" sheetId="3" r:id="rId3"/>
     <sheet name="Выбор защиты" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="102">
   <si>
     <t>Наименование потребителя</t>
   </si>
@@ -279,6 +274,60 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Iрасч.расц, А</t>
+  </si>
+  <si>
+    <t>Iпуск, А</t>
+  </si>
+  <si>
+    <t>I прив.расц, А</t>
+  </si>
+  <si>
+    <t>Iприв.уст, А</t>
+  </si>
+  <si>
+    <t>Iрасч.уст, А</t>
+  </si>
+  <si>
+    <t>Коэф-т защиты</t>
+  </si>
+  <si>
+    <t>Iном.расц, А</t>
+  </si>
+  <si>
+    <t>Iдд, А</t>
+  </si>
+  <si>
+    <t>Марка провода</t>
+  </si>
+  <si>
+    <t>Марка выключателя</t>
+  </si>
+  <si>
+    <t>Iвыкл, А</t>
+  </si>
+  <si>
+    <t>ПР</t>
+  </si>
+  <si>
+    <t>Горизонтально фрезерный станок</t>
+  </si>
+  <si>
+    <t>Наименование электроприемника</t>
+  </si>
+  <si>
+    <t>Номер э/п</t>
+  </si>
+  <si>
+    <t>ГРЩ</t>
+  </si>
+  <si>
+    <t>Итого:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Итого: </t>
   </si>
 </sst>
 </file>
@@ -305,7 +354,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="38">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -802,11 +851,150 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1021,6 +1209,42 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1057,22 +1281,48 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1347,7 +1597,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1357,9 +1607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView zoomScale="95" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2195,8 +2443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="X28" sqref="X28"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2208,99 +2456,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="80" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="88" t="s">
+      <c r="B1" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="84" t="s">
+      <c r="C1" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="84" t="s">
+      <c r="D1" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84" t="s">
+      <c r="E1" s="78"/>
+      <c r="F1" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="84" t="s">
+      <c r="G1" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="84" t="s">
+      <c r="H1" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="84" t="s">
+      <c r="I1" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="84" t="s">
+      <c r="J1" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="84" t="s">
+      <c r="K1" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="78" t="s">
+      <c r="L1" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="84" t="s">
+      <c r="M1" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="78" t="s">
+      <c r="N1" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="78" t="s">
+      <c r="O1" s="90" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="80" t="s">
+      <c r="P1" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="82" t="s">
+      <c r="Q1" s="94" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="87"/>
-      <c r="B2" s="89"/>
-      <c r="C2" s="85"/>
+      <c r="A2" s="81"/>
+      <c r="B2" s="83"/>
+      <c r="C2" s="79"/>
       <c r="D2" s="29" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="79"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="83"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="79"/>
+      <c r="I2" s="79"/>
+      <c r="J2" s="79"/>
+      <c r="K2" s="79"/>
+      <c r="L2" s="91"/>
+      <c r="M2" s="79"/>
+      <c r="N2" s="91"/>
+      <c r="O2" s="91"/>
+      <c r="P2" s="93"/>
+      <c r="Q2" s="95"/>
     </row>
     <row r="3" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="87" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="76"/>
-      <c r="N3" s="76"/>
-      <c r="O3" s="76"/>
-      <c r="P3" s="76"/>
-      <c r="Q3" s="77"/>
+      <c r="B3" s="88"/>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="88"/>
+      <c r="G3" s="88"/>
+      <c r="H3" s="88"/>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="88"/>
+      <c r="L3" s="88"/>
+      <c r="M3" s="88"/>
+      <c r="N3" s="88"/>
+      <c r="O3" s="88"/>
+      <c r="P3" s="88"/>
+      <c r="Q3" s="89"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="58">
@@ -2813,25 +3061,25 @@
       </c>
     </row>
     <row r="14" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="75" t="s">
+      <c r="A14" s="87" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76"/>
-      <c r="D14" s="76"/>
-      <c r="E14" s="76"/>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
-      <c r="H14" s="76"/>
-      <c r="I14" s="76"/>
-      <c r="J14" s="76"/>
-      <c r="K14" s="76"/>
-      <c r="L14" s="76"/>
-      <c r="M14" s="76"/>
-      <c r="N14" s="76"/>
-      <c r="O14" s="76"/>
-      <c r="P14" s="76"/>
-      <c r="Q14" s="77"/>
+      <c r="B14" s="88"/>
+      <c r="C14" s="88"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="88"/>
+      <c r="F14" s="88"/>
+      <c r="G14" s="88"/>
+      <c r="H14" s="88"/>
+      <c r="I14" s="88"/>
+      <c r="J14" s="88"/>
+      <c r="K14" s="88"/>
+      <c r="L14" s="88"/>
+      <c r="M14" s="88"/>
+      <c r="N14" s="88"/>
+      <c r="O14" s="88"/>
+      <c r="P14" s="88"/>
+      <c r="Q14" s="89"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="41">
@@ -3287,25 +3535,25 @@
       </c>
     </row>
     <row r="24" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="75" t="s">
+      <c r="A24" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="76"/>
-      <c r="C24" s="76"/>
-      <c r="D24" s="76"/>
-      <c r="E24" s="76"/>
-      <c r="F24" s="76"/>
-      <c r="G24" s="76"/>
-      <c r="H24" s="76"/>
-      <c r="I24" s="76"/>
-      <c r="J24" s="76"/>
-      <c r="K24" s="76"/>
-      <c r="L24" s="76"/>
-      <c r="M24" s="76"/>
-      <c r="N24" s="76"/>
-      <c r="O24" s="76"/>
-      <c r="P24" s="76"/>
-      <c r="Q24" s="77"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="88"/>
+      <c r="D24" s="88"/>
+      <c r="E24" s="88"/>
+      <c r="F24" s="88"/>
+      <c r="G24" s="88"/>
+      <c r="H24" s="88"/>
+      <c r="I24" s="88"/>
+      <c r="J24" s="88"/>
+      <c r="K24" s="88"/>
+      <c r="L24" s="88"/>
+      <c r="M24" s="88"/>
+      <c r="N24" s="88"/>
+      <c r="O24" s="88"/>
+      <c r="P24" s="88"/>
+      <c r="Q24" s="89"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="41">
@@ -3419,25 +3667,25 @@
       </c>
     </row>
     <row r="27" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="75" t="s">
+      <c r="A27" s="87" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="76"/>
-      <c r="C27" s="76"/>
-      <c r="D27" s="76"/>
-      <c r="E27" s="76"/>
-      <c r="F27" s="76"/>
-      <c r="G27" s="76"/>
-      <c r="H27" s="76"/>
-      <c r="I27" s="76"/>
-      <c r="J27" s="76"/>
-      <c r="K27" s="76"/>
-      <c r="L27" s="76"/>
-      <c r="M27" s="76"/>
-      <c r="N27" s="76"/>
-      <c r="O27" s="76"/>
-      <c r="P27" s="76"/>
-      <c r="Q27" s="77"/>
+      <c r="B27" s="88"/>
+      <c r="C27" s="88"/>
+      <c r="D27" s="88"/>
+      <c r="E27" s="88"/>
+      <c r="F27" s="88"/>
+      <c r="G27" s="88"/>
+      <c r="H27" s="88"/>
+      <c r="I27" s="88"/>
+      <c r="J27" s="88"/>
+      <c r="K27" s="88"/>
+      <c r="L27" s="88"/>
+      <c r="M27" s="88"/>
+      <c r="N27" s="88"/>
+      <c r="O27" s="88"/>
+      <c r="P27" s="88"/>
+      <c r="Q27" s="89"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="41">
@@ -3551,25 +3799,25 @@
       </c>
     </row>
     <row r="30" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="75" t="s">
+      <c r="A30" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="B30" s="76"/>
-      <c r="C30" s="76"/>
-      <c r="D30" s="76"/>
-      <c r="E30" s="76"/>
-      <c r="F30" s="76"/>
-      <c r="G30" s="76"/>
-      <c r="H30" s="76"/>
-      <c r="I30" s="76"/>
-      <c r="J30" s="76"/>
-      <c r="K30" s="76"/>
-      <c r="L30" s="76"/>
-      <c r="M30" s="76"/>
-      <c r="N30" s="76"/>
-      <c r="O30" s="76"/>
-      <c r="P30" s="76"/>
-      <c r="Q30" s="77"/>
+      <c r="B30" s="88"/>
+      <c r="C30" s="88"/>
+      <c r="D30" s="88"/>
+      <c r="E30" s="88"/>
+      <c r="F30" s="88"/>
+      <c r="G30" s="88"/>
+      <c r="H30" s="88"/>
+      <c r="I30" s="88"/>
+      <c r="J30" s="88"/>
+      <c r="K30" s="88"/>
+      <c r="L30" s="88"/>
+      <c r="M30" s="88"/>
+      <c r="N30" s="88"/>
+      <c r="O30" s="88"/>
+      <c r="P30" s="88"/>
+      <c r="Q30" s="89"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="41">
@@ -3752,25 +4000,25 @@
       </c>
     </row>
     <row r="34" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="72" t="s">
+      <c r="A34" s="84" t="s">
         <v>71</v>
       </c>
-      <c r="B34" s="73"/>
-      <c r="C34" s="73"/>
-      <c r="D34" s="73"/>
-      <c r="E34" s="73"/>
-      <c r="F34" s="73"/>
-      <c r="G34" s="73"/>
-      <c r="H34" s="73"/>
-      <c r="I34" s="73"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="73"/>
-      <c r="L34" s="73"/>
-      <c r="M34" s="73"/>
-      <c r="N34" s="73"/>
-      <c r="O34" s="73"/>
-      <c r="P34" s="73"/>
-      <c r="Q34" s="74"/>
+      <c r="B34" s="85"/>
+      <c r="C34" s="85"/>
+      <c r="D34" s="85"/>
+      <c r="E34" s="85"/>
+      <c r="F34" s="85"/>
+      <c r="G34" s="85"/>
+      <c r="H34" s="85"/>
+      <c r="I34" s="85"/>
+      <c r="J34" s="85"/>
+      <c r="K34" s="85"/>
+      <c r="L34" s="85"/>
+      <c r="M34" s="85"/>
+      <c r="N34" s="85"/>
+      <c r="O34" s="85"/>
+      <c r="P34" s="85"/>
+      <c r="Q34" s="86"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
@@ -4032,12 +4280,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:F2"/>
     <mergeCell ref="A34:Q34"/>
     <mergeCell ref="A24:Q24"/>
     <mergeCell ref="A27:Q27"/>
@@ -4054,6 +4296,12 @@
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4067,9 +4315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="A1:G5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4196,12 +4442,1022 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P29" sqref="P29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.21875" customWidth="1"/>
+    <col min="12" max="12" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="105" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="98" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="99" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="99" t="s">
+        <v>85</v>
+      </c>
+      <c r="E1" s="99" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="99" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="99" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="99" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="99" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="99" t="s">
+        <v>90</v>
+      </c>
+      <c r="K1" s="99" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="99" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1" s="99" t="s">
+        <v>93</v>
+      </c>
+      <c r="N1" s="100" t="s">
+        <v>94</v>
+      </c>
+      <c r="O1" s="96"/>
+    </row>
+    <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="84" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="96"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="58">
+        <v>2</v>
+      </c>
+      <c r="B3" s="74" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="32">
+        <f>'Ведомость электропотребителей'!E3</f>
+        <v>14.253834554439168</v>
+      </c>
+      <c r="D3" s="7">
+        <f>'Ведомость электропотребителей'!J3</f>
+        <v>99.776841881074176</v>
+      </c>
+      <c r="E3" s="7">
+        <f>C3/0.85</f>
+        <v>16.769217122869609</v>
+      </c>
+      <c r="F3" s="70">
+        <v>20</v>
+      </c>
+      <c r="G3" s="7">
+        <f>D3*1.25</f>
+        <v>124.72105235134272</v>
+      </c>
+      <c r="H3" s="7"/>
+      <c r="I3" s="70">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="96"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="59">
+        <v>3</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="76">
+        <f>'Ведомость электропотребителей'!E4</f>
+        <v>13.327568540850086</v>
+      </c>
+      <c r="D4" s="72">
+        <f>'Ведомость электропотребителей'!J4</f>
+        <v>93.292979785950607</v>
+      </c>
+      <c r="E4" s="7">
+        <f t="shared" ref="E4:E12" si="0">C4/0.85</f>
+        <v>15.679492401000102</v>
+      </c>
+      <c r="F4" s="110">
+        <v>16</v>
+      </c>
+      <c r="G4" s="7">
+        <f t="shared" ref="G4:G11" si="1">D4*1.25</f>
+        <v>116.61622473243825</v>
+      </c>
+      <c r="H4" s="72"/>
+      <c r="I4" s="70">
+        <v>1</v>
+      </c>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="72"/>
+      <c r="M4" s="72"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="96"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A5" s="59">
+        <v>4</v>
+      </c>
+      <c r="B5" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="76">
+        <f>'Ведомость электропотребителей'!E6</f>
+        <v>25.181264796006161</v>
+      </c>
+      <c r="D5" s="7">
+        <f>'Ведомость электропотребителей'!J6</f>
+        <v>176.26885357204313</v>
+      </c>
+      <c r="E5" s="7">
+        <f t="shared" si="0"/>
+        <v>29.625017407066071</v>
+      </c>
+      <c r="F5" s="110">
+        <v>32</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" si="1"/>
+        <v>220.3360669650539</v>
+      </c>
+      <c r="H5" s="72"/>
+      <c r="I5" s="70">
+        <v>1</v>
+      </c>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+      <c r="L5" s="72"/>
+      <c r="M5" s="72"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="96"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A6" s="59">
+        <v>5</v>
+      </c>
+      <c r="B6" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="76">
+        <f>'Ведомость электропотребителей'!E7</f>
+        <v>21.649172312697946</v>
+      </c>
+      <c r="D6" s="72">
+        <f>'Ведомость электропотребителей'!J7</f>
+        <v>108.24586156348973</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" si="0"/>
+        <v>25.469614485526996</v>
+      </c>
+      <c r="F6" s="110">
+        <v>32</v>
+      </c>
+      <c r="G6" s="7">
+        <f t="shared" si="1"/>
+        <v>135.30732695436217</v>
+      </c>
+      <c r="H6" s="72"/>
+      <c r="I6" s="70">
+        <v>1</v>
+      </c>
+      <c r="J6" s="72"/>
+      <c r="K6" s="72"/>
+      <c r="L6" s="72"/>
+      <c r="M6" s="72"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="96"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A7" s="59">
+        <v>10</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" s="76">
+        <f>'Ведомость электропотребителей'!E11</f>
+        <v>7.8188402106320503</v>
+      </c>
+      <c r="D7" s="7">
+        <f>'Ведомость электропотребителей'!J11</f>
+        <v>54.731881474424355</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="0"/>
+        <v>9.1986355419200585</v>
+      </c>
+      <c r="F7" s="110">
+        <v>10</v>
+      </c>
+      <c r="G7" s="7">
+        <f t="shared" si="1"/>
+        <v>68.414851843030448</v>
+      </c>
+      <c r="H7" s="72"/>
+      <c r="I7" s="70">
+        <v>1</v>
+      </c>
+      <c r="J7" s="72"/>
+      <c r="K7" s="72"/>
+      <c r="L7" s="72"/>
+      <c r="M7" s="72"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="96"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A8" s="59">
+        <v>7</v>
+      </c>
+      <c r="B8" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="76">
+        <f>'Ведомость электропотребителей'!E8</f>
+        <v>19.889988205471482</v>
+      </c>
+      <c r="D8" s="72">
+        <f>'Ведомость электропотребителей'!J8</f>
+        <v>139.22991743830039</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="0"/>
+        <v>23.399986124084098</v>
+      </c>
+      <c r="F8" s="110">
+        <v>25</v>
+      </c>
+      <c r="G8" s="7">
+        <f t="shared" si="1"/>
+        <v>174.03739679787549</v>
+      </c>
+      <c r="H8" s="72"/>
+      <c r="I8" s="70">
+        <v>1</v>
+      </c>
+      <c r="J8" s="72"/>
+      <c r="K8" s="72"/>
+      <c r="L8" s="72"/>
+      <c r="M8" s="72"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="96"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="59">
+        <v>8</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="76">
+        <f>'Ведомость электропотребителей'!E9</f>
+        <v>16.319471682673576</v>
+      </c>
+      <c r="D9" s="7">
+        <f>'Ведомость электропотребителей'!J9</f>
+        <v>114.23630177871503</v>
+      </c>
+      <c r="E9" s="7">
+        <f t="shared" si="0"/>
+        <v>19.199378450204208</v>
+      </c>
+      <c r="F9" s="110">
+        <v>20</v>
+      </c>
+      <c r="G9" s="7">
+        <f t="shared" si="1"/>
+        <v>142.79537722339379</v>
+      </c>
+      <c r="H9" s="72"/>
+      <c r="I9" s="70">
+        <v>1</v>
+      </c>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72"/>
+      <c r="L9" s="72"/>
+      <c r="M9" s="72"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="96"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" s="59">
+        <v>9</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="76">
+        <f>'Ведомость электропотребителей'!E10</f>
+        <v>19.133892377442123</v>
+      </c>
+      <c r="D10" s="72">
+        <f>'Ведомость электропотребителей'!J10</f>
+        <v>133.93724664209486</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="0"/>
+        <v>22.510461620520147</v>
+      </c>
+      <c r="F10" s="110">
+        <v>25</v>
+      </c>
+      <c r="G10" s="7">
+        <f t="shared" si="1"/>
+        <v>167.42155830261856</v>
+      </c>
+      <c r="H10" s="72"/>
+      <c r="I10" s="70">
+        <v>1</v>
+      </c>
+      <c r="J10" s="72"/>
+      <c r="K10" s="72"/>
+      <c r="L10" s="72"/>
+      <c r="M10" s="72"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="96"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A11" s="60">
+        <v>20</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="77">
+        <f>'Ведомость электропотребителей'!E21</f>
+        <v>13.708356213445803</v>
+      </c>
+      <c r="D11" s="26">
+        <f>'Ведомость электропотребителей'!J21</f>
+        <v>95.958493494120631</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="0"/>
+        <v>16.127477898171534</v>
+      </c>
+      <c r="F11" s="71">
+        <v>20</v>
+      </c>
+      <c r="G11" s="7">
+        <f t="shared" si="1"/>
+        <v>119.94811686765078</v>
+      </c>
+      <c r="H11" s="73"/>
+      <c r="I11" s="70">
+        <v>1</v>
+      </c>
+      <c r="J11" s="73"/>
+      <c r="K11" s="73"/>
+      <c r="L11" s="73"/>
+      <c r="M11" s="73"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="96"/>
+    </row>
+    <row r="12" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="60"/>
+      <c r="B12" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="77">
+        <f>'Расчет электрических нагрузок'!Q13</f>
+        <v>79.771373220004264</v>
+      </c>
+      <c r="D12" s="73">
+        <f>SUM(C3:C11)+MAX(D3:D11)-MAX(C3:C11)</f>
+        <v>302.36997766969534</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="0"/>
+        <v>93.848674376475614</v>
+      </c>
+      <c r="F12" s="71">
+        <v>100</v>
+      </c>
+      <c r="G12" s="7">
+        <f>D12*1.25</f>
+        <v>377.96247208711918</v>
+      </c>
+      <c r="H12" s="73"/>
+      <c r="I12" s="70">
+        <v>1</v>
+      </c>
+      <c r="J12" s="73"/>
+      <c r="K12" s="73"/>
+      <c r="L12" s="73"/>
+      <c r="M12" s="73"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="96"/>
+    </row>
+    <row r="13" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="84" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="85"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
+      <c r="F13" s="85"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="85"/>
+      <c r="I13" s="85"/>
+      <c r="J13" s="85"/>
+      <c r="K13" s="85"/>
+      <c r="L13" s="85"/>
+      <c r="M13" s="85"/>
+      <c r="N13" s="86"/>
+      <c r="O13" s="96"/>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A14" s="41">
+        <v>6</v>
+      </c>
+      <c r="B14" s="74" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="32">
+        <f>'Ведомость электропотребителей'!E7</f>
+        <v>21.649172312697946</v>
+      </c>
+      <c r="D14" s="7">
+        <f>'Ведомость электропотребителей'!J7</f>
+        <v>108.24586156348973</v>
+      </c>
+      <c r="E14" s="7">
+        <f>C14/0.85</f>
+        <v>25.469614485526996</v>
+      </c>
+      <c r="F14" s="70">
+        <v>32</v>
+      </c>
+      <c r="G14" s="7">
+        <f>D14*1.25</f>
+        <v>135.30732695436217</v>
+      </c>
+      <c r="H14" s="7"/>
+      <c r="I14" s="70">
+        <v>1</v>
+      </c>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="96"/>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="42">
+        <v>11</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="76">
+        <f>'Ведомость электропотребителей'!E12</f>
+        <v>22.80613528710267</v>
+      </c>
+      <c r="D15" s="72">
+        <f>'Ведомость электропотребителей'!J12</f>
+        <v>159.64294700971868</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" ref="E15:E22" si="2">C15/0.85</f>
+        <v>26.830747396591377</v>
+      </c>
+      <c r="F15" s="110">
+        <v>32</v>
+      </c>
+      <c r="G15" s="7">
+        <f t="shared" ref="G15:G22" si="3">D15*1.25</f>
+        <v>199.55368376214835</v>
+      </c>
+      <c r="H15" s="72"/>
+      <c r="I15" s="70">
+        <v>1</v>
+      </c>
+      <c r="J15" s="72"/>
+      <c r="K15" s="72"/>
+      <c r="L15" s="72"/>
+      <c r="M15" s="72"/>
+      <c r="N15" s="20"/>
+      <c r="O15" s="96"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="42">
+        <v>13</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="76">
+        <f>'Ведомость электропотребителей'!E14</f>
+        <v>13.419482806649054</v>
+      </c>
+      <c r="D16" s="7">
+        <f>'Ведомость электропотребителей'!J14</f>
+        <v>93.936379646543372</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="2"/>
+        <v>15.787626831351828</v>
+      </c>
+      <c r="F16" s="110">
+        <v>20</v>
+      </c>
+      <c r="G16" s="7">
+        <f t="shared" si="3"/>
+        <v>117.42047455817922</v>
+      </c>
+      <c r="H16" s="72"/>
+      <c r="I16" s="70">
+        <v>1</v>
+      </c>
+      <c r="J16" s="72"/>
+      <c r="K16" s="72"/>
+      <c r="L16" s="72"/>
+      <c r="M16" s="72"/>
+      <c r="N16" s="20"/>
+      <c r="O16" s="96"/>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="42">
+        <v>15</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="76">
+        <f>'Ведомость электропотребителей'!E16</f>
+        <v>8.3609404668927887</v>
+      </c>
+      <c r="D17" s="72">
+        <f>'Ведомость электропотребителей'!J16</f>
+        <v>58.526583268249524</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="2"/>
+        <v>9.8364005492856332</v>
+      </c>
+      <c r="F17" s="110">
+        <v>10</v>
+      </c>
+      <c r="G17" s="7">
+        <f t="shared" si="3"/>
+        <v>73.158229085311902</v>
+      </c>
+      <c r="H17" s="72"/>
+      <c r="I17" s="70">
+        <v>1</v>
+      </c>
+      <c r="J17" s="72"/>
+      <c r="K17" s="72"/>
+      <c r="L17" s="72"/>
+      <c r="M17" s="72"/>
+      <c r="N17" s="20"/>
+      <c r="O17" s="96"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A18" s="42">
+        <v>16</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="76">
+        <f>'Ведомость электропотребителей'!E17</f>
+        <v>12.329550617558521</v>
+      </c>
+      <c r="D18" s="7">
+        <f>'Ведомость электропотребителей'!J17</f>
+        <v>86.306854322909643</v>
+      </c>
+      <c r="E18" s="7">
+        <f t="shared" si="2"/>
+        <v>14.505353667715907</v>
+      </c>
+      <c r="F18" s="110">
+        <v>16</v>
+      </c>
+      <c r="G18" s="7">
+        <f t="shared" si="3"/>
+        <v>107.88356790363706</v>
+      </c>
+      <c r="H18" s="72"/>
+      <c r="I18" s="70">
+        <v>1</v>
+      </c>
+      <c r="J18" s="72"/>
+      <c r="K18" s="72"/>
+      <c r="L18" s="72"/>
+      <c r="M18" s="72"/>
+      <c r="N18" s="20"/>
+      <c r="O18" s="96"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="42">
+        <v>17</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="76">
+        <f>'Ведомость электропотребителей'!E18</f>
+        <v>12.300852149554968</v>
+      </c>
+      <c r="D19" s="72">
+        <f>'Ведомость электропотребителей'!J18</f>
+        <v>86.105965046884776</v>
+      </c>
+      <c r="E19" s="7">
+        <f t="shared" si="2"/>
+        <v>14.471590764182316</v>
+      </c>
+      <c r="F19" s="110">
+        <v>16</v>
+      </c>
+      <c r="G19" s="7">
+        <f t="shared" si="3"/>
+        <v>107.63245630860597</v>
+      </c>
+      <c r="H19" s="72"/>
+      <c r="I19" s="70">
+        <v>1</v>
+      </c>
+      <c r="J19" s="72"/>
+      <c r="K19" s="72"/>
+      <c r="L19" s="72"/>
+      <c r="M19" s="72"/>
+      <c r="N19" s="20"/>
+      <c r="O19" s="96"/>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A20" s="42">
+        <v>18</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="76">
+        <f>'Ведомость электропотребителей'!E19</f>
+        <v>18.658595957190119</v>
+      </c>
+      <c r="D20" s="7">
+        <f>'Ведомость электропотребителей'!J19</f>
+        <v>130.61017170033082</v>
+      </c>
+      <c r="E20" s="7">
+        <f t="shared" si="2"/>
+        <v>21.951289361400139</v>
+      </c>
+      <c r="F20" s="110">
+        <v>25</v>
+      </c>
+      <c r="G20" s="7">
+        <f t="shared" si="3"/>
+        <v>163.26271462541354</v>
+      </c>
+      <c r="H20" s="72"/>
+      <c r="I20" s="70">
+        <v>1</v>
+      </c>
+      <c r="J20" s="72"/>
+      <c r="K20" s="72"/>
+      <c r="L20" s="72"/>
+      <c r="M20" s="72"/>
+      <c r="N20" s="20"/>
+      <c r="O20" s="96"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A21" s="43">
+        <v>19</v>
+      </c>
+      <c r="B21" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="77">
+        <f>'Ведомость электропотребителей'!E20</f>
+        <v>11.763800498723676</v>
+      </c>
+      <c r="D21" s="73">
+        <f>'Ведомость электропотребителей'!J20</f>
+        <v>82.346603491065736</v>
+      </c>
+      <c r="E21" s="7">
+        <f t="shared" si="2"/>
+        <v>13.839765292616089</v>
+      </c>
+      <c r="F21" s="71">
+        <v>16</v>
+      </c>
+      <c r="G21" s="7">
+        <f t="shared" si="3"/>
+        <v>102.93325436383216</v>
+      </c>
+      <c r="H21" s="73"/>
+      <c r="I21" s="70">
+        <v>1</v>
+      </c>
+      <c r="J21" s="73"/>
+      <c r="K21" s="73"/>
+      <c r="L21" s="73"/>
+      <c r="M21" s="73"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="96"/>
+    </row>
+    <row r="22" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="107"/>
+      <c r="B22" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="77">
+        <f>'Расчет электрических нагрузок'!Q23</f>
+        <v>67.730461429231127</v>
+      </c>
+      <c r="D22" s="73">
+        <f>SUM(C14:C21)+MAX(D14:D21)-MAX(C14:C21)</f>
+        <v>258.12534181898576</v>
+      </c>
+      <c r="E22" s="7">
+        <f t="shared" si="2"/>
+        <v>79.682895799095448</v>
+      </c>
+      <c r="F22" s="71">
+        <v>100</v>
+      </c>
+      <c r="G22" s="7">
+        <f t="shared" si="3"/>
+        <v>322.65667727373221</v>
+      </c>
+      <c r="H22" s="73"/>
+      <c r="I22" s="70">
+        <v>1</v>
+      </c>
+      <c r="J22" s="73"/>
+      <c r="K22" s="73"/>
+      <c r="L22" s="73"/>
+      <c r="M22" s="73"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="96"/>
+    </row>
+    <row r="23" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="84" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" s="85"/>
+      <c r="C23" s="85"/>
+      <c r="D23" s="85"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="85"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="85"/>
+      <c r="L23" s="85"/>
+      <c r="M23" s="85"/>
+      <c r="N23" s="86"/>
+      <c r="O23" s="96"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24" s="106">
+        <v>1</v>
+      </c>
+      <c r="B24" s="101" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="7">
+        <f>'Ведомость электропотребителей'!E2</f>
+        <v>58.488986510702098</v>
+      </c>
+      <c r="D24" s="7">
+        <f>'Ведомость электропотребителей'!J2</f>
+        <v>146.22246627675526</v>
+      </c>
+      <c r="E24" s="7">
+        <f>C24/0.85</f>
+        <v>68.810572365531883</v>
+      </c>
+      <c r="F24" s="70">
+        <f>100</f>
+        <v>100</v>
+      </c>
+      <c r="G24" s="7">
+        <f>D24*1.25</f>
+        <v>182.77808284594408</v>
+      </c>
+      <c r="H24" s="7"/>
+      <c r="I24" s="70">
+        <v>1</v>
+      </c>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="96"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25" s="106">
+        <v>12</v>
+      </c>
+      <c r="B25" s="97" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="72">
+        <f>'Ведомость электропотребителей'!E13</f>
+        <v>125.81224702562481</v>
+      </c>
+      <c r="D25" s="72">
+        <f>'Ведомость электропотребителей'!J13</f>
+        <v>440.34286458968683</v>
+      </c>
+      <c r="E25" s="7">
+        <f>C25/0.85</f>
+        <v>148.01440826544095</v>
+      </c>
+      <c r="F25" s="110">
+        <f>160</f>
+        <v>160</v>
+      </c>
+      <c r="G25" s="7">
+        <f t="shared" ref="G25:G26" si="4">D25*1.25</f>
+        <v>550.42858073710852</v>
+      </c>
+      <c r="H25" s="72"/>
+      <c r="I25" s="70">
+        <v>1</v>
+      </c>
+      <c r="J25" s="72"/>
+      <c r="K25" s="72"/>
+      <c r="L25" s="72"/>
+      <c r="M25" s="72"/>
+      <c r="N25" s="20"/>
+      <c r="O25" s="96"/>
+    </row>
+    <row r="26" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="106">
+        <v>14</v>
+      </c>
+      <c r="B26" s="102" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="73">
+        <f>'Ведомость электропотребителей'!E15</f>
+        <v>58.488986510702098</v>
+      </c>
+      <c r="D26" s="73">
+        <f>'Ведомость электропотребителей'!J15</f>
+        <v>146.22246627675526</v>
+      </c>
+      <c r="E26" s="7">
+        <f>C26/0.85</f>
+        <v>68.810572365531883</v>
+      </c>
+      <c r="F26" s="71">
+        <v>100</v>
+      </c>
+      <c r="G26" s="7">
+        <f t="shared" si="4"/>
+        <v>182.77808284594408</v>
+      </c>
+      <c r="H26" s="73"/>
+      <c r="I26" s="70">
+        <v>1</v>
+      </c>
+      <c r="J26" s="73"/>
+      <c r="K26" s="73"/>
+      <c r="L26" s="73"/>
+      <c r="M26" s="73"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="96"/>
+    </row>
+    <row r="27" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="84" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" s="85"/>
+      <c r="C27" s="85"/>
+      <c r="D27" s="85"/>
+      <c r="E27" s="85"/>
+      <c r="F27" s="85"/>
+      <c r="G27" s="85"/>
+      <c r="H27" s="85"/>
+      <c r="I27" s="85"/>
+      <c r="J27" s="85"/>
+      <c r="K27" s="85"/>
+      <c r="L27" s="85"/>
+      <c r="M27" s="85"/>
+      <c r="N27" s="86"/>
+      <c r="O27" s="96"/>
+    </row>
+    <row r="28" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="8"/>
+      <c r="B28" s="103"/>
+      <c r="C28" s="104">
+        <f>'Расчет электрических нагрузок'!Q33</f>
+        <v>169.4532332052338</v>
+      </c>
+      <c r="D28" s="104">
+        <f>SUM(C24:C26,C22,C12)+MAX(D24:D26,D22,D12)-MAX(C24:C26,C22,C12)</f>
+        <v>704.82267226032639</v>
+      </c>
+      <c r="E28" s="104">
+        <f>C28/0.85</f>
+        <v>199.35674494733388</v>
+      </c>
+      <c r="F28" s="111">
+        <v>250</v>
+      </c>
+      <c r="G28" s="104">
+        <f>D28*1.25</f>
+        <v>881.02834032540795</v>
+      </c>
+      <c r="H28" s="104"/>
+      <c r="I28" s="111">
+        <v>1</v>
+      </c>
+      <c r="J28" s="104"/>
+      <c r="K28" s="104"/>
+      <c r="L28" s="104"/>
+      <c r="M28" s="104"/>
+      <c r="N28" s="109"/>
+      <c r="O28" s="96"/>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B29" s="96"/>
+      <c r="C29" s="96"/>
+      <c r="D29" s="96"/>
+      <c r="E29" s="96"/>
+      <c r="F29" s="96"/>
+      <c r="G29" s="96"/>
+      <c r="H29" s="96"/>
+      <c r="I29" s="96"/>
+      <c r="J29" s="96"/>
+      <c r="K29" s="96"/>
+      <c r="L29" s="96"/>
+      <c r="M29" s="96"/>
+      <c r="N29" s="96"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D30" s="108"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A27:N27"/>
+    <mergeCell ref="A23:N23"/>
+    <mergeCell ref="A13:N13"/>
+    <mergeCell ref="A2:N2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D18" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
trying to fix coursach
</commit_message>
<xml_diff>
--- a/курсач медведь.xlsx
+++ b/курсач медведь.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megas\OneDrive\Рабочий стол\Projects\Java-English-Study\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="720" yWindow="135" windowWidth="27480" windowHeight="12600" activeTab="3"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12900" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="720" yWindow="135" windowWidth="27480" windowHeight="12600" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Ведомость электропотребителей" sheetId="1" r:id="rId1"/>
@@ -19,7 +13,7 @@
     <sheet name="Выбор защиты" sheetId="4" r:id="rId4"/>
     <sheet name="КЗ" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="153">
   <si>
     <t>Наименование потребителя</t>
   </si>
@@ -169,18 +163,6 @@
     <t>I расч. [А]</t>
   </si>
   <si>
-    <t>ШРА 1</t>
-  </si>
-  <si>
-    <t>Итого ШРА 1</t>
-  </si>
-  <si>
-    <t>ШРА 2</t>
-  </si>
-  <si>
-    <t>Итого ШРА 2</t>
-  </si>
-  <si>
     <t>ПР1</t>
   </si>
   <si>
@@ -457,7 +439,49 @@
     <t>ШР 2</t>
   </si>
   <si>
-    <t>ВВГ 25</t>
+    <t>ВВГнг-LS 4*25 мм2</t>
+  </si>
+  <si>
+    <t>ВВГнг-LS 5*95 мм2</t>
+  </si>
+  <si>
+    <t>ВВГнг-LS 5*25 мм2</t>
+  </si>
+  <si>
+    <t>ВВГнг-LS 4*16 мм2</t>
+  </si>
+  <si>
+    <t>ВВГнг-LS 4*10 мм2</t>
+  </si>
+  <si>
+    <t>ВВГнг-LS 4*6 мм2</t>
+  </si>
+  <si>
+    <t>ВВГнг-LS 4*95 мм2</t>
+  </si>
+  <si>
+    <t>ВА88-32 3Р 25А 25кА TDM</t>
+  </si>
+  <si>
+    <t>ВА88-32 3Р 16А 25кА TDM</t>
+  </si>
+  <si>
+    <t>ВА88-32 3Р 32А 25кА TDM</t>
+  </si>
+  <si>
+    <t>ВА88-32 3Р 100А 35кА TDM</t>
+  </si>
+  <si>
+    <t>ВА88-32 3Р 160А 35кА TDM</t>
+  </si>
+  <si>
+    <t>ВА88-32 3Р 250А 35кА TDM</t>
+  </si>
+  <si>
+    <t>Итого ШР 1</t>
+  </si>
+  <si>
+    <t>Итого ШР 2</t>
   </si>
 </sst>
 </file>
@@ -1145,7 +1169,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="129">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1413,9 +1437,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1429,9 +1450,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1508,6 +1526,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1782,7 +1809,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1795,7 +1822,6 @@
     <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2035,7 +2061,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B7" s="2">
         <v>6</v>
@@ -2631,11 +2657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:B38"/>
-    </sheetView>
-    <sheetView workbookViewId="1">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2647,106 +2670,106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="104" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="108" t="s">
+      <c r="B1" s="106" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="104" t="s">
+      <c r="C1" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="104" t="s">
+      <c r="D1" s="102" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="104"/>
-      <c r="F1" s="104" t="s">
+      <c r="E1" s="102"/>
+      <c r="F1" s="102" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="104" t="s">
+      <c r="G1" s="102" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="104" t="s">
+      <c r="H1" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="104" t="s">
+      <c r="I1" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="104" t="s">
+      <c r="J1" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="104" t="s">
+      <c r="K1" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="116" t="s">
+      <c r="L1" s="114" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="104" t="s">
+      <c r="M1" s="102" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="116" t="s">
+      <c r="N1" s="114" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="116" t="s">
+      <c r="O1" s="114" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="118" t="s">
+      <c r="P1" s="116" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="120" t="s">
+      <c r="Q1" s="118" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="107"/>
-      <c r="B2" s="109"/>
-      <c r="C2" s="105"/>
+      <c r="A2" s="105"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="103"/>
       <c r="D2" s="29" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="105"/>
-      <c r="G2" s="105"/>
-      <c r="H2" s="105"/>
-      <c r="I2" s="105"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="117"/>
-      <c r="M2" s="105"/>
-      <c r="N2" s="117"/>
-      <c r="O2" s="117"/>
-      <c r="P2" s="119"/>
-      <c r="Q2" s="121"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="115"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="115"/>
+      <c r="O2" s="115"/>
+      <c r="P2" s="117"/>
+      <c r="Q2" s="119"/>
     </row>
     <row r="3" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="113" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="114"/>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="114"/>
-      <c r="J3" s="114"/>
-      <c r="K3" s="114"/>
-      <c r="L3" s="114"/>
-      <c r="M3" s="114"/>
-      <c r="N3" s="114"/>
-      <c r="O3" s="114"/>
-      <c r="P3" s="114"/>
-      <c r="Q3" s="115"/>
+      <c r="A3" s="111" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="112"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
+      <c r="J3" s="112"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="112"/>
+      <c r="M3" s="112"/>
+      <c r="N3" s="112"/>
+      <c r="O3" s="112"/>
+      <c r="P3" s="112"/>
+      <c r="Q3" s="113"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="58">
         <v>2</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C4" s="65">
         <v>1</v>
@@ -2795,7 +2818,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C5" s="65">
         <v>1</v>
@@ -2844,7 +2867,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C6" s="65">
         <v>1</v>
@@ -2893,7 +2916,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C7" s="65">
         <v>1</v>
@@ -2942,7 +2965,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C8" s="65">
         <v>1</v>
@@ -2991,7 +3014,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C9" s="65">
         <v>1</v>
@@ -3040,7 +3063,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C10" s="65">
         <v>1</v>
@@ -3089,7 +3112,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C11" s="65">
         <v>1</v>
@@ -3138,7 +3161,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="35" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C12" s="68">
         <v>1</v>
@@ -3185,7 +3208,7 @@
     <row r="13" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="61"/>
       <c r="B13" s="39" t="s">
-        <v>47</v>
+        <v>151</v>
       </c>
       <c r="C13" s="69">
         <f>SUM(C4:C12)</f>
@@ -3252,32 +3275,32 @@
       </c>
     </row>
     <row r="14" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="113" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="114"/>
-      <c r="C14" s="114"/>
-      <c r="D14" s="114"/>
-      <c r="E14" s="114"/>
-      <c r="F14" s="114"/>
-      <c r="G14" s="114"/>
-      <c r="H14" s="114"/>
-      <c r="I14" s="114"/>
-      <c r="J14" s="114"/>
-      <c r="K14" s="114"/>
-      <c r="L14" s="114"/>
-      <c r="M14" s="114"/>
-      <c r="N14" s="114"/>
-      <c r="O14" s="114"/>
-      <c r="P14" s="114"/>
-      <c r="Q14" s="115"/>
+      <c r="A14" s="111" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="112"/>
+      <c r="C14" s="112"/>
+      <c r="D14" s="112"/>
+      <c r="E14" s="112"/>
+      <c r="F14" s="112"/>
+      <c r="G14" s="112"/>
+      <c r="H14" s="112"/>
+      <c r="I14" s="112"/>
+      <c r="J14" s="112"/>
+      <c r="K14" s="112"/>
+      <c r="L14" s="112"/>
+      <c r="M14" s="112"/>
+      <c r="N14" s="112"/>
+      <c r="O14" s="112"/>
+      <c r="P14" s="112"/>
+      <c r="Q14" s="113"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="41">
         <v>6</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C15" s="65">
         <v>1</v>
@@ -3325,7 +3348,7 @@
         <v>11</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C16" s="65">
         <v>1</v>
@@ -3373,7 +3396,7 @@
         <v>13</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C17" s="65">
         <v>1</v>
@@ -3421,7 +3444,7 @@
         <v>15</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C18" s="65">
         <v>1</v>
@@ -3469,7 +3492,7 @@
         <v>16</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C19" s="65">
         <v>1</v>
@@ -3517,7 +3540,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C20" s="65">
         <v>1</v>
@@ -3565,7 +3588,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C21" s="65">
         <v>1</v>
@@ -3613,7 +3636,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C22" s="68">
         <v>1</v>
@@ -3659,7 +3682,7 @@
     <row r="23" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="39"/>
       <c r="B23" s="39" t="s">
-        <v>49</v>
+        <v>152</v>
       </c>
       <c r="C23" s="69">
         <f>SUM(C15:C22)</f>
@@ -3726,32 +3749,32 @@
       </c>
     </row>
     <row r="24" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="113" t="s">
-        <v>50</v>
-      </c>
-      <c r="B24" s="114"/>
-      <c r="C24" s="114"/>
-      <c r="D24" s="114"/>
-      <c r="E24" s="114"/>
-      <c r="F24" s="114"/>
-      <c r="G24" s="114"/>
-      <c r="H24" s="114"/>
-      <c r="I24" s="114"/>
-      <c r="J24" s="114"/>
-      <c r="K24" s="114"/>
-      <c r="L24" s="114"/>
-      <c r="M24" s="114"/>
-      <c r="N24" s="114"/>
-      <c r="O24" s="114"/>
-      <c r="P24" s="114"/>
-      <c r="Q24" s="115"/>
+      <c r="A24" s="111" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="112"/>
+      <c r="C24" s="112"/>
+      <c r="D24" s="112"/>
+      <c r="E24" s="112"/>
+      <c r="F24" s="112"/>
+      <c r="G24" s="112"/>
+      <c r="H24" s="112"/>
+      <c r="I24" s="112"/>
+      <c r="J24" s="112"/>
+      <c r="K24" s="112"/>
+      <c r="L24" s="112"/>
+      <c r="M24" s="112"/>
+      <c r="N24" s="112"/>
+      <c r="O24" s="112"/>
+      <c r="P24" s="112"/>
+      <c r="Q24" s="113"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="41">
         <v>1</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C25" s="65">
         <v>1</v>
@@ -3796,7 +3819,7 @@
     <row r="26" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="40"/>
       <c r="B26" s="40" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C26" s="67">
         <f>SUM(C25)</f>
@@ -3858,32 +3881,32 @@
       </c>
     </row>
     <row r="27" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="113" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="114"/>
-      <c r="C27" s="114"/>
-      <c r="D27" s="114"/>
-      <c r="E27" s="114"/>
-      <c r="F27" s="114"/>
-      <c r="G27" s="114"/>
-      <c r="H27" s="114"/>
-      <c r="I27" s="114"/>
-      <c r="J27" s="114"/>
-      <c r="K27" s="114"/>
-      <c r="L27" s="114"/>
-      <c r="M27" s="114"/>
-      <c r="N27" s="114"/>
-      <c r="O27" s="114"/>
-      <c r="P27" s="114"/>
-      <c r="Q27" s="115"/>
+      <c r="A27" s="111" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="112"/>
+      <c r="C27" s="112"/>
+      <c r="D27" s="112"/>
+      <c r="E27" s="112"/>
+      <c r="F27" s="112"/>
+      <c r="G27" s="112"/>
+      <c r="H27" s="112"/>
+      <c r="I27" s="112"/>
+      <c r="J27" s="112"/>
+      <c r="K27" s="112"/>
+      <c r="L27" s="112"/>
+      <c r="M27" s="112"/>
+      <c r="N27" s="112"/>
+      <c r="O27" s="112"/>
+      <c r="P27" s="112"/>
+      <c r="Q27" s="113"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="41">
         <v>12</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C28" s="70">
         <v>1</v>
@@ -3928,7 +3951,7 @@
     <row r="29" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="40"/>
       <c r="B29" s="36" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C29" s="71">
         <f>SUM(C28)</f>
@@ -3990,32 +4013,32 @@
       </c>
     </row>
     <row r="30" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="113" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="114"/>
-      <c r="C30" s="114"/>
-      <c r="D30" s="114"/>
-      <c r="E30" s="114"/>
-      <c r="F30" s="114"/>
-      <c r="G30" s="114"/>
-      <c r="H30" s="114"/>
-      <c r="I30" s="114"/>
-      <c r="J30" s="114"/>
-      <c r="K30" s="114"/>
-      <c r="L30" s="114"/>
-      <c r="M30" s="114"/>
-      <c r="N30" s="114"/>
-      <c r="O30" s="114"/>
-      <c r="P30" s="114"/>
-      <c r="Q30" s="115"/>
+      <c r="A30" s="111" t="s">
+        <v>50</v>
+      </c>
+      <c r="B30" s="112"/>
+      <c r="C30" s="112"/>
+      <c r="D30" s="112"/>
+      <c r="E30" s="112"/>
+      <c r="F30" s="112"/>
+      <c r="G30" s="112"/>
+      <c r="H30" s="112"/>
+      <c r="I30" s="112"/>
+      <c r="J30" s="112"/>
+      <c r="K30" s="112"/>
+      <c r="L30" s="112"/>
+      <c r="M30" s="112"/>
+      <c r="N30" s="112"/>
+      <c r="O30" s="112"/>
+      <c r="P30" s="112"/>
+      <c r="Q30" s="113"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="41">
         <v>14</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C31" s="65">
         <v>1</v>
@@ -4060,7 +4083,7 @@
     <row r="32" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="35"/>
       <c r="B32" s="35" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C32" s="67">
         <f>SUM(C31)</f>
@@ -4123,12 +4146,12 @@
     </row>
     <row r="33" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="39" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B33" s="39"/>
       <c r="C33" s="69">
-        <f>SUM(C32,C29,C23,C13)</f>
-        <v>19</v>
+        <f>SUM(C32,C29,C23,C13,C26)</f>
+        <v>20</v>
       </c>
       <c r="D33" s="30">
         <f>SUM(D32,D29,D26,D23,D13)</f>
@@ -4191,30 +4214,30 @@
       </c>
     </row>
     <row r="34" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="110" t="s">
-        <v>71</v>
-      </c>
-      <c r="B34" s="111"/>
-      <c r="C34" s="111"/>
-      <c r="D34" s="111"/>
-      <c r="E34" s="111"/>
-      <c r="F34" s="111"/>
-      <c r="G34" s="111"/>
-      <c r="H34" s="111"/>
-      <c r="I34" s="111"/>
-      <c r="J34" s="111"/>
-      <c r="K34" s="111"/>
-      <c r="L34" s="111"/>
-      <c r="M34" s="111"/>
-      <c r="N34" s="111"/>
-      <c r="O34" s="111"/>
-      <c r="P34" s="111"/>
-      <c r="Q34" s="112"/>
+      <c r="A34" s="108" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="109"/>
+      <c r="C34" s="109"/>
+      <c r="D34" s="109"/>
+      <c r="E34" s="109"/>
+      <c r="F34" s="109"/>
+      <c r="G34" s="109"/>
+      <c r="H34" s="109"/>
+      <c r="I34" s="109"/>
+      <c r="J34" s="109"/>
+      <c r="K34" s="109"/>
+      <c r="L34" s="109"/>
+      <c r="M34" s="109"/>
+      <c r="N34" s="109"/>
+      <c r="O34" s="109"/>
+      <c r="P34" s="109"/>
+      <c r="Q34" s="110"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="48" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C35" s="65">
         <f>'Расчет освещения'!G3</f>
@@ -4256,18 +4279,18 @@
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C36" s="66">
         <f>'Расчет освещения'!G4</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="D36" s="63">
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="E36" s="7">
         <f t="shared" ref="E36:E38" si="12">C36*D36</f>
-        <v>0.18</v>
+        <v>0.09</v>
       </c>
       <c r="F36" s="7">
         <v>0.7</v>
@@ -4281,11 +4304,11 @@
       </c>
       <c r="I36" s="7">
         <f t="shared" ref="I36:I38" si="14">E36*F36</f>
-        <v>0.126</v>
+        <v>6.3E-2</v>
       </c>
       <c r="J36" s="7">
-        <f t="shared" ref="J36:J39" si="15">I36*H36</f>
-        <v>2.5585391239884528E-2</v>
+        <f t="shared" ref="J36:J40" si="15">I36*H36</f>
+        <v>1.2792695619942264E-2</v>
       </c>
       <c r="K36" s="28"/>
       <c r="L36" s="28"/>
@@ -4298,7 +4321,7 @@
     <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
       <c r="B37" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C37" s="66">
         <f>'Расчет освещения'!G2</f>
@@ -4340,7 +4363,7 @@
     <row r="38" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="49"/>
       <c r="B38" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C38" s="67">
         <f>'Расчет освещения'!G5</f>
@@ -4381,17 +4404,17 @@
     </row>
     <row r="39" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="8" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="69">
         <f>SUM(C35:C38)</f>
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="30">
         <f>SUM(E35:E38)</f>
-        <v>3.5820000000000003</v>
+        <v>3.4920000000000004</v>
       </c>
       <c r="F39" s="30">
         <f>AVERAGE(F35:F38)</f>
@@ -4407,66 +4430,78 @@
       </c>
       <c r="I39" s="30">
         <f>SUM(I35:I38)</f>
-        <v>2.5074000000000001</v>
+        <v>2.4443999999999999</v>
       </c>
       <c r="J39" s="30">
         <f t="shared" si="15"/>
-        <v>0.5091492856737021</v>
+        <v>0.49635659005375982</v>
       </c>
       <c r="K39" s="30"/>
       <c r="L39" s="30"/>
       <c r="M39" s="30"/>
       <c r="N39" s="30">
         <f>I39</f>
-        <v>2.5074000000000001</v>
+        <v>2.4443999999999999</v>
       </c>
       <c r="O39" s="30">
         <f>J39</f>
-        <v>0.5091492856737021</v>
+        <v>0.49635659005375982</v>
       </c>
       <c r="P39" s="30">
         <f>SQRT(N39*N39+O39*O39)</f>
-        <v>2.5585714285714287</v>
+        <v>2.4942857142857142</v>
       </c>
       <c r="Q39" s="38">
         <f>P39*1000/(220*SQRT(3))</f>
-        <v>6.7145086501209086</v>
+        <v>6.5458024026304322</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B40" s="8"/>
       <c r="C40" s="69">
         <f>C39+C33</f>
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
-      <c r="G40" s="103"/>
-      <c r="H40" s="103"/>
-      <c r="I40" s="103"/>
-      <c r="J40" s="30"/>
+      <c r="G40" s="101">
+        <f>(G39*E39+G33*E33)/(E33+E39)</f>
+        <v>0.95067656062308648</v>
+      </c>
+      <c r="H40" s="101">
+        <f>(H39*E39+H33*E33)/(E33+E39)</f>
+        <v>0.32585099754430247</v>
+      </c>
+      <c r="I40" s="128">
+        <f>I39+I33</f>
+        <v>93.784124999999989</v>
+      </c>
+      <c r="J40" s="30">
+        <f t="shared" si="15"/>
+        <v>30.559650685069553</v>
+      </c>
       <c r="K40" s="30"/>
       <c r="L40" s="30"/>
       <c r="M40" s="30"/>
       <c r="N40" s="30">
         <f>N39+N33</f>
-        <v>108.46148099999998</v>
+        <v>108.39848099999998</v>
       </c>
       <c r="O40" s="30">
         <f>O39+O33</f>
-        <v>35.334571589207478</v>
+        <v>35.321778893587535</v>
       </c>
       <c r="P40" s="30">
         <f>SQRT(O40*O40+N40*N40)</f>
-        <v>114.07201589393512</v>
-      </c>
-      <c r="Q40" s="102">
+        <v>114.00815210902614</v>
+      </c>
+      <c r="Q40" s="100">
         <f>P40*1000/(380*SQRT(3))</f>
-        <v>173.31449758780713</v>
+        <v>173.21746660515277</v>
       </c>
     </row>
   </sheetData>
@@ -4507,7 +4542,6 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4517,27 +4551,27 @@
     <row r="1" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="8"/>
       <c r="B1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="G1" s="11" t="s">
         <v>79</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B2" s="46">
         <v>250</v>
@@ -4560,7 +4594,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B3" s="47">
         <v>300</v>
@@ -4583,7 +4617,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B4" s="47">
         <v>100</v>
@@ -4601,12 +4635,12 @@
         <v>1.6</v>
       </c>
       <c r="G4" s="50">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B5" s="52">
         <v>100</v>
@@ -4636,10 +4670,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="U26" sqref="U26"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4652,72 +4685,72 @@
     <col min="9" max="9" width="14.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.21875" customWidth="1"/>
-    <col min="12" max="12" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="87" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B1" s="80" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C1" s="81" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="81" t="s">
+        <v>81</v>
+      </c>
+      <c r="E1" s="81" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="81" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="81" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="81" t="s">
+        <v>83</v>
+      </c>
+      <c r="I1" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="81" t="s">
-        <v>84</v>
-      </c>
-      <c r="F1" s="81" t="s">
+      <c r="J1" s="81" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="81" t="s">
+      <c r="K1" s="81" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" s="81" t="s">
         <v>88</v>
       </c>
-      <c r="H1" s="81" t="s">
-        <v>87</v>
-      </c>
-      <c r="I1" s="81" t="s">
+      <c r="M1" s="81" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="81" t="s">
+      <c r="N1" s="82" t="s">
         <v>90</v>
       </c>
-      <c r="K1" s="81" t="s">
-        <v>91</v>
-      </c>
-      <c r="L1" s="81" t="s">
-        <v>92</v>
-      </c>
-      <c r="M1" s="81" t="s">
-        <v>93</v>
-      </c>
-      <c r="N1" s="82" t="s">
-        <v>94</v>
-      </c>
       <c r="O1" s="78"/>
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="110" t="s">
-        <v>140</v>
-      </c>
-      <c r="B2" s="111"/>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
-      <c r="M2" s="111"/>
-      <c r="N2" s="112"/>
+      <c r="A2" s="108" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="109"/>
+      <c r="I2" s="109"/>
+      <c r="J2" s="109"/>
+      <c r="K2" s="109"/>
+      <c r="L2" s="109"/>
+      <c r="M2" s="109"/>
+      <c r="N2" s="110"/>
       <c r="O2" s="78"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -4725,7 +4758,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="74" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C3" s="32">
         <f>'Ведомость электропотребителей'!E3</f>
@@ -4740,26 +4773,37 @@
         <v>16.769217122869609</v>
       </c>
       <c r="F3" s="70">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G3" s="7">
         <f>D3*1.25</f>
         <v>124.72105235134272</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="70">
         <f>'Ведомость электропотребителей'!I3*'Выбор защиты'!F3</f>
-        <v>140</v>
+        <v>175</v>
       </c>
       <c r="I3" s="70">
         <v>1</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" s="7"/>
+      <c r="J3" s="70">
+        <f>F3</f>
+        <v>25</v>
+      </c>
+      <c r="K3" s="70">
+        <f>J3</f>
+        <v>25</v>
+      </c>
       <c r="L3" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="M3" s="7"/>
-      <c r="N3" s="23"/>
+        <v>138</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="N3" s="126">
+        <f>K3</f>
+        <v>25</v>
+      </c>
       <c r="O3" s="78"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -4767,7 +4811,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="34" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C4" s="76">
         <f>'Ведомость электропотребителей'!E4</f>
@@ -4781,25 +4825,38 @@
         <f t="shared" ref="E4:E12" si="0">C4/0.85</f>
         <v>15.679492401000102</v>
       </c>
-      <c r="F4" s="92">
+      <c r="F4" s="91">
         <v>16</v>
       </c>
       <c r="G4" s="7">
         <f t="shared" ref="G4:G11" si="1">D4*1.25</f>
         <v>116.61622473243825</v>
       </c>
-      <c r="H4" s="72">
+      <c r="H4" s="91">
         <f>'Ведомость электропотребителей'!I3*F4</f>
         <v>112</v>
       </c>
       <c r="I4" s="70">
         <v>1</v>
       </c>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="72"/>
-      <c r="M4" s="72"/>
-      <c r="N4" s="20"/>
+      <c r="J4" s="70">
+        <f t="shared" ref="J4:J12" si="2">F4</f>
+        <v>16</v>
+      </c>
+      <c r="K4" s="70">
+        <f t="shared" ref="K4:K12" si="3">J4</f>
+        <v>16</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="M4" s="72" t="s">
+        <v>146</v>
+      </c>
+      <c r="N4" s="126">
+        <f t="shared" ref="N4:N12" si="4">K4</f>
+        <v>16</v>
+      </c>
       <c r="O4" s="78"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -4807,7 +4864,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="34" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C5" s="76">
         <f>'Ведомость электропотребителей'!E6</f>
@@ -4821,25 +4878,38 @@
         <f t="shared" si="0"/>
         <v>29.625017407066071</v>
       </c>
-      <c r="F5" s="92">
+      <c r="F5" s="91">
         <v>32</v>
       </c>
       <c r="G5" s="7">
         <f t="shared" si="1"/>
         <v>220.3360669650539</v>
       </c>
-      <c r="H5" s="72">
+      <c r="H5" s="91">
         <f>'Ведомость электропотребителей'!I5*F5</f>
         <v>224</v>
       </c>
       <c r="I5" s="70">
         <v>1</v>
       </c>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-      <c r="L5" s="72"/>
-      <c r="M5" s="72"/>
-      <c r="N5" s="20"/>
+      <c r="J5" s="70">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="K5" s="70">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="M5" s="72" t="s">
+        <v>147</v>
+      </c>
+      <c r="N5" s="126">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
       <c r="O5" s="78"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -4847,7 +4917,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="34" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C6" s="76">
         <f>'Ведомость электропотребителей'!E7</f>
@@ -4861,25 +4931,38 @@
         <f t="shared" si="0"/>
         <v>25.469614485526996</v>
       </c>
-      <c r="F6" s="92">
+      <c r="F6" s="91">
         <v>32</v>
       </c>
       <c r="G6" s="7">
         <f t="shared" si="1"/>
         <v>135.30732695436217</v>
       </c>
-      <c r="H6" s="72">
+      <c r="H6" s="91">
         <f>F6*7</f>
         <v>224</v>
       </c>
       <c r="I6" s="70">
         <v>1</v>
       </c>
-      <c r="J6" s="72"/>
-      <c r="K6" s="72"/>
-      <c r="L6" s="72"/>
-      <c r="M6" s="72"/>
-      <c r="N6" s="20"/>
+      <c r="J6" s="70">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="K6" s="70">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="M6" s="72" t="s">
+        <v>147</v>
+      </c>
+      <c r="N6" s="126">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
       <c r="O6" s="78"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -4887,7 +4970,7 @@
         <v>10</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C7" s="76">
         <f>'Ведомость электропотребителей'!E11</f>
@@ -4901,25 +4984,38 @@
         <f t="shared" si="0"/>
         <v>9.1986355419200585</v>
       </c>
-      <c r="F7" s="92">
-        <v>10</v>
+      <c r="F7" s="91">
+        <v>16</v>
       </c>
       <c r="G7" s="7">
         <f t="shared" si="1"/>
         <v>68.414851843030448</v>
       </c>
-      <c r="H7" s="72">
-        <f t="shared" ref="H7:H12" si="2">7*F7</f>
-        <v>70</v>
+      <c r="H7" s="91">
+        <f t="shared" ref="H7:H12" si="5">7*F7</f>
+        <v>112</v>
       </c>
       <c r="I7" s="70">
         <v>1</v>
       </c>
-      <c r="J7" s="72"/>
-      <c r="K7" s="72"/>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
-      <c r="N7" s="20"/>
+      <c r="J7" s="70">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="K7" s="70">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="M7" s="72" t="s">
+        <v>146</v>
+      </c>
+      <c r="N7" s="126">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
       <c r="O7" s="78"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -4927,7 +5023,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="34" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C8" s="76">
         <f>'Ведомость электропотребителей'!E8</f>
@@ -4941,25 +5037,38 @@
         <f t="shared" si="0"/>
         <v>23.399986124084098</v>
       </c>
-      <c r="F8" s="92">
+      <c r="F8" s="91">
         <v>25</v>
       </c>
       <c r="G8" s="7">
         <f t="shared" si="1"/>
         <v>174.03739679787549</v>
       </c>
-      <c r="H8" s="72">
-        <f t="shared" si="2"/>
+      <c r="H8" s="91">
+        <f t="shared" si="5"/>
         <v>175</v>
       </c>
       <c r="I8" s="70">
         <v>1</v>
       </c>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-      <c r="L8" s="72"/>
-      <c r="M8" s="72"/>
-      <c r="N8" s="20"/>
+      <c r="J8" s="70">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="K8" s="70">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="L8" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="M8" s="72" t="s">
+        <v>145</v>
+      </c>
+      <c r="N8" s="126">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
       <c r="O8" s="78"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -4967,7 +5076,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="34" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C9" s="76">
         <f>'Ведомость электропотребителей'!E9</f>
@@ -4981,25 +5090,38 @@
         <f t="shared" si="0"/>
         <v>19.199378450204208</v>
       </c>
-      <c r="F9" s="92">
-        <v>20</v>
+      <c r="F9" s="91">
+        <v>25</v>
       </c>
       <c r="G9" s="7">
         <f t="shared" si="1"/>
         <v>142.79537722339379</v>
       </c>
-      <c r="H9" s="72">
-        <f t="shared" si="2"/>
-        <v>140</v>
+      <c r="H9" s="91">
+        <f t="shared" si="5"/>
+        <v>175</v>
       </c>
       <c r="I9" s="70">
         <v>1</v>
       </c>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-      <c r="L9" s="72"/>
-      <c r="M9" s="72"/>
-      <c r="N9" s="20"/>
+      <c r="J9" s="70">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="K9" s="70">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="M9" s="72" t="s">
+        <v>145</v>
+      </c>
+      <c r="N9" s="126">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
       <c r="O9" s="78"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -5007,7 +5129,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C10" s="76">
         <f>'Ведомость электропотребителей'!E10</f>
@@ -5021,25 +5143,38 @@
         <f t="shared" si="0"/>
         <v>22.510461620520147</v>
       </c>
-      <c r="F10" s="92">
+      <c r="F10" s="91">
         <v>25</v>
       </c>
       <c r="G10" s="7">
         <f t="shared" si="1"/>
         <v>167.42155830261856</v>
       </c>
-      <c r="H10" s="72">
-        <f t="shared" si="2"/>
+      <c r="H10" s="91">
+        <f t="shared" si="5"/>
         <v>175</v>
       </c>
       <c r="I10" s="70">
         <v>1</v>
       </c>
-      <c r="J10" s="72"/>
-      <c r="K10" s="72"/>
-      <c r="L10" s="72"/>
-      <c r="M10" s="72"/>
-      <c r="N10" s="20"/>
+      <c r="J10" s="70">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="K10" s="70">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="M10" s="72" t="s">
+        <v>145</v>
+      </c>
+      <c r="N10" s="126">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
       <c r="O10" s="78"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -5047,7 +5182,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C11" s="77">
         <f>'Ведомость электропотребителей'!E21</f>
@@ -5062,30 +5197,43 @@
         <v>16.127477898171534</v>
       </c>
       <c r="F11" s="71">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G11" s="7">
         <f t="shared" si="1"/>
         <v>119.94811686765078</v>
       </c>
-      <c r="H11" s="73">
-        <f t="shared" si="2"/>
-        <v>140</v>
+      <c r="H11" s="71">
+        <f t="shared" si="5"/>
+        <v>175</v>
       </c>
       <c r="I11" s="70">
         <v>1</v>
       </c>
-      <c r="J11" s="73"/>
-      <c r="K11" s="73"/>
-      <c r="L11" s="73"/>
-      <c r="M11" s="73"/>
-      <c r="N11" s="21"/>
+      <c r="J11" s="70">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="K11" s="70">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="M11" s="73" t="s">
+        <v>145</v>
+      </c>
+      <c r="N11" s="126">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
       <c r="O11" s="78"/>
     </row>
     <row r="12" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="60"/>
       <c r="B12" s="35" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C12" s="77">
         <f>'Расчет электрических нагрузок'!Q13</f>
@@ -5106,37 +5254,50 @@
         <f>D12*1.25</f>
         <v>377.96247208711918</v>
       </c>
-      <c r="H12" s="73">
-        <f t="shared" si="2"/>
+      <c r="H12" s="71">
+        <f t="shared" si="5"/>
         <v>700</v>
       </c>
       <c r="I12" s="70">
         <v>1</v>
       </c>
-      <c r="J12" s="73"/>
-      <c r="K12" s="73"/>
-      <c r="L12" s="73"/>
-      <c r="M12" s="73"/>
-      <c r="N12" s="21"/>
+      <c r="J12" s="70">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="K12" s="70">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="L12" s="73" t="s">
+        <v>139</v>
+      </c>
+      <c r="M12" s="73" t="s">
+        <v>148</v>
+      </c>
+      <c r="N12" s="126">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
       <c r="O12" s="78"/>
     </row>
     <row r="13" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="110" t="s">
-        <v>141</v>
-      </c>
-      <c r="B13" s="111"/>
-      <c r="C13" s="111"/>
-      <c r="D13" s="111"/>
-      <c r="E13" s="111"/>
-      <c r="F13" s="111"/>
-      <c r="G13" s="111"/>
-      <c r="H13" s="111"/>
-      <c r="I13" s="111"/>
-      <c r="J13" s="111"/>
-      <c r="K13" s="111"/>
-      <c r="L13" s="111"/>
-      <c r="M13" s="111"/>
-      <c r="N13" s="112"/>
+      <c r="A13" s="108" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13" s="109"/>
+      <c r="C13" s="109"/>
+      <c r="D13" s="109"/>
+      <c r="E13" s="109"/>
+      <c r="F13" s="109"/>
+      <c r="G13" s="109"/>
+      <c r="H13" s="109"/>
+      <c r="I13" s="109"/>
+      <c r="J13" s="109"/>
+      <c r="K13" s="109"/>
+      <c r="L13" s="109"/>
+      <c r="M13" s="109"/>
+      <c r="N13" s="110"/>
       <c r="O13" s="78"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -5144,7 +5305,7 @@
         <v>6</v>
       </c>
       <c r="B14" s="74" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C14" s="32">
         <f>'Ведомость электропотребителей'!E7</f>
@@ -5165,18 +5326,31 @@
         <f>D14*1.25</f>
         <v>135.30732695436217</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="70">
         <f>'Ведомость электропотребителей'!I7*F14</f>
         <v>160</v>
       </c>
       <c r="I14" s="70">
         <v>1</v>
       </c>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="7"/>
-      <c r="N14" s="23"/>
+      <c r="J14" s="70">
+        <f>F14</f>
+        <v>32</v>
+      </c>
+      <c r="K14" s="70">
+        <f>J14</f>
+        <v>32</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="M14" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="N14" s="126">
+        <f>K14</f>
+        <v>32</v>
+      </c>
       <c r="O14" s="78"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -5184,7 +5358,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="34" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C15" s="76">
         <f>'Ведомость электропотребителей'!E12</f>
@@ -5195,28 +5369,41 @@
         <v>159.64294700971868</v>
       </c>
       <c r="E15" s="7">
-        <f t="shared" ref="E15:E22" si="3">C15/0.85</f>
+        <f t="shared" ref="E15:E22" si="6">C15/0.85</f>
         <v>26.830747396591377</v>
       </c>
-      <c r="F15" s="92">
+      <c r="F15" s="91">
         <v>32</v>
       </c>
       <c r="G15" s="7">
-        <f t="shared" ref="G15:G22" si="4">D15*1.25</f>
+        <f t="shared" ref="G15:G22" si="7">D15*1.25</f>
         <v>199.55368376214835</v>
       </c>
-      <c r="H15" s="72">
+      <c r="H15" s="91">
         <f>'Ведомость электропотребителей'!I12*F15</f>
         <v>224</v>
       </c>
       <c r="I15" s="70">
         <v>1</v>
       </c>
-      <c r="J15" s="72"/>
-      <c r="K15" s="72"/>
-      <c r="L15" s="72"/>
-      <c r="M15" s="72"/>
-      <c r="N15" s="20"/>
+      <c r="J15" s="70">
+        <f t="shared" ref="J15:J22" si="8">F15</f>
+        <v>32</v>
+      </c>
+      <c r="K15" s="70">
+        <f t="shared" ref="K15:K22" si="9">J15</f>
+        <v>32</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="M15" s="72" t="s">
+        <v>147</v>
+      </c>
+      <c r="N15" s="126">
+        <f t="shared" ref="N15:N22" si="10">K15</f>
+        <v>32</v>
+      </c>
       <c r="O15" s="78"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -5224,7 +5411,7 @@
         <v>13</v>
       </c>
       <c r="B16" s="34" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C16" s="76">
         <f>'Ведомость электропотребителей'!E14</f>
@@ -5235,28 +5422,41 @@
         <v>93.936379646543372</v>
       </c>
       <c r="E16" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>15.787626831351828</v>
       </c>
-      <c r="F16" s="92">
-        <v>20</v>
+      <c r="F16" s="91">
+        <v>25</v>
       </c>
       <c r="G16" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>117.42047455817922</v>
       </c>
-      <c r="H16" s="72">
+      <c r="H16" s="91">
         <f>'Ведомость электропотребителей'!I14*F16</f>
-        <v>140</v>
+        <v>175</v>
       </c>
       <c r="I16" s="70">
         <v>1</v>
       </c>
-      <c r="J16" s="72"/>
-      <c r="K16" s="72"/>
-      <c r="L16" s="72"/>
-      <c r="M16" s="72"/>
-      <c r="N16" s="20"/>
+      <c r="J16" s="70">
+        <f t="shared" si="8"/>
+        <v>25</v>
+      </c>
+      <c r="K16" s="70">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="M16" s="72" t="s">
+        <v>145</v>
+      </c>
+      <c r="N16" s="126">
+        <f t="shared" si="10"/>
+        <v>25</v>
+      </c>
       <c r="O16" s="78"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -5264,7 +5464,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="34" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C17" s="76">
         <f>'Ведомость электропотребителей'!E16</f>
@@ -5275,28 +5475,41 @@
         <v>58.526583268249524</v>
       </c>
       <c r="E17" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>9.8364005492856332</v>
       </c>
-      <c r="F17" s="92">
-        <v>10</v>
+      <c r="F17" s="91">
+        <v>16</v>
       </c>
       <c r="G17" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>73.158229085311902</v>
       </c>
-      <c r="H17" s="72">
+      <c r="H17" s="91">
         <f>'Ведомость электропотребителей'!I14*F17</f>
-        <v>70</v>
+        <v>112</v>
       </c>
       <c r="I17" s="70">
         <v>1</v>
       </c>
-      <c r="J17" s="72"/>
-      <c r="K17" s="72"/>
-      <c r="L17" s="72"/>
-      <c r="M17" s="72"/>
-      <c r="N17" s="20"/>
+      <c r="J17" s="70">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="K17" s="70">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="M17" s="72" t="s">
+        <v>146</v>
+      </c>
+      <c r="N17" s="126">
+        <f t="shared" si="10"/>
+        <v>16</v>
+      </c>
       <c r="O17" s="78"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -5304,7 +5517,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C18" s="76">
         <f>'Ведомость электропотребителей'!E17</f>
@@ -5315,28 +5528,41 @@
         <v>86.306854322909643</v>
       </c>
       <c r="E18" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>14.505353667715907</v>
       </c>
-      <c r="F18" s="92">
+      <c r="F18" s="91">
         <v>16</v>
       </c>
       <c r="G18" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>107.88356790363706</v>
       </c>
-      <c r="H18" s="72">
+      <c r="H18" s="91">
         <f>'Ведомость электропотребителей'!I17*F18</f>
         <v>112</v>
       </c>
       <c r="I18" s="70">
         <v>1</v>
       </c>
-      <c r="J18" s="72"/>
-      <c r="K18" s="72"/>
-      <c r="L18" s="72"/>
-      <c r="M18" s="72"/>
-      <c r="N18" s="20"/>
+      <c r="J18" s="70">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="K18" s="70">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="M18" s="72" t="s">
+        <v>146</v>
+      </c>
+      <c r="N18" s="126">
+        <f t="shared" si="10"/>
+        <v>16</v>
+      </c>
       <c r="O18" s="78"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -5344,7 +5570,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="34" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C19" s="76">
         <f>'Ведомость электропотребителей'!E18</f>
@@ -5355,28 +5581,41 @@
         <v>86.105965046884776</v>
       </c>
       <c r="E19" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>14.471590764182316</v>
       </c>
-      <c r="F19" s="92">
+      <c r="F19" s="91">
         <v>16</v>
       </c>
       <c r="G19" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>107.63245630860597</v>
       </c>
-      <c r="H19" s="72">
+      <c r="H19" s="91">
         <f>'Ведомость электропотребителей'!I18*F19</f>
         <v>112</v>
       </c>
       <c r="I19" s="70">
         <v>1</v>
       </c>
-      <c r="J19" s="72"/>
-      <c r="K19" s="72"/>
-      <c r="L19" s="72"/>
-      <c r="M19" s="72"/>
-      <c r="N19" s="20"/>
+      <c r="J19" s="70">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="K19" s="70">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="L19" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="M19" s="72" t="s">
+        <v>146</v>
+      </c>
+      <c r="N19" s="126">
+        <f t="shared" si="10"/>
+        <v>16</v>
+      </c>
       <c r="O19" s="78"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -5384,7 +5623,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="34" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C20" s="76">
         <f>'Ведомость электропотребителей'!E19</f>
@@ -5395,28 +5634,41 @@
         <v>130.61017170033082</v>
       </c>
       <c r="E20" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>21.951289361400139</v>
       </c>
-      <c r="F20" s="92">
+      <c r="F20" s="91">
         <v>25</v>
       </c>
       <c r="G20" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>163.26271462541354</v>
       </c>
-      <c r="H20" s="101">
+      <c r="H20" s="91">
         <f>'Ведомость электропотребителей'!I19*F20</f>
         <v>175</v>
       </c>
       <c r="I20" s="70">
         <v>1</v>
       </c>
-      <c r="J20" s="72"/>
-      <c r="K20" s="72"/>
-      <c r="L20" s="72"/>
-      <c r="M20" s="72"/>
-      <c r="N20" s="20"/>
+      <c r="J20" s="70">
+        <f t="shared" si="8"/>
+        <v>25</v>
+      </c>
+      <c r="K20" s="70">
+        <f t="shared" si="9"/>
+        <v>25</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="M20" s="72" t="s">
+        <v>145</v>
+      </c>
+      <c r="N20" s="126">
+        <f t="shared" si="10"/>
+        <v>25</v>
+      </c>
       <c r="O20" s="78"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -5424,7 +5676,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="35" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C21" s="77">
         <f>'Ведомость электропотребителей'!E20</f>
@@ -5435,34 +5687,47 @@
         <v>82.346603491065736</v>
       </c>
       <c r="E21" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>13.839765292616089</v>
       </c>
       <c r="F21" s="71">
         <v>16</v>
       </c>
       <c r="G21" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>102.93325436383216</v>
       </c>
-      <c r="H21" s="73">
+      <c r="H21" s="71">
         <f>'Ведомость электропотребителей'!I20*F21</f>
         <v>112</v>
       </c>
       <c r="I21" s="70">
         <v>1</v>
       </c>
-      <c r="J21" s="73"/>
-      <c r="K21" s="73"/>
-      <c r="L21" s="73"/>
-      <c r="M21" s="73"/>
-      <c r="N21" s="21"/>
+      <c r="J21" s="70">
+        <f t="shared" si="8"/>
+        <v>16</v>
+      </c>
+      <c r="K21" s="70">
+        <f t="shared" si="9"/>
+        <v>16</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="M21" s="73" t="s">
+        <v>146</v>
+      </c>
+      <c r="N21" s="126">
+        <f t="shared" si="10"/>
+        <v>16</v>
+      </c>
       <c r="O21" s="78"/>
     </row>
     <row r="22" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="89"/>
       <c r="B22" s="75" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C22" s="77">
         <f>'Расчет электрических нагрузок'!Q23</f>
@@ -5473,47 +5738,60 @@
         <v>258.12534181898576</v>
       </c>
       <c r="E22" s="7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>79.682895799095448</v>
       </c>
       <c r="F22" s="71">
         <v>100</v>
       </c>
       <c r="G22" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>322.65667727373221</v>
       </c>
-      <c r="H22" s="73">
+      <c r="H22" s="71">
         <f>7*F22</f>
         <v>700</v>
       </c>
       <c r="I22" s="70">
         <v>1</v>
       </c>
-      <c r="J22" s="73"/>
-      <c r="K22" s="73"/>
-      <c r="L22" s="73"/>
-      <c r="M22" s="73"/>
-      <c r="N22" s="21"/>
+      <c r="J22" s="70">
+        <f t="shared" si="8"/>
+        <v>100</v>
+      </c>
+      <c r="K22" s="70">
+        <f t="shared" si="9"/>
+        <v>100</v>
+      </c>
+      <c r="L22" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="M22" s="73" t="s">
+        <v>148</v>
+      </c>
+      <c r="N22" s="126">
+        <f t="shared" si="10"/>
+        <v>100</v>
+      </c>
       <c r="O22" s="78"/>
     </row>
     <row r="23" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="110" t="s">
-        <v>95</v>
-      </c>
-      <c r="B23" s="111"/>
-      <c r="C23" s="111"/>
-      <c r="D23" s="111"/>
-      <c r="E23" s="111"/>
-      <c r="F23" s="111"/>
-      <c r="G23" s="111"/>
-      <c r="H23" s="111"/>
-      <c r="I23" s="111"/>
-      <c r="J23" s="111"/>
-      <c r="K23" s="111"/>
-      <c r="L23" s="111"/>
-      <c r="M23" s="111"/>
-      <c r="N23" s="112"/>
+      <c r="A23" s="108" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="109"/>
+      <c r="C23" s="109"/>
+      <c r="D23" s="109"/>
+      <c r="E23" s="109"/>
+      <c r="F23" s="109"/>
+      <c r="G23" s="109"/>
+      <c r="H23" s="109"/>
+      <c r="I23" s="109"/>
+      <c r="J23" s="109"/>
+      <c r="K23" s="109"/>
+      <c r="L23" s="109"/>
+      <c r="M23" s="109"/>
+      <c r="N23" s="110"/>
       <c r="O23" s="78"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -5521,7 +5799,7 @@
         <v>1</v>
       </c>
       <c r="B24" s="83" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C24" s="7">
         <f>'Ведомость электропотребителей'!E2</f>
@@ -5543,18 +5821,31 @@
         <f>D24*1.25</f>
         <v>182.77808284594408</v>
       </c>
-      <c r="H24" s="7">
+      <c r="H24" s="70">
         <f>F24*'Ведомость электропотребителей'!I2</f>
         <v>250</v>
       </c>
       <c r="I24" s="70">
         <v>1</v>
       </c>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-      <c r="L24" s="7"/>
-      <c r="M24" s="7"/>
-      <c r="N24" s="23"/>
+      <c r="J24" s="70">
+        <f>F24</f>
+        <v>100</v>
+      </c>
+      <c r="K24" s="70">
+        <f>J24</f>
+        <v>100</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="N24" s="126">
+        <f>K24</f>
+        <v>100</v>
+      </c>
       <c r="O24" s="78"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -5562,7 +5853,7 @@
         <v>12</v>
       </c>
       <c r="B25" s="79" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C25" s="72">
         <f>'Ведомость электропотребителей'!E13</f>
@@ -5576,26 +5867,39 @@
         <f>C25/0.85</f>
         <v>148.01440826544095</v>
       </c>
-      <c r="F25" s="92">
+      <c r="F25" s="91">
         <f>160</f>
         <v>160</v>
       </c>
       <c r="G25" s="7">
-        <f t="shared" ref="G25:G26" si="5">D25*1.25</f>
+        <f t="shared" ref="G25:G26" si="11">D25*1.25</f>
         <v>550.42858073710852</v>
       </c>
-      <c r="H25" s="72">
+      <c r="H25" s="91">
         <f>F25*'Ведомость электропотребителей'!I13</f>
         <v>560</v>
       </c>
       <c r="I25" s="70">
         <v>1</v>
       </c>
-      <c r="J25" s="72"/>
-      <c r="K25" s="72"/>
-      <c r="L25" s="72"/>
-      <c r="M25" s="72"/>
-      <c r="N25" s="20"/>
+      <c r="J25" s="70">
+        <f t="shared" ref="J25:J26" si="12">F25</f>
+        <v>160</v>
+      </c>
+      <c r="K25" s="70">
+        <f t="shared" ref="K25:K26" si="13">J25</f>
+        <v>160</v>
+      </c>
+      <c r="L25" s="72" t="s">
+        <v>143</v>
+      </c>
+      <c r="M25" s="72" t="s">
+        <v>149</v>
+      </c>
+      <c r="N25" s="126">
+        <f t="shared" ref="N25:N26" si="14">K25</f>
+        <v>160</v>
+      </c>
       <c r="O25" s="78"/>
     </row>
     <row r="26" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -5603,7 +5907,7 @@
         <v>14</v>
       </c>
       <c r="B26" s="84" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C26" s="73">
         <f>'Ведомость электропотребителей'!E15</f>
@@ -5621,40 +5925,53 @@
         <v>100</v>
       </c>
       <c r="G26" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="11"/>
         <v>182.77808284594408</v>
       </c>
-      <c r="H26" s="73">
+      <c r="H26" s="71">
         <f>F26*'Ведомость электропотребителей'!I15</f>
         <v>250</v>
       </c>
       <c r="I26" s="70">
         <v>1</v>
       </c>
-      <c r="J26" s="73"/>
-      <c r="K26" s="73"/>
-      <c r="L26" s="73"/>
-      <c r="M26" s="73"/>
-      <c r="N26" s="21"/>
+      <c r="J26" s="70">
+        <f t="shared" si="12"/>
+        <v>100</v>
+      </c>
+      <c r="K26" s="70">
+        <f t="shared" si="13"/>
+        <v>100</v>
+      </c>
+      <c r="L26" s="73" t="s">
+        <v>142</v>
+      </c>
+      <c r="M26" s="73" t="s">
+        <v>148</v>
+      </c>
+      <c r="N26" s="126">
+        <f t="shared" si="14"/>
+        <v>100</v>
+      </c>
       <c r="O26" s="78"/>
     </row>
     <row r="27" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="110" t="s">
-        <v>99</v>
-      </c>
-      <c r="B27" s="111"/>
-      <c r="C27" s="111"/>
-      <c r="D27" s="111"/>
-      <c r="E27" s="111"/>
-      <c r="F27" s="111"/>
-      <c r="G27" s="111"/>
-      <c r="H27" s="111"/>
-      <c r="I27" s="111"/>
-      <c r="J27" s="111"/>
-      <c r="K27" s="111"/>
-      <c r="L27" s="111"/>
-      <c r="M27" s="111"/>
-      <c r="N27" s="112"/>
+      <c r="A27" s="108" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="109"/>
+      <c r="C27" s="109"/>
+      <c r="D27" s="109"/>
+      <c r="E27" s="109"/>
+      <c r="F27" s="109"/>
+      <c r="G27" s="109"/>
+      <c r="H27" s="109"/>
+      <c r="I27" s="109"/>
+      <c r="J27" s="109"/>
+      <c r="K27" s="109"/>
+      <c r="L27" s="109"/>
+      <c r="M27" s="109"/>
+      <c r="N27" s="110"/>
       <c r="O27" s="78"/>
     </row>
     <row r="28" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -5672,25 +5989,38 @@
         <f>C28/0.85</f>
         <v>199.35674494733388</v>
       </c>
-      <c r="F28" s="93">
+      <c r="F28" s="92">
         <v>250</v>
       </c>
       <c r="G28" s="86">
         <f>D28*1.25</f>
         <v>881.02834032540795</v>
       </c>
-      <c r="H28" s="86">
+      <c r="H28" s="92">
         <f>7*F28</f>
         <v>1750</v>
       </c>
-      <c r="I28" s="93">
+      <c r="I28" s="92">
         <v>1</v>
       </c>
-      <c r="J28" s="86"/>
-      <c r="K28" s="86"/>
-      <c r="L28" s="86"/>
-      <c r="M28" s="86"/>
-      <c r="N28" s="91"/>
+      <c r="J28" s="92">
+        <f>F28</f>
+        <v>250</v>
+      </c>
+      <c r="K28" s="92">
+        <f>J28</f>
+        <v>250</v>
+      </c>
+      <c r="L28" s="86" t="s">
+        <v>144</v>
+      </c>
+      <c r="M28" s="86" t="s">
+        <v>150</v>
+      </c>
+      <c r="N28" s="127">
+        <f>K28</f>
+        <v>250</v>
+      </c>
       <c r="O28" s="78"/>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -5731,10 +6061,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
-    </sheetView>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="1">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -5746,565 +6073,565 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="126"/>
-      <c r="B1" s="122" t="s">
+      <c r="A1" s="124"/>
+      <c r="B1" s="120" t="s">
+        <v>129</v>
+      </c>
+      <c r="C1" s="120" t="s">
+        <v>128</v>
+      </c>
+      <c r="D1" s="120" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="120" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="120"/>
+      <c r="G1" s="120" t="s">
+        <v>125</v>
+      </c>
+      <c r="H1" s="120" t="s">
+        <v>131</v>
+      </c>
+      <c r="I1" s="120" t="s">
+        <v>132</v>
+      </c>
+      <c r="J1" s="120" t="s">
         <v>133</v>
       </c>
-      <c r="C1" s="122" t="s">
-        <v>132</v>
-      </c>
-      <c r="D1" s="122" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" s="122" t="s">
-        <v>113</v>
-      </c>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122" t="s">
-        <v>129</v>
-      </c>
-      <c r="H1" s="122" t="s">
-        <v>135</v>
-      </c>
-      <c r="I1" s="122" t="s">
-        <v>136</v>
-      </c>
-      <c r="J1" s="122" t="s">
-        <v>137</v>
-      </c>
-      <c r="K1" s="122" t="s">
-        <v>134</v>
-      </c>
-      <c r="L1" s="124" t="s">
-        <v>114</v>
+      <c r="K1" s="120" t="s">
+        <v>130</v>
+      </c>
+      <c r="L1" s="122" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="127"/>
-      <c r="B2" s="123"/>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="95" t="s">
-        <v>130</v>
-      </c>
-      <c r="F2" s="95" t="s">
-        <v>128</v>
-      </c>
-      <c r="G2" s="123"/>
-      <c r="H2" s="123"/>
-      <c r="I2" s="123"/>
-      <c r="J2" s="123"/>
-      <c r="K2" s="123"/>
-      <c r="L2" s="125"/>
+      <c r="A2" s="125"/>
+      <c r="B2" s="121"/>
+      <c r="C2" s="121"/>
+      <c r="D2" s="121"/>
+      <c r="E2" s="94" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="94" t="s">
+        <v>124</v>
+      </c>
+      <c r="G2" s="121"/>
+      <c r="H2" s="121"/>
+      <c r="I2" s="121"/>
+      <c r="J2" s="121"/>
+      <c r="K2" s="121"/>
+      <c r="L2" s="123"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="96" t="s">
-        <v>102</v>
-      </c>
-      <c r="B3" s="94">
+      <c r="A3" s="95" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="93">
         <f>(4.5*400*400)/(100*100000)</f>
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="94"/>
-      <c r="K3" s="94">
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
+      <c r="J3" s="93"/>
+      <c r="K3" s="93">
         <f>B3/3</f>
         <v>2.3999999999999997E-2</v>
       </c>
-      <c r="L3" s="97"/>
+      <c r="L3" s="96"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="96" t="s">
-        <v>138</v>
-      </c>
-      <c r="B4" s="94">
+      <c r="A4" s="95" t="s">
+        <v>134</v>
+      </c>
+      <c r="B4" s="93">
         <f t="shared" ref="B4:B15" si="0">SQRT(C4*C4+D4*D4)</f>
         <v>1.8762079442321952E-3</v>
       </c>
-      <c r="C4" s="94">
+      <c r="C4" s="93">
         <f xml:space="preserve"> 0.37 * 5 / 1000</f>
         <v>1.8500000000000001E-3</v>
       </c>
-      <c r="D4" s="94">
+      <c r="D4" s="93">
         <f xml:space="preserve"> 0.0625 * 5 / 1000</f>
         <v>3.1250000000000001E-4</v>
       </c>
-      <c r="E4" s="94">
+      <c r="E4" s="93">
         <f>(400/SQRT(3))/(K3+2*B4)</f>
         <v>8321.441585625822</v>
       </c>
-      <c r="F4" s="94">
+      <c r="F4" s="93">
         <f>(400/SQRT(3))/(K3+B4)</f>
         <v>8924.8049085695693</v>
       </c>
-      <c r="G4" s="94">
+      <c r="G4" s="93">
         <v>95</v>
       </c>
-      <c r="H4" s="94">
+      <c r="H4" s="93">
         <v>5</v>
       </c>
-      <c r="I4" s="94">
+      <c r="I4" s="93">
         <f xml:space="preserve"> 0.0037</f>
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="J4" s="94">
+      <c r="J4" s="93">
         <v>6.3000000000000003E-4</v>
       </c>
-      <c r="K4" s="94"/>
-      <c r="L4" s="97" t="s">
-        <v>115</v>
+      <c r="K4" s="93"/>
+      <c r="L4" s="96" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="96" t="s">
-        <v>117</v>
-      </c>
-      <c r="B5" s="94">
+      <c r="A5" s="95" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="93">
         <f t="shared" si="0"/>
         <v>1.8762079442321952E-3</v>
       </c>
-      <c r="C5" s="94">
+      <c r="C5" s="93">
         <f>C4</f>
         <v>1.8500000000000001E-3</v>
       </c>
-      <c r="D5" s="94">
+      <c r="D5" s="93">
         <f>D4</f>
         <v>3.1250000000000001E-4</v>
       </c>
-      <c r="E5" s="94">
+      <c r="E5" s="93">
         <f>(400/SQRT(3))/(K3+2*B4+2*B5)</f>
         <v>7330.307595705669</v>
       </c>
-      <c r="F5" s="94">
+      <c r="F5" s="93">
         <f>(400/SQRT(3))/(K3+B4+B5)</f>
         <v>8321.441585625822</v>
       </c>
-      <c r="G5" s="94">
+      <c r="G5" s="93">
         <v>95</v>
       </c>
-      <c r="H5" s="94">
+      <c r="H5" s="93">
         <v>5</v>
       </c>
-      <c r="I5" s="94">
+      <c r="I5" s="93">
         <f t="shared" ref="I5:I6" si="1" xml:space="preserve"> 0.0037</f>
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="J5" s="94">
+      <c r="J5" s="93">
         <v>6.3000000000000003E-4</v>
       </c>
-      <c r="K5" s="94"/>
-      <c r="L5" s="97" t="s">
-        <v>116</v>
+      <c r="K5" s="93"/>
+      <c r="L5" s="96" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="96" t="s">
-        <v>103</v>
-      </c>
-      <c r="B6" s="94">
+      <c r="A6" s="95" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="93">
         <f t="shared" si="0"/>
         <v>7.1311786543319759E-3</v>
       </c>
-      <c r="C6" s="94">
+      <c r="C6" s="93">
         <f>0.37*19/1000</f>
         <v>7.0300000000000007E-3</v>
       </c>
-      <c r="D6" s="94">
+      <c r="D6" s="93">
         <f>0.063*19/1000</f>
         <v>1.1970000000000001E-3</v>
       </c>
-      <c r="E6" s="94">
+      <c r="E6" s="93">
         <f>(400/SQRT(3))/(K3+2*B4+2*B5+2*B6)</f>
         <v>5045.9753436889368</v>
       </c>
-      <c r="F6" s="94">
+      <c r="F6" s="93">
         <f>(400/SQRT(3))/(K3+B4+B5+B6)</f>
         <v>6620.3070727853255</v>
       </c>
-      <c r="G6" s="94">
+      <c r="G6" s="93">
         <v>95</v>
       </c>
-      <c r="H6" s="94">
+      <c r="H6" s="93">
         <v>19</v>
       </c>
-      <c r="I6" s="94">
+      <c r="I6" s="93">
         <f t="shared" si="1"/>
         <v>3.7000000000000002E-3</v>
       </c>
-      <c r="J6" s="94">
+      <c r="J6" s="93">
         <v>6.3000000000000003E-4</v>
       </c>
-      <c r="K6" s="94"/>
-      <c r="L6" s="97" t="s">
-        <v>118</v>
+      <c r="K6" s="93"/>
+      <c r="L6" s="96" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="96" t="s">
-        <v>104</v>
-      </c>
-      <c r="B7" s="94">
+      <c r="A7" s="95" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" s="93">
         <f t="shared" si="0"/>
         <v>6.228273872462578E-2</v>
       </c>
-      <c r="C7" s="94">
+      <c r="C7" s="93">
         <f>1.16 * 53.6 / 1000</f>
         <v>6.2175999999999995E-2</v>
       </c>
-      <c r="D7" s="94">
+      <c r="D7" s="93">
         <f>0.068 * 53.6 / 1000</f>
         <v>3.6448000000000006E-3</v>
       </c>
-      <c r="E7" s="94">
+      <c r="E7" s="93">
         <f>(400/SQRT(3))/(K3+2*B4+2*B5+2*B6+2*B7)</f>
         <v>1355.8180727981958</v>
       </c>
-      <c r="F7" s="94">
+      <c r="F7" s="93">
         <f>(400/SQRT(3))/(K3+B4+B5+B6+B7)</f>
         <v>2376.7502581398712</v>
       </c>
-      <c r="G7" s="94">
+      <c r="G7" s="93">
         <v>25</v>
       </c>
-      <c r="H7" s="94">
+      <c r="H7" s="93">
         <v>53.6</v>
       </c>
-      <c r="I7" s="94">
+      <c r="I7" s="93">
         <v>1.1599999999999999E-2</v>
       </c>
-      <c r="J7" s="94">
+      <c r="J7" s="93">
         <f>0.00068</f>
         <v>6.8000000000000005E-4</v>
       </c>
-      <c r="K7" s="94"/>
-      <c r="L7" s="97" t="s">
-        <v>121</v>
+      <c r="K7" s="93"/>
+      <c r="L7" s="96" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="96" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8" s="94">
+      <c r="A8" s="95" t="s">
+        <v>103</v>
+      </c>
+      <c r="B8" s="93">
         <f t="shared" si="0"/>
         <v>0.19065000000000001</v>
       </c>
-      <c r="C8" s="94">
+      <c r="C8" s="93">
         <f>12.3*15.5/1000</f>
         <v>0.19065000000000001</v>
       </c>
-      <c r="D8" s="94">
+      <c r="D8" s="93">
         <v>0</v>
       </c>
-      <c r="E8" s="94">
+      <c r="E8" s="93">
         <f>(400/SQRT(3))/(K3+2*B4+2*B5+2*B8)</f>
         <v>559.4413870636223</v>
       </c>
-      <c r="F8" s="94">
+      <c r="F8" s="93">
         <f>(400/SQRT(3))/(K3+B4+B8)</f>
         <v>1066.5688457229644</v>
       </c>
-      <c r="G8" s="94">
+      <c r="G8" s="93">
         <v>10</v>
       </c>
-      <c r="H8" s="94">
+      <c r="H8" s="93">
         <v>15.5</v>
       </c>
-      <c r="I8" s="94">
+      <c r="I8" s="93">
         <v>1.23E-2</v>
       </c>
-      <c r="J8" s="94">
+      <c r="J8" s="93">
         <v>0</v>
       </c>
-      <c r="K8" s="94"/>
-      <c r="L8" s="97" t="s">
-        <v>120</v>
+      <c r="K8" s="93"/>
+      <c r="L8" s="96" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="96" t="s">
-        <v>106</v>
-      </c>
-      <c r="B9" s="94">
+      <c r="A9" s="95" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="93">
         <f t="shared" si="0"/>
         <v>0.38991000000000003</v>
       </c>
-      <c r="C9" s="94">
+      <c r="C9" s="93">
         <f>12.3*31.7/1000</f>
         <v>0.38991000000000003</v>
       </c>
-      <c r="D9" s="94">
+      <c r="D9" s="93">
         <v>0</v>
       </c>
-      <c r="E9" s="94">
+      <c r="E9" s="93">
         <f>(400/SQRT(3))/(K3+2*B4+2*B5+2*B9)</f>
         <v>284.64567905564434</v>
       </c>
-      <c r="F9" s="94">
+      <c r="F9" s="93">
         <f>(400/SQRT(3))/(K3+B4+B9)</f>
         <v>555.42993794259144</v>
       </c>
-      <c r="G9" s="94">
+      <c r="G9" s="93">
         <v>6</v>
       </c>
-      <c r="H9" s="94">
+      <c r="H9" s="93">
         <v>31.7</v>
       </c>
-      <c r="I9" s="94">
+      <c r="I9" s="93">
         <v>1.23E-2</v>
       </c>
-      <c r="J9" s="94">
+      <c r="J9" s="93">
         <v>0</v>
       </c>
-      <c r="K9" s="94"/>
-      <c r="L9" s="97" t="s">
-        <v>125</v>
+      <c r="K9" s="93"/>
+      <c r="L9" s="96" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="96" t="s">
-        <v>108</v>
-      </c>
-      <c r="B10" s="94">
+      <c r="A10" s="95" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="93">
         <f t="shared" si="0"/>
         <v>0.15621000000000002</v>
       </c>
-      <c r="C10" s="94">
+      <c r="C10" s="93">
         <f>12.3*12.7/1000</f>
         <v>0.15621000000000002</v>
       </c>
-      <c r="D10" s="94">
+      <c r="D10" s="93">
         <v>0</v>
       </c>
-      <c r="E10" s="94">
+      <c r="E10" s="93">
         <f>(400/SQRT(3))/(K3+2*B4+2*B5+2*B10)</f>
         <v>671.48424986550299</v>
       </c>
-      <c r="F10" s="94">
+      <c r="F10" s="93">
         <f>(400/SQRT(3))/(K3+B4+B10)</f>
         <v>1268.3009343935632</v>
       </c>
-      <c r="G10" s="94">
+      <c r="G10" s="93">
         <v>16</v>
       </c>
-      <c r="H10" s="94">
+      <c r="H10" s="93">
         <v>12.7</v>
       </c>
-      <c r="I10" s="94">
+      <c r="I10" s="93">
         <v>1.23E-2</v>
       </c>
-      <c r="J10" s="94">
+      <c r="J10" s="93">
         <v>0</v>
       </c>
-      <c r="K10" s="94"/>
-      <c r="L10" s="97" t="s">
-        <v>122</v>
+      <c r="K10" s="93"/>
+      <c r="L10" s="96" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="96" t="s">
-        <v>105</v>
-      </c>
-      <c r="B11" s="94">
+      <c r="A11" s="95" t="s">
+        <v>101</v>
+      </c>
+      <c r="B11" s="93">
         <f t="shared" si="0"/>
         <v>9.2499999999999999E-2</v>
       </c>
-      <c r="C11" s="94">
+      <c r="C11" s="93">
         <f>18.5*5/1000</f>
         <v>9.2499999999999999E-2</v>
       </c>
-      <c r="D11" s="94">
+      <c r="D11" s="93">
         <v>0</v>
       </c>
-      <c r="E11" s="94">
+      <c r="E11" s="93">
         <f>(400/SQRT(3))/(K3+2*B4+2*B5+2*B6+2*B11)</f>
         <v>1000.7493205205765</v>
       </c>
-      <c r="F11" s="94">
+      <c r="F11" s="93">
         <f>(400/SQRT(3))/(K3+B4+B5+B6+B11)</f>
         <v>1812.9501566095521</v>
       </c>
-      <c r="G11" s="94">
+      <c r="G11" s="93">
         <v>25</v>
       </c>
-      <c r="H11" s="94">
+      <c r="H11" s="93">
         <v>5</v>
       </c>
-      <c r="I11" s="94">
+      <c r="I11" s="93">
         <v>1.8499999999999999E-2</v>
       </c>
-      <c r="J11" s="94">
+      <c r="J11" s="93">
         <v>0</v>
       </c>
-      <c r="K11" s="94"/>
-      <c r="L11" s="97" t="s">
-        <v>123</v>
+      <c r="K11" s="93"/>
+      <c r="L11" s="96" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="96" t="s">
-        <v>109</v>
-      </c>
-      <c r="B12" s="94">
+      <c r="A12" s="95" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" s="93">
         <f t="shared" si="0"/>
         <v>9.2499999999999999E-2</v>
       </c>
-      <c r="C12" s="94">
+      <c r="C12" s="93">
         <f>18.5*5/1000</f>
         <v>9.2499999999999999E-2</v>
       </c>
-      <c r="D12" s="94">
+      <c r="D12" s="93">
         <v>0</v>
       </c>
-      <c r="E12" s="94">
+      <c r="E12" s="93">
         <f>(400/SQRT(3))/(K3+2*B4+2*B5+2*B7+2*B11)</f>
         <v>677.10410853353619</v>
       </c>
-      <c r="F12" s="94">
+      <c r="F12" s="93">
         <f>(400/SQRT(3))/(K3+B4+B5+B7+B11)</f>
         <v>1265.1815381281567</v>
       </c>
-      <c r="G12" s="94">
+      <c r="G12" s="93">
         <v>16</v>
       </c>
-      <c r="H12" s="94">
+      <c r="H12" s="93">
         <v>5</v>
       </c>
-      <c r="I12" s="94">
+      <c r="I12" s="93">
         <v>1.8499999999999999E-2</v>
       </c>
-      <c r="J12" s="94">
+      <c r="J12" s="93">
         <v>0</v>
       </c>
-      <c r="K12" s="94"/>
-      <c r="L12" s="97" t="s">
-        <v>119</v>
+      <c r="K12" s="93"/>
+      <c r="L12" s="96" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="96" t="s">
-        <v>110</v>
-      </c>
-      <c r="B13" s="94">
+      <c r="A13" s="95" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="93">
         <f t="shared" si="0"/>
         <v>6.1499999999999999E-2</v>
       </c>
-      <c r="C13" s="94">
+      <c r="C13" s="93">
         <f>12.3*5/1000</f>
         <v>6.1499999999999999E-2</v>
       </c>
-      <c r="D13" s="94">
+      <c r="D13" s="93">
         <v>0</v>
       </c>
-      <c r="E13" s="94">
+      <c r="E13" s="93">
         <f>(400/SQRT(3))/(K3+2*B4+2*B5+2*B8+2*B13)</f>
         <v>431.01535107469397</v>
       </c>
-      <c r="F13" s="94">
+      <c r="F13" s="93">
         <f>(400/SQRT(3))/(K3+B4+B5+B8+B13)</f>
         <v>825.07364912446985</v>
       </c>
-      <c r="G13" s="94">
+      <c r="G13" s="93">
         <v>10</v>
       </c>
-      <c r="H13" s="94">
+      <c r="H13" s="93">
         <v>5</v>
       </c>
-      <c r="I13" s="94">
+      <c r="I13" s="93">
         <v>1.23E-2</v>
       </c>
-      <c r="J13" s="94">
+      <c r="J13" s="93">
         <v>0</v>
       </c>
-      <c r="K13" s="94"/>
-      <c r="L13" s="97" t="s">
-        <v>124</v>
+      <c r="K13" s="93"/>
+      <c r="L13" s="96" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="96" t="s">
-        <v>111</v>
-      </c>
-      <c r="B14" s="94">
+      <c r="A14" s="95" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="93">
         <f t="shared" si="0"/>
         <v>6.1499999999999999E-2</v>
       </c>
-      <c r="C14" s="94">
+      <c r="C14" s="93">
         <f t="shared" ref="C14:C15" si="2">12.3*5/1000</f>
         <v>6.1499999999999999E-2</v>
       </c>
-      <c r="D14" s="94">
+      <c r="D14" s="93">
         <v>0</v>
       </c>
-      <c r="E14" s="94">
+      <c r="E14" s="93">
         <f>(400/SQRT(3))/(K3+2*B4+2*B5+2*B9+2*B14)</f>
         <v>247.17325262204693</v>
       </c>
-      <c r="F14" s="94">
+      <c r="F14" s="93">
         <f>(400/SQRT(3))/(K3+B4+B5+B9+B14)</f>
         <v>481.96623945899529</v>
       </c>
-      <c r="G14" s="94">
+      <c r="G14" s="93">
         <v>6</v>
       </c>
-      <c r="H14" s="94">
+      <c r="H14" s="93">
         <v>5</v>
       </c>
-      <c r="I14" s="94">
+      <c r="I14" s="93">
         <v>1.23E-2</v>
       </c>
-      <c r="J14" s="94">
+      <c r="J14" s="93">
         <v>0</v>
       </c>
-      <c r="K14" s="94"/>
-      <c r="L14" s="97" t="s">
-        <v>127</v>
+      <c r="K14" s="93"/>
+      <c r="L14" s="96" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="98" t="s">
-        <v>112</v>
-      </c>
-      <c r="B15" s="99">
+      <c r="A15" s="97" t="s">
+        <v>108</v>
+      </c>
+      <c r="B15" s="98">
         <f t="shared" si="0"/>
         <v>6.1499999999999999E-2</v>
       </c>
-      <c r="C15" s="99">
+      <c r="C15" s="98">
         <f t="shared" si="2"/>
         <v>6.1499999999999999E-2</v>
       </c>
-      <c r="D15" s="99">
+      <c r="D15" s="98">
         <v>0</v>
       </c>
-      <c r="E15" s="99">
+      <c r="E15" s="98">
         <f>(400/SQRT(3))/(K3+2*B4+2*B5+2*B10+2*B15)</f>
         <v>494.59804225229323</v>
       </c>
-      <c r="F15" s="99">
+      <c r="F15" s="98">
         <f>(400/SQRT(3))/(K3+B4+B5+B10+B15)</f>
         <v>940.83693766294198</v>
       </c>
-      <c r="G15" s="99">
+      <c r="G15" s="98">
         <v>10</v>
       </c>
-      <c r="H15" s="99">
+      <c r="H15" s="98">
         <v>5</v>
       </c>
-      <c r="I15" s="99">
+      <c r="I15" s="98">
         <v>1.23E-2</v>
       </c>
-      <c r="J15" s="99">
+      <c r="J15" s="98">
         <v>0</v>
       </c>
-      <c r="K15" s="99"/>
-      <c r="L15" s="100" t="s">
-        <v>126</v>
+      <c r="K15" s="98"/>
+      <c r="L15" s="99" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
going to the college......
</commit_message>
<xml_diff>
--- a/курсач медведь.xlsx
+++ b/курсач медведь.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="135" windowWidth="27480" windowHeight="12600" activeTab="1"/>
+    <workbookView xWindow="720" yWindow="135" windowWidth="27480" windowHeight="12600" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Ведомость электропотребителей" sheetId="1" r:id="rId1"/>
@@ -500,21 +500,15 @@
       <charset val="204"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="50">
+  <borders count="51">
     <border>
       <left/>
       <right/>
@@ -1165,11 +1159,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="134">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1450,12 +1455,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="50" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1526,15 +1553,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1819,7 +1837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
@@ -2657,8 +2675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2670,99 +2688,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="112" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="114" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="102" t="s">
+      <c r="C1" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="102" t="s">
+      <c r="D1" s="110" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102" t="s">
+      <c r="E1" s="110"/>
+      <c r="F1" s="110" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="102" t="s">
+      <c r="G1" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="102" t="s">
+      <c r="H1" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="102" t="s">
+      <c r="I1" s="110" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="102" t="s">
+      <c r="J1" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="102" t="s">
+      <c r="K1" s="110" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="114" t="s">
+      <c r="L1" s="122" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="102" t="s">
+      <c r="M1" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="114" t="s">
+      <c r="N1" s="122" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="114" t="s">
+      <c r="O1" s="122" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="116" t="s">
+      <c r="P1" s="124" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="118" t="s">
+      <c r="Q1" s="126" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="105"/>
-      <c r="B2" s="107"/>
-      <c r="C2" s="103"/>
+      <c r="A2" s="113"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="111"/>
       <c r="D2" s="29" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="115"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="115"/>
-      <c r="O2" s="115"/>
-      <c r="P2" s="117"/>
-      <c r="Q2" s="119"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="123"/>
+      <c r="O2" s="123"/>
+      <c r="P2" s="125"/>
+      <c r="Q2" s="127"/>
     </row>
     <row r="3" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="111" t="s">
+      <c r="A3" s="119" t="s">
         <v>136</v>
       </c>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="112"/>
-      <c r="I3" s="112"/>
-      <c r="J3" s="112"/>
-      <c r="K3" s="112"/>
-      <c r="L3" s="112"/>
-      <c r="M3" s="112"/>
-      <c r="N3" s="112"/>
-      <c r="O3" s="112"/>
-      <c r="P3" s="112"/>
-      <c r="Q3" s="113"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="120"/>
+      <c r="I3" s="120"/>
+      <c r="J3" s="120"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="120"/>
+      <c r="M3" s="120"/>
+      <c r="N3" s="120"/>
+      <c r="O3" s="120"/>
+      <c r="P3" s="120"/>
+      <c r="Q3" s="121"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="58">
@@ -3246,28 +3264,26 @@
         <f>SUM(K4:K12)</f>
         <v>473.73159999999996</v>
       </c>
-      <c r="L13" s="37">
-        <f>_xlfn.FLOOR.MATH(E13*E13/K13)</f>
-        <v>7</v>
-      </c>
+      <c r="L13" s="37"/>
       <c r="M13" s="30">
-        <v>1.21</v>
+        <f>M33</f>
+        <v>1.1599999999999999</v>
       </c>
       <c r="N13" s="30">
         <f>I13*M13</f>
-        <v>49.878673777777792</v>
+        <v>47.817571555555567</v>
       </c>
       <c r="O13" s="30">
         <f>J13*M13</f>
-        <v>16.394327258157297</v>
+        <v>15.716875718564019</v>
       </c>
       <c r="P13" s="30">
         <f>SQRT(O13*O13+N13*N13)</f>
-        <v>52.503867134502933</v>
+        <v>50.334285847953218</v>
       </c>
       <c r="Q13" s="38">
         <f>P13*1000/(380*SQRT(3))</f>
-        <v>79.771373220004264</v>
+        <v>76.475035483640426</v>
       </c>
       <c r="R13">
         <f>I13/E13</f>
@@ -3275,25 +3291,25 @@
       </c>
     </row>
     <row r="14" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="111" t="s">
+      <c r="A14" s="119" t="s">
         <v>137</v>
       </c>
-      <c r="B14" s="112"/>
-      <c r="C14" s="112"/>
-      <c r="D14" s="112"/>
-      <c r="E14" s="112"/>
-      <c r="F14" s="112"/>
-      <c r="G14" s="112"/>
-      <c r="H14" s="112"/>
-      <c r="I14" s="112"/>
-      <c r="J14" s="112"/>
-      <c r="K14" s="112"/>
-      <c r="L14" s="112"/>
-      <c r="M14" s="112"/>
-      <c r="N14" s="112"/>
-      <c r="O14" s="112"/>
-      <c r="P14" s="112"/>
-      <c r="Q14" s="113"/>
+      <c r="B14" s="120"/>
+      <c r="C14" s="120"/>
+      <c r="D14" s="120"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="120"/>
+      <c r="G14" s="120"/>
+      <c r="H14" s="120"/>
+      <c r="I14" s="120"/>
+      <c r="J14" s="120"/>
+      <c r="K14" s="120"/>
+      <c r="L14" s="120"/>
+      <c r="M14" s="120"/>
+      <c r="N14" s="120"/>
+      <c r="O14" s="120"/>
+      <c r="P14" s="120"/>
+      <c r="Q14" s="121"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="41">
@@ -3720,28 +3736,26 @@
         <f>SUM(K15:K22)</f>
         <v>387.11970000000002</v>
       </c>
-      <c r="L23" s="30">
-        <f>_xlfn.FLOOR.MATH(E23*E23/K23)</f>
-        <v>7</v>
-      </c>
+      <c r="L23" s="30"/>
       <c r="M23" s="30">
-        <v>1.21</v>
+        <f>M33</f>
+        <v>1.1599999999999999</v>
       </c>
       <c r="N23" s="30">
         <f>I23*M23</f>
-        <v>42.34984875</v>
+        <v>40.599854999999998</v>
       </c>
       <c r="O23" s="30">
         <f>J23*M23</f>
-        <v>13.919722140853928</v>
+        <v>13.344527011066575</v>
       </c>
       <c r="P23" s="30">
         <f>SQRT(O23*O23+N23*N23)</f>
-        <v>44.578788157894735</v>
+        <v>42.736689473684201</v>
       </c>
       <c r="Q23" s="38">
         <f>P23*1000/(380*SQRT(3))</f>
-        <v>67.730461429231127</v>
+        <v>64.931682031329004</v>
       </c>
       <c r="R23">
         <f>I23/E23</f>
@@ -3749,25 +3763,25 @@
       </c>
     </row>
     <row r="24" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="111" t="s">
+      <c r="A24" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="112"/>
-      <c r="C24" s="112"/>
-      <c r="D24" s="112"/>
-      <c r="E24" s="112"/>
-      <c r="F24" s="112"/>
-      <c r="G24" s="112"/>
-      <c r="H24" s="112"/>
-      <c r="I24" s="112"/>
-      <c r="J24" s="112"/>
-      <c r="K24" s="112"/>
-      <c r="L24" s="112"/>
-      <c r="M24" s="112"/>
-      <c r="N24" s="112"/>
-      <c r="O24" s="112"/>
-      <c r="P24" s="112"/>
-      <c r="Q24" s="113"/>
+      <c r="B24" s="120"/>
+      <c r="C24" s="120"/>
+      <c r="D24" s="120"/>
+      <c r="E24" s="120"/>
+      <c r="F24" s="120"/>
+      <c r="G24" s="120"/>
+      <c r="H24" s="120"/>
+      <c r="I24" s="120"/>
+      <c r="J24" s="120"/>
+      <c r="K24" s="120"/>
+      <c r="L24" s="120"/>
+      <c r="M24" s="120"/>
+      <c r="N24" s="120"/>
+      <c r="O24" s="120"/>
+      <c r="P24" s="120"/>
+      <c r="Q24" s="121"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="41">
@@ -3856,50 +3870,48 @@
         <f>SUM(K25)</f>
         <v>163.84000000000003</v>
       </c>
-      <c r="L26" s="29">
-        <f>_xlfn.FLOOR.MATH(E26*E26/K26)</f>
-        <v>1</v>
-      </c>
+      <c r="L26" s="29"/>
       <c r="M26" s="29">
-        <v>2.67</v>
+        <f>M33</f>
+        <v>1.1599999999999999</v>
       </c>
       <c r="N26" s="29">
         <f>I26*M26</f>
-        <v>10.252799999999999</v>
+        <v>4.4543999999999997</v>
       </c>
       <c r="O26" s="29">
         <f>J26*M26</f>
-        <v>3.369932393577848</v>
+        <v>1.4640904781087281</v>
       </c>
       <c r="P26" s="18">
         <f>SQRT(O36*O26+N26*N26)</f>
-        <v>10.252799999999999</v>
+        <v>4.4543999999999997</v>
       </c>
       <c r="Q26" s="16">
         <f>P26*1000/(380*SQRT(3))</f>
-        <v>15.577517999861566</v>
+        <v>6.7677606291533392</v>
       </c>
     </row>
     <row r="27" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="111" t="s">
+      <c r="A27" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="112"/>
-      <c r="C27" s="112"/>
-      <c r="D27" s="112"/>
-      <c r="E27" s="112"/>
-      <c r="F27" s="112"/>
-      <c r="G27" s="112"/>
-      <c r="H27" s="112"/>
-      <c r="I27" s="112"/>
-      <c r="J27" s="112"/>
-      <c r="K27" s="112"/>
-      <c r="L27" s="112"/>
-      <c r="M27" s="112"/>
-      <c r="N27" s="112"/>
-      <c r="O27" s="112"/>
-      <c r="P27" s="112"/>
-      <c r="Q27" s="113"/>
+      <c r="B27" s="120"/>
+      <c r="C27" s="120"/>
+      <c r="D27" s="120"/>
+      <c r="E27" s="120"/>
+      <c r="F27" s="120"/>
+      <c r="G27" s="120"/>
+      <c r="H27" s="120"/>
+      <c r="I27" s="120"/>
+      <c r="J27" s="120"/>
+      <c r="K27" s="120"/>
+      <c r="L27" s="120"/>
+      <c r="M27" s="120"/>
+      <c r="N27" s="120"/>
+      <c r="O27" s="120"/>
+      <c r="P27" s="120"/>
+      <c r="Q27" s="121"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="41">
@@ -3988,50 +4000,48 @@
         <f>SUM(K28)</f>
         <v>139.24</v>
       </c>
-      <c r="L29" s="29">
-        <f>_xlfn.FLOOR.MATH(E29*E29/K29)</f>
-        <v>1</v>
-      </c>
+      <c r="L29" s="29"/>
       <c r="M29" s="29">
-        <v>8</v>
+        <f>M33</f>
+        <v>1.1599999999999999</v>
       </c>
       <c r="N29" s="29">
         <f>I29*M29</f>
-        <v>9.4400000000000013</v>
+        <v>1.3688</v>
       </c>
       <c r="O29" s="29">
         <f>J29*M29</f>
-        <v>3.1027779528884691</v>
+        <v>0.44990280316882797</v>
       </c>
       <c r="P29" s="18">
         <f>SQRT(O29*O29+N29*N29)</f>
-        <v>9.9368421052631604</v>
+        <v>1.4408421052631579</v>
       </c>
       <c r="Q29" s="16">
         <f>P29*1000/(380*SQRT(3))</f>
-        <v>15.097469643074984</v>
+        <v>2.1891330982458723</v>
       </c>
     </row>
     <row r="30" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="111" t="s">
+      <c r="A30" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="112"/>
-      <c r="C30" s="112"/>
-      <c r="D30" s="112"/>
-      <c r="E30" s="112"/>
-      <c r="F30" s="112"/>
-      <c r="G30" s="112"/>
-      <c r="H30" s="112"/>
-      <c r="I30" s="112"/>
-      <c r="J30" s="112"/>
-      <c r="K30" s="112"/>
-      <c r="L30" s="112"/>
-      <c r="M30" s="112"/>
-      <c r="N30" s="112"/>
-      <c r="O30" s="112"/>
-      <c r="P30" s="112"/>
-      <c r="Q30" s="113"/>
+      <c r="B30" s="120"/>
+      <c r="C30" s="120"/>
+      <c r="D30" s="120"/>
+      <c r="E30" s="120"/>
+      <c r="F30" s="120"/>
+      <c r="G30" s="120"/>
+      <c r="H30" s="120"/>
+      <c r="I30" s="120"/>
+      <c r="J30" s="120"/>
+      <c r="K30" s="120"/>
+      <c r="L30" s="120"/>
+      <c r="M30" s="120"/>
+      <c r="N30" s="120"/>
+      <c r="O30" s="120"/>
+      <c r="P30" s="120"/>
+      <c r="Q30" s="121"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="41">
@@ -4120,28 +4130,26 @@
         <f>SUM(K31)</f>
         <v>163.84000000000003</v>
       </c>
-      <c r="L32" s="29">
-        <f>_xlfn.FLOOR.MATH(E32*E32/K32)</f>
-        <v>1</v>
-      </c>
+      <c r="L32" s="29"/>
       <c r="M32" s="29">
-        <v>2.67</v>
+        <f>M33</f>
+        <v>1.1599999999999999</v>
       </c>
       <c r="N32" s="29">
         <f>I32*M32</f>
-        <v>10.252799999999999</v>
+        <v>4.4543999999999997</v>
       </c>
       <c r="O32" s="29">
         <f>J32*M32</f>
-        <v>3.369932393577848</v>
+        <v>1.4640904781087281</v>
       </c>
       <c r="P32" s="18">
         <f>SQRT(O32*O32+N32*N32)</f>
-        <v>10.792421052631578</v>
+        <v>4.6888421052631575</v>
       </c>
       <c r="Q32" s="16">
         <f>P32*1000/(380*SQRT(3))</f>
-        <v>16.397387368275332</v>
+        <v>7.1239585570035153</v>
       </c>
     </row>
     <row r="33" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -4185,7 +4193,7 @@
         <f>SUM(K32,K29,K26,K23,K13)</f>
         <v>1327.7712999999999</v>
       </c>
-      <c r="L33" s="30">
+      <c r="L33" s="104">
         <f>_xlfn.FLOOR.MATH(E33*E33/K33)</f>
         <v>17</v>
       </c>
@@ -4214,25 +4222,25 @@
       </c>
     </row>
     <row r="34" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="108" t="s">
+      <c r="A34" s="116" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="109"/>
-      <c r="C34" s="109"/>
-      <c r="D34" s="109"/>
-      <c r="E34" s="109"/>
-      <c r="F34" s="109"/>
-      <c r="G34" s="109"/>
-      <c r="H34" s="109"/>
-      <c r="I34" s="109"/>
-      <c r="J34" s="109"/>
-      <c r="K34" s="109"/>
-      <c r="L34" s="109"/>
-      <c r="M34" s="109"/>
-      <c r="N34" s="109"/>
-      <c r="O34" s="109"/>
-      <c r="P34" s="109"/>
-      <c r="Q34" s="110"/>
+      <c r="B34" s="117"/>
+      <c r="C34" s="117"/>
+      <c r="D34" s="117"/>
+      <c r="E34" s="117"/>
+      <c r="F34" s="117"/>
+      <c r="G34" s="117"/>
+      <c r="H34" s="117"/>
+      <c r="I34" s="117"/>
+      <c r="J34" s="117"/>
+      <c r="K34" s="117"/>
+      <c r="L34" s="117"/>
+      <c r="M34" s="117"/>
+      <c r="N34" s="117"/>
+      <c r="O34" s="117"/>
+      <c r="P34" s="117"/>
+      <c r="Q34" s="118"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
@@ -4407,51 +4415,51 @@
         <v>72</v>
       </c>
       <c r="B39" s="8"/>
-      <c r="C39" s="69">
+      <c r="C39" s="106">
         <f>SUM(C35:C38)</f>
         <v>83</v>
       </c>
-      <c r="D39" s="10"/>
-      <c r="E39" s="30">
+      <c r="D39" s="81"/>
+      <c r="E39" s="105">
         <f>SUM(E35:E38)</f>
         <v>3.4920000000000004</v>
       </c>
-      <c r="F39" s="30">
+      <c r="F39" s="105">
         <f>AVERAGE(F35:F38)</f>
         <v>0.7</v>
       </c>
-      <c r="G39" s="30">
+      <c r="G39" s="105">
         <f>AVERAGE(G35:G38)</f>
         <v>0.98</v>
       </c>
-      <c r="H39" s="30">
+      <c r="H39" s="105">
         <f>AVERAGE(H35:H38)</f>
         <v>0.20305866063400418</v>
       </c>
-      <c r="I39" s="30">
+      <c r="I39" s="105">
         <f>SUM(I35:I38)</f>
         <v>2.4443999999999999</v>
       </c>
-      <c r="J39" s="30">
+      <c r="J39" s="105">
         <f t="shared" si="15"/>
         <v>0.49635659005375982</v>
       </c>
-      <c r="K39" s="30"/>
-      <c r="L39" s="30"/>
-      <c r="M39" s="30"/>
-      <c r="N39" s="30">
+      <c r="K39" s="105"/>
+      <c r="L39" s="105"/>
+      <c r="M39" s="105"/>
+      <c r="N39" s="105">
         <f>I39</f>
         <v>2.4443999999999999</v>
       </c>
-      <c r="O39" s="30">
+      <c r="O39" s="105">
         <f>J39</f>
         <v>0.49635659005375982</v>
       </c>
-      <c r="P39" s="30">
+      <c r="P39" s="105">
         <f>SQRT(N39*N39+O39*O39)</f>
         <v>2.4942857142857142</v>
       </c>
-      <c r="Q39" s="38">
+      <c r="Q39" s="107">
         <f>P39*1000/(220*SQRT(3))</f>
         <v>6.5458024026304322</v>
       </c>
@@ -4461,45 +4469,45 @@
         <v>47</v>
       </c>
       <c r="B40" s="8"/>
-      <c r="C40" s="69">
+      <c r="C40" s="108">
         <f>C39+C33</f>
         <v>103</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
-      <c r="G40" s="101">
+      <c r="G40" s="109">
         <f>(G39*E39+G33*E33)/(E33+E39)</f>
         <v>0.95067656062308648</v>
       </c>
-      <c r="H40" s="101">
+      <c r="H40" s="109">
         <f>(H39*E39+H33*E33)/(E33+E39)</f>
         <v>0.32585099754430247</v>
       </c>
-      <c r="I40" s="128">
+      <c r="I40" s="109">
         <f>I39+I33</f>
         <v>93.784124999999989</v>
       </c>
-      <c r="J40" s="30">
+      <c r="J40" s="100">
         <f t="shared" si="15"/>
         <v>30.559650685069553</v>
       </c>
-      <c r="K40" s="30"/>
-      <c r="L40" s="30"/>
-      <c r="M40" s="30"/>
-      <c r="N40" s="30">
+      <c r="K40" s="100"/>
+      <c r="L40" s="100"/>
+      <c r="M40" s="100"/>
+      <c r="N40" s="100">
         <f>N39+N33</f>
         <v>108.39848099999998</v>
       </c>
-      <c r="O40" s="30">
+      <c r="O40" s="100">
         <f>O39+O33</f>
         <v>35.321778893587535</v>
       </c>
-      <c r="P40" s="30">
+      <c r="P40" s="100">
         <f>SQRT(O40*O40+N40*N40)</f>
         <v>114.00815210902614</v>
       </c>
-      <c r="Q40" s="100">
+      <c r="Q40" s="101">
         <f>P40*1000/(380*SQRT(3))</f>
         <v>173.21746660515277</v>
       </c>
@@ -4670,8 +4678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="U26" sqref="U26"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -4735,22 +4743,22 @@
       <c r="O1" s="78"/>
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="108" t="s">
+      <c r="A2" s="116" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="109"/>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
-      <c r="E2" s="109"/>
-      <c r="F2" s="109"/>
-      <c r="G2" s="109"/>
-      <c r="H2" s="109"/>
-      <c r="I2" s="109"/>
-      <c r="J2" s="109"/>
-      <c r="K2" s="109"/>
-      <c r="L2" s="109"/>
-      <c r="M2" s="109"/>
-      <c r="N2" s="110"/>
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="117"/>
+      <c r="M2" s="117"/>
+      <c r="N2" s="118"/>
       <c r="O2" s="78"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -4800,7 +4808,7 @@
       <c r="M3" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="N3" s="126">
+      <c r="N3" s="102">
         <f>K3</f>
         <v>25</v>
       </c>
@@ -4853,7 +4861,7 @@
       <c r="M4" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="N4" s="126">
+      <c r="N4" s="102">
         <f t="shared" ref="N4:N12" si="4">K4</f>
         <v>16</v>
       </c>
@@ -4906,7 +4914,7 @@
       <c r="M5" s="72" t="s">
         <v>147</v>
       </c>
-      <c r="N5" s="126">
+      <c r="N5" s="102">
         <f t="shared" si="4"/>
         <v>32</v>
       </c>
@@ -4959,7 +4967,7 @@
       <c r="M6" s="72" t="s">
         <v>147</v>
       </c>
-      <c r="N6" s="126">
+      <c r="N6" s="102">
         <f t="shared" si="4"/>
         <v>32</v>
       </c>
@@ -5012,7 +5020,7 @@
       <c r="M7" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="N7" s="126">
+      <c r="N7" s="102">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
@@ -5065,7 +5073,7 @@
       <c r="M8" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="N8" s="126">
+      <c r="N8" s="102">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
@@ -5118,7 +5126,7 @@
       <c r="M9" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="N9" s="126">
+      <c r="N9" s="102">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
@@ -5171,7 +5179,7 @@
       <c r="M10" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="N10" s="126">
+      <c r="N10" s="102">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
@@ -5224,7 +5232,7 @@
       <c r="M11" s="73" t="s">
         <v>145</v>
       </c>
-      <c r="N11" s="126">
+      <c r="N11" s="102">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
@@ -5237,7 +5245,7 @@
       </c>
       <c r="C12" s="77">
         <f>'Расчет электрических нагрузок'!Q13</f>
-        <v>79.771373220004264</v>
+        <v>76.475035483640426</v>
       </c>
       <c r="D12" s="73">
         <f>SUM(C3:C11)+MAX(D3:D11)-MAX(C3:C11)</f>
@@ -5245,7 +5253,7 @@
       </c>
       <c r="E12" s="7">
         <f t="shared" si="0"/>
-        <v>93.848674376475614</v>
+        <v>89.970629980753444</v>
       </c>
       <c r="F12" s="71">
         <v>100</v>
@@ -5275,29 +5283,29 @@
       <c r="M12" s="73" t="s">
         <v>148</v>
       </c>
-      <c r="N12" s="126">
+      <c r="N12" s="102">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="O12" s="78"/>
     </row>
     <row r="13" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="108" t="s">
+      <c r="A13" s="116" t="s">
         <v>137</v>
       </c>
-      <c r="B13" s="109"/>
-      <c r="C13" s="109"/>
-      <c r="D13" s="109"/>
-      <c r="E13" s="109"/>
-      <c r="F13" s="109"/>
-      <c r="G13" s="109"/>
-      <c r="H13" s="109"/>
-      <c r="I13" s="109"/>
-      <c r="J13" s="109"/>
-      <c r="K13" s="109"/>
-      <c r="L13" s="109"/>
-      <c r="M13" s="109"/>
-      <c r="N13" s="110"/>
+      <c r="B13" s="117"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117"/>
+      <c r="G13" s="117"/>
+      <c r="H13" s="117"/>
+      <c r="I13" s="117"/>
+      <c r="J13" s="117"/>
+      <c r="K13" s="117"/>
+      <c r="L13" s="117"/>
+      <c r="M13" s="117"/>
+      <c r="N13" s="118"/>
       <c r="O13" s="78"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -5347,7 +5355,7 @@
       <c r="M14" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="N14" s="126">
+      <c r="N14" s="102">
         <f>K14</f>
         <v>32</v>
       </c>
@@ -5400,7 +5408,7 @@
       <c r="M15" s="72" t="s">
         <v>147</v>
       </c>
-      <c r="N15" s="126">
+      <c r="N15" s="102">
         <f t="shared" ref="N15:N22" si="10">K15</f>
         <v>32</v>
       </c>
@@ -5453,7 +5461,7 @@
       <c r="M16" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="N16" s="126">
+      <c r="N16" s="102">
         <f t="shared" si="10"/>
         <v>25</v>
       </c>
@@ -5506,7 +5514,7 @@
       <c r="M17" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="N17" s="126">
+      <c r="N17" s="102">
         <f t="shared" si="10"/>
         <v>16</v>
       </c>
@@ -5559,7 +5567,7 @@
       <c r="M18" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="N18" s="126">
+      <c r="N18" s="102">
         <f t="shared" si="10"/>
         <v>16</v>
       </c>
@@ -5612,7 +5620,7 @@
       <c r="M19" s="72" t="s">
         <v>146</v>
       </c>
-      <c r="N19" s="126">
+      <c r="N19" s="102">
         <f t="shared" si="10"/>
         <v>16</v>
       </c>
@@ -5665,7 +5673,7 @@
       <c r="M20" s="72" t="s">
         <v>145</v>
       </c>
-      <c r="N20" s="126">
+      <c r="N20" s="102">
         <f t="shared" si="10"/>
         <v>25</v>
       </c>
@@ -5718,7 +5726,7 @@
       <c r="M21" s="73" t="s">
         <v>146</v>
       </c>
-      <c r="N21" s="126">
+      <c r="N21" s="102">
         <f t="shared" si="10"/>
         <v>16</v>
       </c>
@@ -5731,7 +5739,7 @@
       </c>
       <c r="C22" s="77">
         <f>'Расчет электрических нагрузок'!Q23</f>
-        <v>67.730461429231127</v>
+        <v>64.931682031329004</v>
       </c>
       <c r="D22" s="73">
         <f>SUM(C14:C21)+MAX(D14:D21)-MAX(C14:C21)</f>
@@ -5739,7 +5747,7 @@
       </c>
       <c r="E22" s="7">
         <f t="shared" si="6"/>
-        <v>79.682895799095448</v>
+        <v>76.390214154504719</v>
       </c>
       <c r="F22" s="71">
         <v>100</v>
@@ -5769,29 +5777,29 @@
       <c r="M22" s="73" t="s">
         <v>148</v>
       </c>
-      <c r="N22" s="126">
+      <c r="N22" s="102">
         <f t="shared" si="10"/>
         <v>100</v>
       </c>
       <c r="O22" s="78"/>
     </row>
     <row r="23" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="108" t="s">
+      <c r="A23" s="116" t="s">
         <v>91</v>
       </c>
-      <c r="B23" s="109"/>
-      <c r="C23" s="109"/>
-      <c r="D23" s="109"/>
-      <c r="E23" s="109"/>
-      <c r="F23" s="109"/>
-      <c r="G23" s="109"/>
-      <c r="H23" s="109"/>
-      <c r="I23" s="109"/>
-      <c r="J23" s="109"/>
-      <c r="K23" s="109"/>
-      <c r="L23" s="109"/>
-      <c r="M23" s="109"/>
-      <c r="N23" s="110"/>
+      <c r="B23" s="117"/>
+      <c r="C23" s="117"/>
+      <c r="D23" s="117"/>
+      <c r="E23" s="117"/>
+      <c r="F23" s="117"/>
+      <c r="G23" s="117"/>
+      <c r="H23" s="117"/>
+      <c r="I23" s="117"/>
+      <c r="J23" s="117"/>
+      <c r="K23" s="117"/>
+      <c r="L23" s="117"/>
+      <c r="M23" s="117"/>
+      <c r="N23" s="118"/>
       <c r="O23" s="78"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -5842,7 +5850,7 @@
       <c r="M24" s="7" t="s">
         <v>148</v>
       </c>
-      <c r="N24" s="126">
+      <c r="N24" s="102">
         <f>K24</f>
         <v>100</v>
       </c>
@@ -5896,7 +5904,7 @@
       <c r="M25" s="72" t="s">
         <v>149</v>
       </c>
-      <c r="N25" s="126">
+      <c r="N25" s="102">
         <f t="shared" ref="N25:N26" si="14">K25</f>
         <v>160</v>
       </c>
@@ -5949,29 +5957,29 @@
       <c r="M26" s="73" t="s">
         <v>148</v>
       </c>
-      <c r="N26" s="126">
+      <c r="N26" s="102">
         <f t="shared" si="14"/>
         <v>100</v>
       </c>
       <c r="O26" s="78"/>
     </row>
     <row r="27" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="108" t="s">
+      <c r="A27" s="116" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="109"/>
-      <c r="C27" s="109"/>
-      <c r="D27" s="109"/>
-      <c r="E27" s="109"/>
-      <c r="F27" s="109"/>
-      <c r="G27" s="109"/>
-      <c r="H27" s="109"/>
-      <c r="I27" s="109"/>
-      <c r="J27" s="109"/>
-      <c r="K27" s="109"/>
-      <c r="L27" s="109"/>
-      <c r="M27" s="109"/>
-      <c r="N27" s="110"/>
+      <c r="B27" s="117"/>
+      <c r="C27" s="117"/>
+      <c r="D27" s="117"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="117"/>
+      <c r="G27" s="117"/>
+      <c r="H27" s="117"/>
+      <c r="I27" s="117"/>
+      <c r="J27" s="117"/>
+      <c r="K27" s="117"/>
+      <c r="L27" s="117"/>
+      <c r="M27" s="117"/>
+      <c r="N27" s="118"/>
       <c r="O27" s="78"/>
     </row>
     <row r="28" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -5983,7 +5991,7 @@
       </c>
       <c r="D28" s="86">
         <f>SUM(C24:C26,C22,C12)+MAX(D24:D26,D22,D12)-MAX(C24:C26,C22,C12)</f>
-        <v>704.82267226032639</v>
+        <v>698.72755512606045</v>
       </c>
       <c r="E28" s="86">
         <f>C28/0.85</f>
@@ -5994,7 +6002,7 @@
       </c>
       <c r="G28" s="86">
         <f>D28*1.25</f>
-        <v>881.02834032540795</v>
+        <v>873.40944390757556</v>
       </c>
       <c r="H28" s="92">
         <f>7*F28</f>
@@ -6017,7 +6025,7 @@
       <c r="M28" s="86" t="s">
         <v>150</v>
       </c>
-      <c r="N28" s="127">
+      <c r="N28" s="103">
         <f>K28</f>
         <v>250</v>
       </c>
@@ -6073,56 +6081,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="124"/>
-      <c r="B1" s="120" t="s">
+      <c r="A1" s="132"/>
+      <c r="B1" s="128" t="s">
         <v>129</v>
       </c>
-      <c r="C1" s="120" t="s">
+      <c r="C1" s="128" t="s">
         <v>128</v>
       </c>
-      <c r="D1" s="120" t="s">
+      <c r="D1" s="128" t="s">
         <v>127</v>
       </c>
-      <c r="E1" s="120" t="s">
+      <c r="E1" s="128" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="120"/>
-      <c r="G1" s="120" t="s">
+      <c r="F1" s="128"/>
+      <c r="G1" s="128" t="s">
         <v>125</v>
       </c>
-      <c r="H1" s="120" t="s">
+      <c r="H1" s="128" t="s">
         <v>131</v>
       </c>
-      <c r="I1" s="120" t="s">
+      <c r="I1" s="128" t="s">
         <v>132</v>
       </c>
-      <c r="J1" s="120" t="s">
+      <c r="J1" s="128" t="s">
         <v>133</v>
       </c>
-      <c r="K1" s="120" t="s">
+      <c r="K1" s="128" t="s">
         <v>130</v>
       </c>
-      <c r="L1" s="122" t="s">
+      <c r="L1" s="130" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="125"/>
-      <c r="B2" s="121"/>
-      <c r="C2" s="121"/>
-      <c r="D2" s="121"/>
+      <c r="A2" s="133"/>
+      <c r="B2" s="129"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
       <c r="E2" s="94" t="s">
         <v>126</v>
       </c>
       <c r="F2" s="94" t="s">
         <v>124</v>
       </c>
-      <c r="G2" s="121"/>
-      <c r="H2" s="121"/>
-      <c r="I2" s="121"/>
-      <c r="J2" s="121"/>
-      <c r="K2" s="121"/>
-      <c r="L2" s="123"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="129"/>
+      <c r="I2" s="129"/>
+      <c r="J2" s="129"/>
+      <c r="K2" s="129"/>
+      <c r="L2" s="131"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="95" t="s">

</xml_diff>

<commit_message>
i have killed this course project (and listened present perfect)
</commit_message>
<xml_diff>
--- a/курсач медведь.xlsx
+++ b/курсач медведь.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="135" windowWidth="27480" windowHeight="12600" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="720" yWindow="135" windowWidth="27480" windowHeight="12600" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Ведомость электропотребителей" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Расчет освещения" sheetId="3" r:id="rId3"/>
     <sheet name="Выбор защиты" sheetId="4" r:id="rId4"/>
     <sheet name="КЗ" sheetId="5" r:id="rId5"/>
+    <sheet name="Чтение по жипегу" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="176">
   <si>
     <t>Наименование потребителя</t>
   </si>
@@ -479,6 +480,78 @@
   </si>
   <si>
     <t>ВВГнг-LS 4*35 мм2</t>
+  </si>
+  <si>
+    <t>Отношение расстояний между вертикальными электродами к их длине</t>
+  </si>
+  <si>
+    <t>Число вертикальных электродов</t>
+  </si>
+  <si>
+    <t>nтр</t>
+  </si>
+  <si>
+    <t>0.66 - 0.72</t>
+  </si>
+  <si>
+    <t>0.58 - 0.65</t>
+  </si>
+  <si>
+    <t>0.52 - 0.58</t>
+  </si>
+  <si>
+    <t>0.44 - 0.50</t>
+  </si>
+  <si>
+    <t>0.38 - 0.44</t>
+  </si>
+  <si>
+    <t>0.36 - 0.42</t>
+  </si>
+  <si>
+    <t>0.33 - 0.39</t>
+  </si>
+  <si>
+    <t>0.76 - 0.80</t>
+  </si>
+  <si>
+    <t>0.71 - 0.75</t>
+  </si>
+  <si>
+    <t>0.66 - 0.71</t>
+  </si>
+  <si>
+    <t>0.61 - 0.66</t>
+  </si>
+  <si>
+    <t>0.55 - 0.61</t>
+  </si>
+  <si>
+    <t>0.49 - 0.55</t>
+  </si>
+  <si>
+    <t>0.84 - 0.86</t>
+  </si>
+  <si>
+    <t>0.78- 0.82</t>
+  </si>
+  <si>
+    <t>0.74 - 0.78</t>
+  </si>
+  <si>
+    <t>0.68 - 0.73</t>
+  </si>
+  <si>
+    <t>0.64 - 0.69</t>
+  </si>
+  <si>
+    <t>0.62 - 0.67</t>
+  </si>
+  <si>
+    <t>0.59 - 0.65</t>
+  </si>
+  <si>
+    <t>45 + 3</t>
   </si>
 </sst>
 </file>
@@ -505,7 +578,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="51">
+  <borders count="54">
     <border>
       <left/>
       <right/>
@@ -1167,11 +1240,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1480,6 +1590,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1516,24 +1644,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1551,6 +1661,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1824,7 +1958,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2672,8 +2806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T32" sqref="T32"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G46" sqref="G46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2685,99 +2819,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="124" t="s">
+      <c r="A1" s="112" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="126" t="s">
+      <c r="B1" s="114" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="122" t="s">
+      <c r="C1" s="110" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="122" t="s">
+      <c r="D1" s="110" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122" t="s">
+      <c r="E1" s="110"/>
+      <c r="F1" s="110" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="122" t="s">
+      <c r="G1" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="122" t="s">
+      <c r="H1" s="110" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="122" t="s">
+      <c r="I1" s="110" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="122" t="s">
+      <c r="J1" s="110" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="122" t="s">
+      <c r="K1" s="110" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="116" t="s">
+      <c r="L1" s="122" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="122" t="s">
+      <c r="M1" s="110" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="116" t="s">
+      <c r="N1" s="122" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="116" t="s">
+      <c r="O1" s="122" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="118" t="s">
+      <c r="P1" s="124" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="120" t="s">
+      <c r="Q1" s="126" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="125"/>
-      <c r="B2" s="127"/>
-      <c r="C2" s="123"/>
+      <c r="A2" s="113"/>
+      <c r="B2" s="115"/>
+      <c r="C2" s="111"/>
       <c r="D2" s="29" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="123"/>
-      <c r="I2" s="123"/>
-      <c r="J2" s="123"/>
-      <c r="K2" s="123"/>
-      <c r="L2" s="117"/>
-      <c r="M2" s="123"/>
-      <c r="N2" s="117"/>
-      <c r="O2" s="117"/>
-      <c r="P2" s="119"/>
-      <c r="Q2" s="121"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="123"/>
+      <c r="O2" s="123"/>
+      <c r="P2" s="125"/>
+      <c r="Q2" s="127"/>
     </row>
     <row r="3" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="113" t="s">
+      <c r="A3" s="119" t="s">
         <v>136</v>
       </c>
-      <c r="B3" s="114"/>
-      <c r="C3" s="114"/>
-      <c r="D3" s="114"/>
-      <c r="E3" s="114"/>
-      <c r="F3" s="114"/>
-      <c r="G3" s="114"/>
-      <c r="H3" s="114"/>
-      <c r="I3" s="114"/>
-      <c r="J3" s="114"/>
-      <c r="K3" s="114"/>
-      <c r="L3" s="114"/>
-      <c r="M3" s="114"/>
-      <c r="N3" s="114"/>
-      <c r="O3" s="114"/>
-      <c r="P3" s="114"/>
-      <c r="Q3" s="115"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="120"/>
+      <c r="I3" s="120"/>
+      <c r="J3" s="120"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="120"/>
+      <c r="M3" s="120"/>
+      <c r="N3" s="120"/>
+      <c r="O3" s="120"/>
+      <c r="P3" s="120"/>
+      <c r="Q3" s="121"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="58">
@@ -3288,25 +3422,25 @@
       </c>
     </row>
     <row r="14" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="113" t="s">
+      <c r="A14" s="119" t="s">
         <v>137</v>
       </c>
-      <c r="B14" s="114"/>
-      <c r="C14" s="114"/>
-      <c r="D14" s="114"/>
-      <c r="E14" s="114"/>
-      <c r="F14" s="114"/>
-      <c r="G14" s="114"/>
-      <c r="H14" s="114"/>
-      <c r="I14" s="114"/>
-      <c r="J14" s="114"/>
-      <c r="K14" s="114"/>
-      <c r="L14" s="114"/>
-      <c r="M14" s="114"/>
-      <c r="N14" s="114"/>
-      <c r="O14" s="114"/>
-      <c r="P14" s="114"/>
-      <c r="Q14" s="115"/>
+      <c r="B14" s="120"/>
+      <c r="C14" s="120"/>
+      <c r="D14" s="120"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="120"/>
+      <c r="G14" s="120"/>
+      <c r="H14" s="120"/>
+      <c r="I14" s="120"/>
+      <c r="J14" s="120"/>
+      <c r="K14" s="120"/>
+      <c r="L14" s="120"/>
+      <c r="M14" s="120"/>
+      <c r="N14" s="120"/>
+      <c r="O14" s="120"/>
+      <c r="P14" s="120"/>
+      <c r="Q14" s="121"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="41">
@@ -3760,25 +3894,25 @@
       </c>
     </row>
     <row r="24" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="113" t="s">
+      <c r="A24" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="114"/>
-      <c r="C24" s="114"/>
-      <c r="D24" s="114"/>
-      <c r="E24" s="114"/>
-      <c r="F24" s="114"/>
-      <c r="G24" s="114"/>
-      <c r="H24" s="114"/>
-      <c r="I24" s="114"/>
-      <c r="J24" s="114"/>
-      <c r="K24" s="114"/>
-      <c r="L24" s="114"/>
-      <c r="M24" s="114"/>
-      <c r="N24" s="114"/>
-      <c r="O24" s="114"/>
-      <c r="P24" s="114"/>
-      <c r="Q24" s="115"/>
+      <c r="B24" s="120"/>
+      <c r="C24" s="120"/>
+      <c r="D24" s="120"/>
+      <c r="E24" s="120"/>
+      <c r="F24" s="120"/>
+      <c r="G24" s="120"/>
+      <c r="H24" s="120"/>
+      <c r="I24" s="120"/>
+      <c r="J24" s="120"/>
+      <c r="K24" s="120"/>
+      <c r="L24" s="120"/>
+      <c r="M24" s="120"/>
+      <c r="N24" s="120"/>
+      <c r="O24" s="120"/>
+      <c r="P24" s="120"/>
+      <c r="Q24" s="121"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="41">
@@ -3890,25 +4024,25 @@
       </c>
     </row>
     <row r="27" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="113" t="s">
+      <c r="A27" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="114"/>
-      <c r="C27" s="114"/>
-      <c r="D27" s="114"/>
-      <c r="E27" s="114"/>
-      <c r="F27" s="114"/>
-      <c r="G27" s="114"/>
-      <c r="H27" s="114"/>
-      <c r="I27" s="114"/>
-      <c r="J27" s="114"/>
-      <c r="K27" s="114"/>
-      <c r="L27" s="114"/>
-      <c r="M27" s="114"/>
-      <c r="N27" s="114"/>
-      <c r="O27" s="114"/>
-      <c r="P27" s="114"/>
-      <c r="Q27" s="115"/>
+      <c r="B27" s="120"/>
+      <c r="C27" s="120"/>
+      <c r="D27" s="120"/>
+      <c r="E27" s="120"/>
+      <c r="F27" s="120"/>
+      <c r="G27" s="120"/>
+      <c r="H27" s="120"/>
+      <c r="I27" s="120"/>
+      <c r="J27" s="120"/>
+      <c r="K27" s="120"/>
+      <c r="L27" s="120"/>
+      <c r="M27" s="120"/>
+      <c r="N27" s="120"/>
+      <c r="O27" s="120"/>
+      <c r="P27" s="120"/>
+      <c r="Q27" s="121"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="41">
@@ -4020,25 +4154,25 @@
       </c>
     </row>
     <row r="30" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="113" t="s">
+      <c r="A30" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="114"/>
-      <c r="C30" s="114"/>
-      <c r="D30" s="114"/>
-      <c r="E30" s="114"/>
-      <c r="F30" s="114"/>
-      <c r="G30" s="114"/>
-      <c r="H30" s="114"/>
-      <c r="I30" s="114"/>
-      <c r="J30" s="114"/>
-      <c r="K30" s="114"/>
-      <c r="L30" s="114"/>
-      <c r="M30" s="114"/>
-      <c r="N30" s="114"/>
-      <c r="O30" s="114"/>
-      <c r="P30" s="114"/>
-      <c r="Q30" s="115"/>
+      <c r="B30" s="120"/>
+      <c r="C30" s="120"/>
+      <c r="D30" s="120"/>
+      <c r="E30" s="120"/>
+      <c r="F30" s="120"/>
+      <c r="G30" s="120"/>
+      <c r="H30" s="120"/>
+      <c r="I30" s="120"/>
+      <c r="J30" s="120"/>
+      <c r="K30" s="120"/>
+      <c r="L30" s="120"/>
+      <c r="M30" s="120"/>
+      <c r="N30" s="120"/>
+      <c r="O30" s="120"/>
+      <c r="P30" s="120"/>
+      <c r="Q30" s="121"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="41">
@@ -4219,25 +4353,25 @@
       </c>
     </row>
     <row r="34" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="110" t="s">
+      <c r="A34" s="116" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="111"/>
-      <c r="C34" s="111"/>
-      <c r="D34" s="111"/>
-      <c r="E34" s="111"/>
-      <c r="F34" s="111"/>
-      <c r="G34" s="111"/>
-      <c r="H34" s="111"/>
-      <c r="I34" s="111"/>
-      <c r="J34" s="111"/>
-      <c r="K34" s="111"/>
-      <c r="L34" s="111"/>
-      <c r="M34" s="111"/>
-      <c r="N34" s="111"/>
-      <c r="O34" s="111"/>
-      <c r="P34" s="111"/>
-      <c r="Q34" s="112"/>
+      <c r="B34" s="117"/>
+      <c r="C34" s="117"/>
+      <c r="D34" s="117"/>
+      <c r="E34" s="117"/>
+      <c r="F34" s="117"/>
+      <c r="G34" s="117"/>
+      <c r="H34" s="117"/>
+      <c r="I34" s="117"/>
+      <c r="J34" s="117"/>
+      <c r="K34" s="117"/>
+      <c r="L34" s="117"/>
+      <c r="M34" s="117"/>
+      <c r="N34" s="117"/>
+      <c r="O34" s="117"/>
+      <c r="P34" s="117"/>
+      <c r="Q34" s="118"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
@@ -4329,15 +4463,14 @@
         <v>70</v>
       </c>
       <c r="C37" s="66">
-        <f>'Расчет освещения'!G2</f>
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D37" s="63">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E37" s="7">
         <f t="shared" si="12"/>
-        <v>3.1500000000000004</v>
+        <v>3.3600000000000003</v>
       </c>
       <c r="F37" s="7">
         <v>0.7</v>
@@ -4351,11 +4484,11 @@
       </c>
       <c r="I37" s="7">
         <f t="shared" si="14"/>
-        <v>2.2050000000000001</v>
+        <v>2.3519999999999999</v>
       </c>
       <c r="J37" s="7">
         <f t="shared" si="15"/>
-        <v>0.44774434669797925</v>
+        <v>0.4775939698111778</v>
       </c>
       <c r="K37" s="28"/>
       <c r="L37" s="28"/>
@@ -4414,12 +4547,12 @@
       <c r="B39" s="8"/>
       <c r="C39" s="106">
         <f>SUM(C35:C38)</f>
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D39" s="81"/>
       <c r="E39" s="105">
         <f>SUM(E35:E38)</f>
-        <v>3.4920000000000004</v>
+        <v>3.7020000000000004</v>
       </c>
       <c r="F39" s="105">
         <f>AVERAGE(F35:F38)</f>
@@ -4435,30 +4568,30 @@
       </c>
       <c r="I39" s="105">
         <f>SUM(I35:I38)</f>
-        <v>2.4443999999999999</v>
+        <v>2.5913999999999997</v>
       </c>
       <c r="J39" s="105">
         <f t="shared" si="15"/>
-        <v>0.49635659005375982</v>
+        <v>0.52620621316695837</v>
       </c>
       <c r="K39" s="105"/>
       <c r="L39" s="105"/>
       <c r="M39" s="105"/>
       <c r="N39" s="105">
         <f>I39</f>
-        <v>2.4443999999999999</v>
+        <v>2.5913999999999997</v>
       </c>
       <c r="O39" s="105">
         <f>J39</f>
-        <v>0.49635659005375982</v>
+        <v>0.52620621316695837</v>
       </c>
       <c r="P39" s="105">
         <f>SQRT(N39*N39+O39*O39)</f>
-        <v>2.4942857142857142</v>
+        <v>2.6442857142857141</v>
       </c>
       <c r="Q39" s="107">
         <f>P39*1000/(220*SQRT(3))</f>
-        <v>6.5458024026304322</v>
+        <v>6.9394503134415411</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -4468,55 +4601,49 @@
       <c r="B40" s="8"/>
       <c r="C40" s="108">
         <f>C39+C33</f>
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D40" s="10"/>
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
       <c r="G40" s="109">
         <f>(G39*E39+G33*E33)/(E33+E39)</f>
-        <v>0.95067656062308648</v>
+        <v>0.95071627583004381</v>
       </c>
       <c r="H40" s="109">
         <f>(H39*E39+H33*E33)/(E33+E39)</f>
-        <v>0.32585099754430247</v>
+        <v>0.32568468952666219</v>
       </c>
       <c r="I40" s="109">
         <f>I39+I33</f>
-        <v>93.784124999999989</v>
+        <v>93.93112499999998</v>
       </c>
       <c r="J40" s="100">
         <f t="shared" si="15"/>
-        <v>30.559650685069553</v>
+        <v>30.591929282515089</v>
       </c>
       <c r="K40" s="100"/>
       <c r="L40" s="100"/>
       <c r="M40" s="100"/>
       <c r="N40" s="100">
         <f>N39+N33</f>
-        <v>108.39848099999998</v>
+        <v>108.54548099999997</v>
       </c>
       <c r="O40" s="100">
         <f>O39+O33</f>
-        <v>35.321778893587535</v>
+        <v>35.351628516700735</v>
       </c>
       <c r="P40" s="100">
         <f>SQRT(O40*O40+N40*N40)</f>
-        <v>114.00815210902614</v>
+        <v>114.15716834392907</v>
       </c>
       <c r="Q40" s="101">
         <f>P40*1000/(380*SQRT(3))</f>
-        <v>173.21746660515277</v>
+        <v>173.44387335077076</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:F2"/>
     <mergeCell ref="A34:Q34"/>
     <mergeCell ref="A24:Q24"/>
     <mergeCell ref="A27:Q27"/>
@@ -4533,6 +4660,12 @@
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4546,7 +4679,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4593,8 +4728,8 @@
       <c r="F2" s="56">
         <v>2.13</v>
       </c>
-      <c r="G2" s="51">
-        <v>45</v>
+      <c r="G2" s="51" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -4675,8 +4810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q34" sqref="Q34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -4740,22 +4875,22 @@
       <c r="O1" s="78"/>
     </row>
     <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="110" t="s">
+      <c r="A2" s="116" t="s">
         <v>136</v>
       </c>
-      <c r="B2" s="111"/>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
-      <c r="M2" s="111"/>
-      <c r="N2" s="112"/>
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="117"/>
+      <c r="M2" s="117"/>
+      <c r="N2" s="118"/>
       <c r="O2" s="78"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -5277,22 +5412,22 @@
       <c r="O12" s="78"/>
     </row>
     <row r="13" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="110" t="s">
+      <c r="A13" s="116" t="s">
         <v>137</v>
       </c>
-      <c r="B13" s="111"/>
-      <c r="C13" s="111"/>
-      <c r="D13" s="111"/>
-      <c r="E13" s="111"/>
-      <c r="F13" s="111"/>
-      <c r="G13" s="111"/>
-      <c r="H13" s="111"/>
-      <c r="I13" s="111"/>
-      <c r="J13" s="111"/>
-      <c r="K13" s="111"/>
-      <c r="L13" s="111"/>
-      <c r="M13" s="111"/>
-      <c r="N13" s="112"/>
+      <c r="B13" s="117"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117"/>
+      <c r="G13" s="117"/>
+      <c r="H13" s="117"/>
+      <c r="I13" s="117"/>
+      <c r="J13" s="117"/>
+      <c r="K13" s="117"/>
+      <c r="L13" s="117"/>
+      <c r="M13" s="117"/>
+      <c r="N13" s="118"/>
       <c r="O13" s="78"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -5763,22 +5898,22 @@
       <c r="O22" s="78"/>
     </row>
     <row r="23" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="110" t="s">
+      <c r="A23" s="116" t="s">
         <v>91</v>
       </c>
-      <c r="B23" s="111"/>
-      <c r="C23" s="111"/>
-      <c r="D23" s="111"/>
-      <c r="E23" s="111"/>
-      <c r="F23" s="111"/>
-      <c r="G23" s="111"/>
-      <c r="H23" s="111"/>
-      <c r="I23" s="111"/>
-      <c r="J23" s="111"/>
-      <c r="K23" s="111"/>
-      <c r="L23" s="111"/>
-      <c r="M23" s="111"/>
-      <c r="N23" s="112"/>
+      <c r="B23" s="117"/>
+      <c r="C23" s="117"/>
+      <c r="D23" s="117"/>
+      <c r="E23" s="117"/>
+      <c r="F23" s="117"/>
+      <c r="G23" s="117"/>
+      <c r="H23" s="117"/>
+      <c r="I23" s="117"/>
+      <c r="J23" s="117"/>
+      <c r="K23" s="117"/>
+      <c r="L23" s="117"/>
+      <c r="M23" s="117"/>
+      <c r="N23" s="118"/>
       <c r="O23" s="78"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -5940,22 +6075,22 @@
       <c r="O26" s="78"/>
     </row>
     <row r="27" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="110" t="s">
+      <c r="A27" s="116" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="111"/>
-      <c r="C27" s="111"/>
-      <c r="D27" s="111"/>
-      <c r="E27" s="111"/>
-      <c r="F27" s="111"/>
-      <c r="G27" s="111"/>
-      <c r="H27" s="111"/>
-      <c r="I27" s="111"/>
-      <c r="J27" s="111"/>
-      <c r="K27" s="111"/>
-      <c r="L27" s="111"/>
-      <c r="M27" s="111"/>
-      <c r="N27" s="112"/>
+      <c r="B27" s="117"/>
+      <c r="C27" s="117"/>
+      <c r="D27" s="117"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="117"/>
+      <c r="G27" s="117"/>
+      <c r="H27" s="117"/>
+      <c r="I27" s="117"/>
+      <c r="J27" s="117"/>
+      <c r="K27" s="117"/>
+      <c r="L27" s="117"/>
+      <c r="M27" s="117"/>
+      <c r="N27" s="118"/>
       <c r="O27" s="78"/>
     </row>
     <row r="28" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -6044,7 +6179,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="P25" sqref="P25:P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -6633,4 +6768,235 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="A1:C22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="37.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="137" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="137" t="s">
+        <v>153</v>
+      </c>
+      <c r="C1" s="138" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="134">
+        <v>1</v>
+      </c>
+      <c r="B2" s="139">
+        <v>4</v>
+      </c>
+      <c r="C2" s="139" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="135"/>
+      <c r="B3" s="140">
+        <v>6</v>
+      </c>
+      <c r="C3" s="140" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="135"/>
+      <c r="B4" s="140">
+        <v>10</v>
+      </c>
+      <c r="C4" s="140" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="135"/>
+      <c r="B5" s="140">
+        <v>20</v>
+      </c>
+      <c r="C5" s="140" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="135"/>
+      <c r="B6" s="140">
+        <v>40</v>
+      </c>
+      <c r="C6" s="140" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="135"/>
+      <c r="B7" s="140">
+        <v>50</v>
+      </c>
+      <c r="C7" s="140" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="136"/>
+      <c r="B8" s="141">
+        <v>100</v>
+      </c>
+      <c r="C8" s="141" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="134">
+        <v>2</v>
+      </c>
+      <c r="B9" s="139">
+        <v>4</v>
+      </c>
+      <c r="C9" s="139" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="135"/>
+      <c r="B10" s="140">
+        <v>6</v>
+      </c>
+      <c r="C10" s="140" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="135"/>
+      <c r="B11" s="140">
+        <v>10</v>
+      </c>
+      <c r="C11" s="140" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="135"/>
+      <c r="B12" s="140">
+        <v>20</v>
+      </c>
+      <c r="C12" s="140" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="135"/>
+      <c r="B13" s="140">
+        <v>40</v>
+      </c>
+      <c r="C13" s="140" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="135"/>
+      <c r="B14" s="140">
+        <v>50</v>
+      </c>
+      <c r="C14" s="140" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="136"/>
+      <c r="B15" s="141">
+        <v>100</v>
+      </c>
+      <c r="C15" s="141" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="134">
+        <v>3</v>
+      </c>
+      <c r="B16" s="139">
+        <v>4</v>
+      </c>
+      <c r="C16" s="139" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="135"/>
+      <c r="B17" s="140">
+        <v>6</v>
+      </c>
+      <c r="C17" s="140" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="135"/>
+      <c r="B18" s="140">
+        <v>10</v>
+      </c>
+      <c r="C18" s="140" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="135"/>
+      <c r="B19" s="140">
+        <v>20</v>
+      </c>
+      <c r="C19" s="140" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="135"/>
+      <c r="B20" s="140">
+        <v>40</v>
+      </c>
+      <c r="C20" s="140" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="135"/>
+      <c r="B21" s="140">
+        <v>50</v>
+      </c>
+      <c r="C21" s="140" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="136"/>
+      <c r="B22" s="141">
+        <v>100</v>
+      </c>
+      <c r="C22" s="141" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="A9:A15"/>
+    <mergeCell ref="A16:A22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
i've back from college
</commit_message>
<xml_diff>
--- a/курсач медведь.xlsx
+++ b/курсач медведь.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megas\OneDrive\Рабочий стол\Projects\Java-English-Study\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="720" yWindow="135" windowWidth="27480" windowHeight="12600" activeTab="3"/>
   </bookViews>
@@ -14,7 +19,7 @@
     <sheet name="КЗ" sheetId="5" r:id="rId5"/>
     <sheet name="Чтение по жипегу" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="183">
   <si>
     <t>Наименование потребителя</t>
   </si>
@@ -446,24 +451,6 @@
     <t>ВВГнг-LS 4*95 мм2</t>
   </si>
   <si>
-    <t>ВА88-32 3Р 25А 25кА TDM</t>
-  </si>
-  <si>
-    <t>ВА88-32 3Р 16А 25кА TDM</t>
-  </si>
-  <si>
-    <t>ВА88-32 3Р 32А 25кА TDM</t>
-  </si>
-  <si>
-    <t>ВА88-32 3Р 100А 35кА TDM</t>
-  </si>
-  <si>
-    <t>ВА88-32 3Р 160А 35кА TDM</t>
-  </si>
-  <si>
-    <t>ВА88-32 3Р 250А 35кА TDM</t>
-  </si>
-  <si>
     <t>Итого ШР 1</t>
   </si>
   <si>
@@ -552,16 +539,56 @@
   </si>
   <si>
     <t>ГРЩ - ШР 1</t>
+  </si>
+  <si>
+    <t>BA47-29 3P 16A 4,5кА C TDM</t>
+  </si>
+  <si>
+    <t>BA47-29 3P 10A 4,5кА C TDM</t>
+  </si>
+  <si>
+    <t>BA47-29 3P 25A 4,5кА B TDM</t>
+  </si>
+  <si>
+    <t>BA47-29 3P 6A 4,5кА B TDM</t>
+  </si>
+  <si>
+    <t>BA47-29 3P 25A 4,5кА C TDM</t>
+  </si>
+  <si>
+    <t>BA47-29 3P 8A 4,5кА B TDM</t>
+  </si>
+  <si>
+    <t>BA47-29 3P 12,5A 4,5кА C TDM</t>
+  </si>
+  <si>
+    <t>BA47-29 3P 12,5A 4,5кА B TDM</t>
+  </si>
+  <si>
+    <t>ВА88-32 3P 100А 35кА TDM</t>
+  </si>
+  <si>
+    <t>ВА88-32 3P 80А 35кА TDM</t>
+  </si>
+  <si>
+    <t>ВА88-32 3P 200А 35кА TDM</t>
+  </si>
+  <si>
+    <t>по току</t>
+  </si>
+  <si>
+    <t>по току кз</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -569,16 +596,40 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF9C0006"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF9C6500"/>
+      <name val="Times New Roman"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="56">
+  <borders count="57">
     <border>
       <left/>
       <right/>
@@ -1303,11 +1354,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1619,16 +1681,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1648,10 +1701,16 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1661,6 +1720,24 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1688,24 +1765,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="55" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Нейтральный" xfId="2" builtinId="28"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Плохой" xfId="1" builtinId="27"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1975,7 +2048,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1986,7 +2059,7 @@
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2836,99 +2909,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="112" t="s">
+      <c r="A1" s="126" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="135" t="s">
+      <c r="B1" s="128" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="136" t="s">
+      <c r="C1" s="124" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="136" t="s">
+      <c r="D1" s="124" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136" t="s">
+      <c r="E1" s="124"/>
+      <c r="F1" s="124" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="136" t="s">
+      <c r="G1" s="124" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="136" t="s">
+      <c r="H1" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="136" t="s">
+      <c r="I1" s="124" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="136" t="s">
+      <c r="J1" s="124" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="136" t="s">
+      <c r="K1" s="124" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="137" t="s">
+      <c r="L1" s="118" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="136" t="s">
+      <c r="M1" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="137" t="s">
+      <c r="N1" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="137" t="s">
+      <c r="O1" s="118" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="138" t="s">
+      <c r="P1" s="120" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="123" t="s">
+      <c r="Q1" s="122" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="113"/>
-      <c r="B2" s="114"/>
-      <c r="C2" s="111"/>
+      <c r="A2" s="127"/>
+      <c r="B2" s="129"/>
+      <c r="C2" s="125"/>
       <c r="D2" s="107" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="121"/>
-      <c r="M2" s="111"/>
-      <c r="N2" s="121"/>
-      <c r="O2" s="121"/>
-      <c r="P2" s="122"/>
-      <c r="Q2" s="124"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="125"/>
+      <c r="L2" s="119"/>
+      <c r="M2" s="125"/>
+      <c r="N2" s="119"/>
+      <c r="O2" s="119"/>
+      <c r="P2" s="121"/>
+      <c r="Q2" s="123"/>
     </row>
     <row r="3" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="118" t="s">
+      <c r="A3" s="115" t="s">
         <v>134</v>
       </c>
-      <c r="B3" s="119"/>
-      <c r="C3" s="119"/>
-      <c r="D3" s="119"/>
-      <c r="E3" s="119"/>
-      <c r="F3" s="119"/>
-      <c r="G3" s="119"/>
-      <c r="H3" s="119"/>
-      <c r="I3" s="119"/>
-      <c r="J3" s="119"/>
-      <c r="K3" s="119"/>
-      <c r="L3" s="119"/>
-      <c r="M3" s="119"/>
-      <c r="N3" s="119"/>
-      <c r="O3" s="119"/>
-      <c r="P3" s="119"/>
-      <c r="Q3" s="120"/>
+      <c r="B3" s="116"/>
+      <c r="C3" s="116"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="116"/>
+      <c r="F3" s="116"/>
+      <c r="G3" s="116"/>
+      <c r="H3" s="116"/>
+      <c r="I3" s="116"/>
+      <c r="J3" s="116"/>
+      <c r="K3" s="116"/>
+      <c r="L3" s="116"/>
+      <c r="M3" s="116"/>
+      <c r="N3" s="116"/>
+      <c r="O3" s="116"/>
+      <c r="P3" s="116"/>
+      <c r="Q3" s="117"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="49">
@@ -3374,7 +3447,7 @@
     <row r="13" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="52"/>
       <c r="B13" s="31" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C13" s="60">
         <f>SUM(C4:C12)</f>
@@ -3439,25 +3512,25 @@
       </c>
     </row>
     <row r="14" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="118" t="s">
+      <c r="A14" s="115" t="s">
         <v>135</v>
       </c>
-      <c r="B14" s="119"/>
-      <c r="C14" s="119"/>
-      <c r="D14" s="119"/>
-      <c r="E14" s="119"/>
-      <c r="F14" s="119"/>
-      <c r="G14" s="119"/>
-      <c r="H14" s="119"/>
-      <c r="I14" s="119"/>
-      <c r="J14" s="119"/>
-      <c r="K14" s="119"/>
-      <c r="L14" s="119"/>
-      <c r="M14" s="119"/>
-      <c r="N14" s="119"/>
-      <c r="O14" s="119"/>
-      <c r="P14" s="119"/>
-      <c r="Q14" s="120"/>
+      <c r="B14" s="116"/>
+      <c r="C14" s="116"/>
+      <c r="D14" s="116"/>
+      <c r="E14" s="116"/>
+      <c r="F14" s="116"/>
+      <c r="G14" s="116"/>
+      <c r="H14" s="116"/>
+      <c r="I14" s="116"/>
+      <c r="J14" s="116"/>
+      <c r="K14" s="116"/>
+      <c r="L14" s="116"/>
+      <c r="M14" s="116"/>
+      <c r="N14" s="116"/>
+      <c r="O14" s="116"/>
+      <c r="P14" s="116"/>
+      <c r="Q14" s="117"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="32">
@@ -3841,12 +3914,12 @@
       <c r="N22" s="77"/>
       <c r="O22" s="77"/>
       <c r="P22" s="77"/>
-      <c r="Q22" s="134"/>
+      <c r="Q22" s="111"/>
     </row>
     <row r="23" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="31"/>
       <c r="B23" s="31" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C23" s="60">
         <f>SUM(C15:C22)</f>
@@ -3911,25 +3984,25 @@
       </c>
     </row>
     <row r="24" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="118" t="s">
+      <c r="A24" s="115" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="119"/>
-      <c r="C24" s="119"/>
-      <c r="D24" s="119"/>
-      <c r="E24" s="119"/>
-      <c r="F24" s="119"/>
-      <c r="G24" s="119"/>
-      <c r="H24" s="119"/>
-      <c r="I24" s="119"/>
-      <c r="J24" s="119"/>
-      <c r="K24" s="119"/>
-      <c r="L24" s="119"/>
-      <c r="M24" s="119"/>
-      <c r="N24" s="119"/>
-      <c r="O24" s="119"/>
-      <c r="P24" s="119"/>
-      <c r="Q24" s="120"/>
+      <c r="B24" s="116"/>
+      <c r="C24" s="116"/>
+      <c r="D24" s="116"/>
+      <c r="E24" s="116"/>
+      <c r="F24" s="116"/>
+      <c r="G24" s="116"/>
+      <c r="H24" s="116"/>
+      <c r="I24" s="116"/>
+      <c r="J24" s="116"/>
+      <c r="K24" s="116"/>
+      <c r="L24" s="116"/>
+      <c r="M24" s="116"/>
+      <c r="N24" s="116"/>
+      <c r="O24" s="116"/>
+      <c r="P24" s="116"/>
+      <c r="Q24" s="117"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="32">
@@ -4041,25 +4114,25 @@
       </c>
     </row>
     <row r="27" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="118" t="s">
+      <c r="A27" s="115" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="119"/>
-      <c r="C27" s="119"/>
-      <c r="D27" s="119"/>
-      <c r="E27" s="119"/>
-      <c r="F27" s="119"/>
-      <c r="G27" s="119"/>
-      <c r="H27" s="119"/>
-      <c r="I27" s="119"/>
-      <c r="J27" s="119"/>
-      <c r="K27" s="119"/>
-      <c r="L27" s="119"/>
-      <c r="M27" s="119"/>
-      <c r="N27" s="119"/>
-      <c r="O27" s="119"/>
-      <c r="P27" s="119"/>
-      <c r="Q27" s="120"/>
+      <c r="B27" s="116"/>
+      <c r="C27" s="116"/>
+      <c r="D27" s="116"/>
+      <c r="E27" s="116"/>
+      <c r="F27" s="116"/>
+      <c r="G27" s="116"/>
+      <c r="H27" s="116"/>
+      <c r="I27" s="116"/>
+      <c r="J27" s="116"/>
+      <c r="K27" s="116"/>
+      <c r="L27" s="116"/>
+      <c r="M27" s="116"/>
+      <c r="N27" s="116"/>
+      <c r="O27" s="116"/>
+      <c r="P27" s="116"/>
+      <c r="Q27" s="117"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="32">
@@ -4171,25 +4244,25 @@
       </c>
     </row>
     <row r="30" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="118" t="s">
+      <c r="A30" s="115" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="119"/>
-      <c r="C30" s="119"/>
-      <c r="D30" s="119"/>
-      <c r="E30" s="119"/>
-      <c r="F30" s="119"/>
-      <c r="G30" s="119"/>
-      <c r="H30" s="119"/>
-      <c r="I30" s="119"/>
-      <c r="J30" s="119"/>
-      <c r="K30" s="119"/>
-      <c r="L30" s="119"/>
-      <c r="M30" s="119"/>
-      <c r="N30" s="119"/>
-      <c r="O30" s="119"/>
-      <c r="P30" s="119"/>
-      <c r="Q30" s="120"/>
+      <c r="B30" s="116"/>
+      <c r="C30" s="116"/>
+      <c r="D30" s="116"/>
+      <c r="E30" s="116"/>
+      <c r="F30" s="116"/>
+      <c r="G30" s="116"/>
+      <c r="H30" s="116"/>
+      <c r="I30" s="116"/>
+      <c r="J30" s="116"/>
+      <c r="K30" s="116"/>
+      <c r="L30" s="116"/>
+      <c r="M30" s="116"/>
+      <c r="N30" s="116"/>
+      <c r="O30" s="116"/>
+      <c r="P30" s="116"/>
+      <c r="Q30" s="117"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="32">
@@ -4370,25 +4443,25 @@
       </c>
     </row>
     <row r="34" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="115" t="s">
+      <c r="A34" s="112" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="116"/>
-      <c r="C34" s="116"/>
-      <c r="D34" s="116"/>
-      <c r="E34" s="116"/>
-      <c r="F34" s="116"/>
-      <c r="G34" s="116"/>
-      <c r="H34" s="116"/>
-      <c r="I34" s="116"/>
-      <c r="J34" s="116"/>
-      <c r="K34" s="116"/>
-      <c r="L34" s="116"/>
-      <c r="M34" s="116"/>
-      <c r="N34" s="116"/>
-      <c r="O34" s="116"/>
-      <c r="P34" s="116"/>
-      <c r="Q34" s="117"/>
+      <c r="B34" s="113"/>
+      <c r="C34" s="113"/>
+      <c r="D34" s="113"/>
+      <c r="E34" s="113"/>
+      <c r="F34" s="113"/>
+      <c r="G34" s="113"/>
+      <c r="H34" s="113"/>
+      <c r="I34" s="113"/>
+      <c r="J34" s="113"/>
+      <c r="K34" s="113"/>
+      <c r="L34" s="113"/>
+      <c r="M34" s="113"/>
+      <c r="N34" s="113"/>
+      <c r="O34" s="113"/>
+      <c r="P34" s="113"/>
+      <c r="Q34" s="114"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
@@ -4664,6 +4737,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="A34:Q34"/>
     <mergeCell ref="A24:Q24"/>
     <mergeCell ref="A27:Q27"/>
@@ -4680,12 +4759,6 @@
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4749,7 +4822,7 @@
         <v>2.13</v>
       </c>
       <c r="G2" s="42" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -4828,10 +4901,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="Q29" sqref="Q29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -4846,10 +4919,11 @@
     <col min="10" max="10" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.21875" customWidth="1"/>
     <col min="12" max="12" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="78" t="s">
         <v>94</v>
       </c>
@@ -4894,26 +4968,32 @@
       </c>
       <c r="O1" s="69"/>
     </row>
-    <row r="2" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="115" t="s">
+    <row r="2" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="112" t="s">
         <v>134</v>
       </c>
-      <c r="B2" s="116"/>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="116"/>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="116"/>
-      <c r="M2" s="116"/>
-      <c r="N2" s="117"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
+      <c r="M2" s="113"/>
+      <c r="N2" s="114"/>
       <c r="O2" s="69"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="P2" t="s">
+        <v>182</v>
+      </c>
+      <c r="R2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="49">
         <v>2</v>
       </c>
@@ -4933,22 +5013,22 @@
         <v>13.415373698295689</v>
       </c>
       <c r="F3" s="61">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="G3" s="6">
         <f>D3*1.25</f>
         <v>99.776841881074176</v>
       </c>
       <c r="H3" s="61">
-        <f>'Ведомость электропотребителей'!I3*'Выбор защиты'!F3</f>
-        <v>175</v>
+        <f>F3*O3</f>
+        <v>112</v>
       </c>
       <c r="I3" s="61">
         <v>1</v>
       </c>
       <c r="J3" s="61">
         <f>F3</f>
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="K3" s="61">
         <v>104</v>
@@ -4957,15 +5037,21 @@
         <v>136</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="N3" s="91">
         <f>K3</f>
         <v>104</v>
       </c>
-      <c r="O3" s="69"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O3" s="142">
+        <f>_xlfn.CEILING.MATH(G3/F3)</f>
+        <v>7</v>
+      </c>
+      <c r="P3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="50">
         <v>3</v>
       </c>
@@ -4985,22 +5071,22 @@
         <v>9.4076954406000617</v>
       </c>
       <c r="F4" s="82">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="G4" s="6">
         <f t="shared" ref="G4:G11" si="1">D4*1.25</f>
         <v>69.969734839462959</v>
       </c>
-      <c r="H4" s="82">
-        <f>'Ведомость электропотребителей'!I3*F4</f>
-        <v>112</v>
+      <c r="H4" s="61">
+        <f t="shared" ref="H4:H12" si="2">F4*O4</f>
+        <v>70</v>
       </c>
       <c r="I4" s="61">
         <v>1</v>
       </c>
       <c r="J4" s="61">
-        <f t="shared" ref="J4:J12" si="2">F4</f>
-        <v>16</v>
+        <f t="shared" ref="J4:J12" si="3">F4</f>
+        <v>10</v>
       </c>
       <c r="K4" s="61">
         <v>104</v>
@@ -5008,16 +5094,22 @@
       <c r="L4" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="M4" s="63" t="s">
-        <v>141</v>
+      <c r="M4" s="6" t="s">
+        <v>171</v>
       </c>
       <c r="N4" s="91">
-        <f t="shared" ref="N4:N12" si="3">K4</f>
+        <f t="shared" ref="N4:N12" si="4">K4</f>
         <v>104</v>
       </c>
-      <c r="O4" s="69"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O4" s="142">
+        <f t="shared" ref="O4:O28" si="5">_xlfn.CEILING.MATH(G4/F4)</f>
+        <v>7</v>
+      </c>
+      <c r="P4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="50">
         <v>4</v>
       </c>
@@ -5037,22 +5129,22 @@
         <v>15.1087588776037</v>
       </c>
       <c r="F5" s="82">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G5" s="6">
         <f t="shared" si="1"/>
         <v>112.37139415217752</v>
       </c>
-      <c r="H5" s="82">
-        <f>'Ведомость электропотребителей'!I5*F5</f>
-        <v>224</v>
+      <c r="H5" s="61">
+        <f t="shared" si="2"/>
+        <v>128</v>
       </c>
       <c r="I5" s="61">
         <v>1</v>
       </c>
       <c r="J5" s="61">
-        <f t="shared" si="2"/>
-        <v>32</v>
+        <f t="shared" si="3"/>
+        <v>16</v>
       </c>
       <c r="K5" s="61">
         <v>104</v>
@@ -5060,16 +5152,22 @@
       <c r="L5" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="M5" s="63" t="s">
-        <v>142</v>
+      <c r="M5" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="N5" s="91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>104</v>
       </c>
-      <c r="O5" s="69"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O5" s="142">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="P5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="50">
         <v>5</v>
       </c>
@@ -5089,22 +5187,22 @@
         <v>20.885083878132136</v>
       </c>
       <c r="F6" s="82">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G6" s="6">
         <f t="shared" si="1"/>
         <v>110.95200810257697</v>
       </c>
-      <c r="H6" s="82">
-        <f>F6*7</f>
-        <v>224</v>
+      <c r="H6" s="61">
+        <f t="shared" si="2"/>
+        <v>125</v>
       </c>
       <c r="I6" s="61">
         <v>1</v>
       </c>
       <c r="J6" s="61">
-        <f t="shared" si="2"/>
-        <v>32</v>
+        <f t="shared" si="3"/>
+        <v>25</v>
       </c>
       <c r="K6" s="61">
         <v>104</v>
@@ -5112,16 +5210,22 @@
       <c r="L6" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="M6" s="63" t="s">
-        <v>142</v>
+      <c r="M6" s="6" t="s">
+        <v>172</v>
       </c>
       <c r="N6" s="91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>104</v>
       </c>
-      <c r="O6" s="69"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O6" s="141">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="P6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="50">
         <v>10</v>
       </c>
@@ -5141,22 +5245,22 @@
         <v>4.1393859938640274</v>
       </c>
       <c r="F7" s="82">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="G7" s="6">
         <f t="shared" si="1"/>
         <v>30.786683329363701</v>
       </c>
-      <c r="H7" s="82">
-        <f t="shared" ref="H7:H12" si="4">7*F7</f>
-        <v>112</v>
+      <c r="H7" s="61">
+        <f t="shared" si="2"/>
+        <v>36</v>
       </c>
       <c r="I7" s="61">
         <v>1</v>
       </c>
       <c r="J7" s="61">
-        <f t="shared" si="2"/>
-        <v>16</v>
+        <f t="shared" si="3"/>
+        <v>6</v>
       </c>
       <c r="K7" s="61">
         <v>104</v>
@@ -5164,16 +5268,22 @@
       <c r="L7" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="M7" s="63" t="s">
-        <v>141</v>
+      <c r="M7" s="6" t="s">
+        <v>173</v>
       </c>
       <c r="N7" s="91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>104</v>
       </c>
-      <c r="O7" s="69"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O7" s="141">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="P7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="50">
         <v>7</v>
       </c>
@@ -5199,15 +5309,15 @@
         <f t="shared" si="1"/>
         <v>123.56655172649158</v>
       </c>
-      <c r="H8" s="82">
-        <f t="shared" si="4"/>
-        <v>175</v>
+      <c r="H8" s="61">
+        <f t="shared" si="2"/>
+        <v>125</v>
       </c>
       <c r="I8" s="61">
         <v>1</v>
       </c>
       <c r="J8" s="61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="K8" s="61">
@@ -5216,16 +5326,22 @@
       <c r="L8" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="M8" s="63" t="s">
-        <v>140</v>
+      <c r="M8" s="6" t="s">
+        <v>172</v>
       </c>
       <c r="N8" s="91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>104</v>
       </c>
-      <c r="O8" s="69"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O8" s="141">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="P8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="50">
         <v>8</v>
       </c>
@@ -5251,15 +5367,15 @@
         <f t="shared" si="1"/>
         <v>139.93946967892592</v>
       </c>
-      <c r="H9" s="82">
-        <f t="shared" si="4"/>
-        <v>175</v>
+      <c r="H9" s="61">
+        <f t="shared" si="2"/>
+        <v>150</v>
       </c>
       <c r="I9" s="61">
         <v>1</v>
       </c>
       <c r="J9" s="61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="K9" s="61">
@@ -5268,16 +5384,22 @@
       <c r="L9" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="M9" s="63" t="s">
-        <v>140</v>
+      <c r="M9" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="N9" s="91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>104</v>
       </c>
-      <c r="O9" s="69"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O9" s="142">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="P9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="50">
         <v>9</v>
       </c>
@@ -5303,15 +5425,15 @@
         <f t="shared" si="1"/>
         <v>138.95989339117341</v>
       </c>
-      <c r="H10" s="82">
-        <f t="shared" si="4"/>
-        <v>175</v>
+      <c r="H10" s="61">
+        <f t="shared" si="2"/>
+        <v>150</v>
       </c>
       <c r="I10" s="61">
         <v>1</v>
       </c>
       <c r="J10" s="61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25</v>
       </c>
       <c r="K10" s="61">
@@ -5320,16 +5442,22 @@
       <c r="L10" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="M10" s="63" t="s">
-        <v>140</v>
+      <c r="M10" s="6" t="s">
+        <v>174</v>
       </c>
       <c r="N10" s="91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>104</v>
       </c>
-      <c r="O10" s="69"/>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O10" s="142">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="P10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="51">
         <v>20</v>
       </c>
@@ -5349,22 +5477,22 @@
         <v>11.289234528720074</v>
       </c>
       <c r="F11" s="62">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="G11" s="6">
         <f t="shared" si="1"/>
         <v>83.963681807355556</v>
       </c>
-      <c r="H11" s="62">
-        <f t="shared" si="4"/>
-        <v>175</v>
+      <c r="H11" s="61">
+        <f t="shared" si="2"/>
+        <v>96</v>
       </c>
       <c r="I11" s="61">
         <v>1</v>
       </c>
       <c r="J11" s="61">
-        <f t="shared" si="2"/>
-        <v>25</v>
+        <f t="shared" si="3"/>
+        <v>16</v>
       </c>
       <c r="K11" s="61">
         <v>104</v>
@@ -5372,16 +5500,22 @@
       <c r="L11" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="M11" s="64" t="s">
-        <v>140</v>
+      <c r="M11" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="N11" s="91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>104</v>
       </c>
-      <c r="O11" s="69"/>
-    </row>
-    <row r="12" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O11" s="142">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="P11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="51"/>
       <c r="B12" s="29" t="s">
         <v>96</v>
@@ -5405,15 +5539,15 @@
         <f>D12*1.25</f>
         <v>254.13007693692947</v>
       </c>
-      <c r="H12" s="62">
-        <f t="shared" si="4"/>
-        <v>700</v>
+      <c r="H12" s="61">
+        <f t="shared" si="2"/>
+        <v>300</v>
       </c>
       <c r="I12" s="61">
         <v>1</v>
       </c>
       <c r="J12" s="61">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100</v>
       </c>
       <c r="K12" s="61">
@@ -5422,35 +5556,41 @@
       <c r="L12" s="64" t="s">
         <v>137</v>
       </c>
-      <c r="M12" s="64" t="s">
-        <v>143</v>
+      <c r="M12" s="6" t="s">
+        <v>178</v>
       </c>
       <c r="N12" s="91">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>242</v>
       </c>
-      <c r="O12" s="69"/>
-    </row>
-    <row r="13" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="115" t="s">
+      <c r="O12" s="141">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="P12">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="112" t="s">
         <v>135</v>
       </c>
-      <c r="B13" s="116"/>
-      <c r="C13" s="116"/>
-      <c r="D13" s="116"/>
-      <c r="E13" s="116"/>
-      <c r="F13" s="116"/>
-      <c r="G13" s="116"/>
-      <c r="H13" s="116"/>
-      <c r="I13" s="116"/>
-      <c r="J13" s="116"/>
-      <c r="K13" s="116"/>
-      <c r="L13" s="116"/>
-      <c r="M13" s="116"/>
-      <c r="N13" s="117"/>
+      <c r="B13" s="113"/>
+      <c r="C13" s="113"/>
+      <c r="D13" s="113"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="113"/>
+      <c r="G13" s="113"/>
+      <c r="H13" s="113"/>
+      <c r="I13" s="113"/>
+      <c r="J13" s="113"/>
+      <c r="K13" s="113"/>
+      <c r="L13" s="113"/>
+      <c r="M13" s="113"/>
+      <c r="N13" s="114"/>
       <c r="O13" s="69"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="32">
         <v>6</v>
       </c>
@@ -5470,22 +5610,22 @@
         <v>20.885083878132136</v>
       </c>
       <c r="F14" s="61">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G14" s="6">
         <f>D14*1.25</f>
         <v>110.95200810257697</v>
       </c>
       <c r="H14" s="61">
-        <f>'Ведомость электропотребителей'!I7*F14</f>
-        <v>160</v>
+        <f>F14*O14</f>
+        <v>125</v>
       </c>
       <c r="I14" s="61">
         <v>1</v>
       </c>
       <c r="J14" s="61">
         <f>F14</f>
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="K14" s="61">
         <v>78</v>
@@ -5494,15 +5634,21 @@
         <v>138</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="N14" s="91">
         <f>K14</f>
         <v>78</v>
       </c>
-      <c r="O14" s="69"/>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O14" s="141">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="P14">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="33">
         <v>11</v>
       </c>
@@ -5518,26 +5664,26 @@
         <v>79.821473504859341</v>
       </c>
       <c r="E15" s="6">
-        <f t="shared" ref="E15:E22" si="5">C15/0.85</f>
+        <f t="shared" ref="E15:E22" si="6">C15/0.85</f>
         <v>13.415373698295689</v>
       </c>
       <c r="F15" s="82">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G15" s="6">
-        <f t="shared" ref="G15:G22" si="6">D15*1.25</f>
+        <f t="shared" ref="G15:G22" si="7">D15*1.25</f>
         <v>99.776841881074176</v>
       </c>
-      <c r="H15" s="82">
-        <f>'Ведомость электропотребителей'!I12*F15</f>
-        <v>224</v>
+      <c r="H15" s="61">
+        <f t="shared" ref="H15:H22" si="8">F15*O15</f>
+        <v>112</v>
       </c>
       <c r="I15" s="61">
         <v>1</v>
       </c>
       <c r="J15" s="61">
-        <f t="shared" ref="J15:J22" si="7">F15</f>
-        <v>32</v>
+        <f t="shared" ref="J15:J22" si="9">F15</f>
+        <v>16</v>
       </c>
       <c r="K15" s="61">
         <v>78</v>
@@ -5545,16 +5691,22 @@
       <c r="L15" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M15" s="63" t="s">
-        <v>142</v>
+      <c r="M15" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="N15" s="91">
-        <f t="shared" ref="N15:N22" si="8">K15</f>
+        <f t="shared" ref="N15:N22" si="10">K15</f>
         <v>78</v>
       </c>
-      <c r="O15" s="69"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O15" s="142">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="P15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="33">
         <v>13</v>
       </c>
@@ -5570,26 +5722,26 @@
         <v>81.724650292492726</v>
       </c>
       <c r="E16" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>13.73523534327609</v>
       </c>
       <c r="F16" s="82">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="G16" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>102.1558128656159</v>
       </c>
-      <c r="H16" s="82">
-        <f>'Ведомость электропотребителей'!I14*F16</f>
-        <v>175</v>
+      <c r="H16" s="61">
+        <f t="shared" si="8"/>
+        <v>112</v>
       </c>
       <c r="I16" s="61">
         <v>1</v>
       </c>
       <c r="J16" s="61">
-        <f t="shared" si="7"/>
-        <v>25</v>
+        <f t="shared" si="9"/>
+        <v>16</v>
       </c>
       <c r="K16" s="61">
         <v>78</v>
@@ -5597,16 +5749,22 @@
       <c r="L16" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M16" s="63" t="s">
-        <v>140</v>
+      <c r="M16" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="N16" s="91">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>78</v>
       </c>
-      <c r="O16" s="69"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O16" s="142">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="P16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="33">
         <v>15</v>
       </c>
@@ -5622,26 +5780,26 @@
         <v>46.236000781917127</v>
       </c>
       <c r="E17" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>7.7707564339356514</v>
       </c>
       <c r="F17" s="82">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="G17" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>57.795000977396413</v>
       </c>
-      <c r="H17" s="82">
-        <f>'Ведомость электропотребителей'!I14*F17</f>
-        <v>112</v>
+      <c r="H17" s="61">
+        <f t="shared" si="8"/>
+        <v>64</v>
       </c>
       <c r="I17" s="61">
         <v>1</v>
       </c>
       <c r="J17" s="61">
-        <f t="shared" si="7"/>
-        <v>16</v>
+        <f t="shared" si="9"/>
+        <v>8</v>
       </c>
       <c r="K17" s="61">
         <v>78</v>
@@ -5649,16 +5807,22 @@
       <c r="L17" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M17" s="63" t="s">
-        <v>141</v>
+      <c r="M17" s="6" t="s">
+        <v>175</v>
       </c>
       <c r="N17" s="91">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>78</v>
       </c>
-      <c r="O17" s="69"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O17" s="141">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="P17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="33">
         <v>16</v>
       </c>
@@ -5674,26 +5838,26 @@
         <v>74.223894717702308</v>
       </c>
       <c r="E18" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12.474604154235683</v>
       </c>
-      <c r="F18" s="82">
-        <v>16</v>
+      <c r="F18" s="139">
+        <v>12.5</v>
       </c>
       <c r="G18" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>92.779868397127885</v>
       </c>
-      <c r="H18" s="82">
-        <f>'Ведомость электропотребителей'!I17*F18</f>
-        <v>112</v>
+      <c r="H18" s="61">
+        <f t="shared" si="8"/>
+        <v>100</v>
       </c>
       <c r="I18" s="61">
         <v>1</v>
       </c>
       <c r="J18" s="61">
-        <f t="shared" si="7"/>
-        <v>16</v>
+        <f t="shared" si="9"/>
+        <v>12.5</v>
       </c>
       <c r="K18" s="61">
         <v>78</v>
@@ -5701,16 +5865,22 @@
       <c r="L18" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M18" s="63" t="s">
-        <v>141</v>
+      <c r="M18" s="6" t="s">
+        <v>176</v>
       </c>
       <c r="N18" s="91">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>78</v>
       </c>
-      <c r="O18" s="69"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O18" s="142">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="P18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="33">
         <v>17</v>
       </c>
@@ -5726,26 +5896,26 @@
         <v>69.745831687976676</v>
       </c>
       <c r="E19" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11.721988518987677</v>
       </c>
-      <c r="F19" s="82">
-        <v>16</v>
+      <c r="F19" s="139">
+        <v>12.5</v>
       </c>
       <c r="G19" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>87.182289609970837</v>
       </c>
-      <c r="H19" s="82">
-        <f>'Ведомость электропотребителей'!I18*F19</f>
-        <v>112</v>
+      <c r="H19" s="61">
+        <f t="shared" si="8"/>
+        <v>87.5</v>
       </c>
       <c r="I19" s="61">
         <v>1</v>
       </c>
       <c r="J19" s="61">
-        <f t="shared" si="7"/>
-        <v>16</v>
+        <f t="shared" si="9"/>
+        <v>12.5</v>
       </c>
       <c r="K19" s="61">
         <v>78</v>
@@ -5753,16 +5923,22 @@
       <c r="L19" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M19" s="63" t="s">
-        <v>141</v>
+      <c r="M19" s="6" t="s">
+        <v>176</v>
       </c>
       <c r="N19" s="91">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>78</v>
       </c>
-      <c r="O19" s="69"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O19" s="142">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="P19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="33">
         <v>18</v>
       </c>
@@ -5778,26 +5954,26 @@
         <v>78.366103020198508</v>
       </c>
       <c r="E20" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>13.170773616840085</v>
       </c>
       <c r="F20" s="82">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="G20" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>97.957628775248139</v>
       </c>
-      <c r="H20" s="82">
-        <f>'Ведомость электропотребителей'!I19*F20</f>
-        <v>175</v>
+      <c r="H20" s="61">
+        <f t="shared" si="8"/>
+        <v>112</v>
       </c>
       <c r="I20" s="61">
         <v>1</v>
       </c>
       <c r="J20" s="61">
-        <f t="shared" si="7"/>
-        <v>25</v>
+        <f t="shared" si="9"/>
+        <v>16</v>
       </c>
       <c r="K20" s="61">
         <v>78</v>
@@ -5805,16 +5981,22 @@
       <c r="L20" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M20" s="63" t="s">
-        <v>140</v>
+      <c r="M20" s="6" t="s">
+        <v>170</v>
       </c>
       <c r="N20" s="91">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>78</v>
       </c>
-      <c r="O20" s="69"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O20" s="142">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="P20">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="34">
         <v>19</v>
       </c>
@@ -5830,26 +6012,26 @@
         <v>37.05597157097958</v>
       </c>
       <c r="E21" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.2278943816772401</v>
       </c>
-      <c r="F21" s="62">
-        <v>16</v>
+      <c r="F21" s="140">
+        <v>12.5</v>
       </c>
       <c r="G21" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>46.319964463724475</v>
       </c>
-      <c r="H21" s="62">
-        <f>'Ведомость электропотребителей'!I20*F21</f>
-        <v>112</v>
+      <c r="H21" s="61">
+        <f t="shared" si="8"/>
+        <v>50</v>
       </c>
       <c r="I21" s="61">
         <v>1</v>
       </c>
       <c r="J21" s="61">
-        <f t="shared" si="7"/>
-        <v>16</v>
+        <f t="shared" si="9"/>
+        <v>12.5</v>
       </c>
       <c r="K21" s="61">
         <v>78</v>
@@ -5857,16 +6039,22 @@
       <c r="L21" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M21" s="64" t="s">
-        <v>141</v>
+      <c r="M21" s="6" t="s">
+        <v>177</v>
       </c>
       <c r="N21" s="91">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>78</v>
       </c>
-      <c r="O21" s="69"/>
-    </row>
-    <row r="22" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O21" s="141">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="P21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="80"/>
       <c r="B22" s="66" t="s">
         <v>97</v>
@@ -5880,63 +6068,69 @@
         <v>155.5007387072225</v>
       </c>
       <c r="E22" s="6">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>76.390214154504719</v>
       </c>
       <c r="F22" s="62">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="G22" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>194.37592338402811</v>
       </c>
-      <c r="H22" s="62">
-        <f>7*F22</f>
-        <v>700</v>
+      <c r="H22" s="61">
+        <f t="shared" si="8"/>
+        <v>240</v>
       </c>
       <c r="I22" s="61">
         <v>1</v>
       </c>
       <c r="J22" s="61">
-        <f t="shared" si="7"/>
-        <v>100</v>
+        <f t="shared" si="9"/>
+        <v>80</v>
       </c>
       <c r="K22" s="61">
         <f>158</f>
         <v>158</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="M22" s="64" t="s">
-        <v>143</v>
+        <v>142</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>179</v>
       </c>
       <c r="N22" s="91">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>158</v>
       </c>
-      <c r="O22" s="69"/>
-    </row>
-    <row r="23" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="115" t="s">
+      <c r="O22" s="141">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="P22">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="112" t="s">
         <v>91</v>
       </c>
-      <c r="B23" s="116"/>
-      <c r="C23" s="116"/>
-      <c r="D23" s="116"/>
-      <c r="E23" s="116"/>
-      <c r="F23" s="116"/>
-      <c r="G23" s="116"/>
-      <c r="H23" s="116"/>
-      <c r="I23" s="116"/>
-      <c r="J23" s="116"/>
-      <c r="K23" s="116"/>
-      <c r="L23" s="116"/>
-      <c r="M23" s="116"/>
-      <c r="N23" s="117"/>
+      <c r="B23" s="113"/>
+      <c r="C23" s="113"/>
+      <c r="D23" s="113"/>
+      <c r="E23" s="113"/>
+      <c r="F23" s="113"/>
+      <c r="G23" s="113"/>
+      <c r="H23" s="113"/>
+      <c r="I23" s="113"/>
+      <c r="J23" s="113"/>
+      <c r="K23" s="113"/>
+      <c r="L23" s="113"/>
+      <c r="M23" s="113"/>
+      <c r="N23" s="114"/>
       <c r="O23" s="69"/>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="79">
         <v>1</v>
       </c>
@@ -5956,23 +6150,23 @@
         <v>24.083700327936157</v>
       </c>
       <c r="F24" s="61">
-        <f>100</f>
-        <v>100</v>
+        <f>25</f>
+        <v>25</v>
       </c>
       <c r="G24" s="6">
         <f>D24*1.25</f>
         <v>63.972328996080421</v>
       </c>
       <c r="H24" s="61">
-        <f>F24*'Ведомость электропотребителей'!I2</f>
-        <v>250</v>
+        <f>F24*O24</f>
+        <v>75</v>
       </c>
       <c r="I24" s="61">
         <v>1</v>
       </c>
       <c r="J24" s="61">
         <f>F24</f>
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="K24" s="61">
         <v>78</v>
@@ -5981,15 +6175,27 @@
         <v>138</v>
       </c>
       <c r="M24" s="6" t="s">
-        <v>143</v>
+        <v>172</v>
       </c>
       <c r="N24" s="91">
         <f>K24</f>
         <v>78</v>
       </c>
-      <c r="O24" s="69"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O24" s="141">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="P24">
+        <v>4</v>
+      </c>
+      <c r="Q24">
+        <v>16</v>
+      </c>
+      <c r="R24">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="79">
         <v>12</v>
       </c>
@@ -6009,40 +6215,52 @@
         <v>22.202161239816146</v>
       </c>
       <c r="F25" s="82">
-        <f>160</f>
-        <v>160</v>
+        <f>25</f>
+        <v>25</v>
       </c>
       <c r="G25" s="6">
-        <f t="shared" ref="G25:G26" si="9">D25*1.25</f>
+        <f t="shared" ref="G25:G26" si="11">D25*1.25</f>
         <v>82.564287110566283</v>
       </c>
-      <c r="H25" s="82">
-        <f>F25*'Ведомость электропотребителей'!I13</f>
-        <v>560</v>
+      <c r="H25" s="61">
+        <f t="shared" ref="H25:H26" si="12">F25*O25</f>
+        <v>100</v>
       </c>
       <c r="I25" s="61">
         <v>1</v>
       </c>
       <c r="J25" s="61">
-        <f t="shared" ref="J25:J26" si="10">F25</f>
-        <v>160</v>
+        <f t="shared" ref="J25:J26" si="13">F25</f>
+        <v>25</v>
       </c>
       <c r="K25" s="61">
         <v>127</v>
       </c>
       <c r="L25" s="63" t="s">
-        <v>149</v>
-      </c>
-      <c r="M25" s="63" t="s">
-        <v>144</v>
+        <v>143</v>
+      </c>
+      <c r="M25" s="6" t="s">
+        <v>172</v>
       </c>
       <c r="N25" s="91">
-        <f t="shared" ref="N25:N26" si="11">K25</f>
+        <f t="shared" ref="N25:N26" si="14">K25</f>
         <v>127</v>
       </c>
-      <c r="O25" s="69"/>
-    </row>
-    <row r="26" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O25" s="141">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="P25">
+        <v>4</v>
+      </c>
+      <c r="Q25">
+        <v>6</v>
+      </c>
+      <c r="R25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="79">
         <v>14</v>
       </c>
@@ -6062,22 +6280,22 @@
         <v>24.083700327936157</v>
       </c>
       <c r="F26" s="62">
-        <v>100</v>
+        <v>25</v>
       </c>
       <c r="G26" s="6">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>63.972328996080421</v>
       </c>
-      <c r="H26" s="62">
-        <f>F26*'Ведомость электропотребителей'!I15</f>
-        <v>250</v>
+      <c r="H26" s="61">
+        <f t="shared" si="12"/>
+        <v>75</v>
       </c>
       <c r="I26" s="61">
         <v>1</v>
       </c>
       <c r="J26" s="61">
-        <f t="shared" si="10"/>
-        <v>100</v>
+        <f t="shared" si="13"/>
+        <v>25</v>
       </c>
       <c r="K26" s="61">
         <v>78</v>
@@ -6085,35 +6303,47 @@
       <c r="L26" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="M26" s="64" t="s">
-        <v>143</v>
+      <c r="M26" s="6" t="s">
+        <v>172</v>
       </c>
       <c r="N26" s="91">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>78</v>
       </c>
-      <c r="O26" s="69"/>
-    </row>
-    <row r="27" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="115" t="s">
+      <c r="O26" s="141">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="P26">
+        <v>4</v>
+      </c>
+      <c r="Q26">
+        <v>16</v>
+      </c>
+      <c r="R26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="112" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="116"/>
-      <c r="C27" s="116"/>
-      <c r="D27" s="116"/>
-      <c r="E27" s="116"/>
-      <c r="F27" s="116"/>
-      <c r="G27" s="116"/>
-      <c r="H27" s="116"/>
-      <c r="I27" s="116"/>
-      <c r="J27" s="116"/>
-      <c r="K27" s="116"/>
-      <c r="L27" s="116"/>
-      <c r="M27" s="116"/>
-      <c r="N27" s="117"/>
+      <c r="B27" s="113"/>
+      <c r="C27" s="113"/>
+      <c r="D27" s="113"/>
+      <c r="E27" s="113"/>
+      <c r="F27" s="113"/>
+      <c r="G27" s="113"/>
+      <c r="H27" s="113"/>
+      <c r="I27" s="113"/>
+      <c r="J27" s="113"/>
+      <c r="K27" s="113"/>
+      <c r="L27" s="113"/>
+      <c r="M27" s="113"/>
+      <c r="N27" s="114"/>
       <c r="O27" s="69"/>
     </row>
-    <row r="28" spans="1:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="7"/>
       <c r="B28" s="76"/>
       <c r="C28" s="77">
@@ -6136,8 +6366,8 @@
         <v>410.06233899025972</v>
       </c>
       <c r="H28" s="83">
-        <f>7*F28</f>
-        <v>1750</v>
+        <f>F28*O28</f>
+        <v>750</v>
       </c>
       <c r="I28" s="83">
         <v>1</v>
@@ -6153,15 +6383,21 @@
         <v>139</v>
       </c>
       <c r="M28" s="77" t="s">
-        <v>145</v>
+        <v>180</v>
       </c>
       <c r="N28" s="92">
         <f>K28</f>
         <v>242</v>
       </c>
-      <c r="O28" s="69"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O28" s="141">
+        <f>_xlfn.CEILING.MATH(G28/F28) + 1</f>
+        <v>3</v>
+      </c>
+      <c r="P28">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B29" s="69"/>
       <c r="C29" s="69"/>
       <c r="D29" s="69"/>
@@ -6176,7 +6412,7 @@
       <c r="M29" s="69"/>
       <c r="N29" s="69"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D30" s="81"/>
     </row>
   </sheetData>
@@ -6196,10 +6432,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L15"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -6210,59 +6446,59 @@
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="129"/>
-      <c r="B1" s="125" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="134"/>
+      <c r="B1" s="130" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="125" t="s">
+      <c r="C1" s="130" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="125" t="s">
+      <c r="D1" s="130" t="s">
         <v>125</v>
       </c>
-      <c r="E1" s="125" t="s">
+      <c r="E1" s="130" t="s">
         <v>107</v>
       </c>
-      <c r="F1" s="125"/>
-      <c r="G1" s="125" t="s">
+      <c r="F1" s="130"/>
+      <c r="G1" s="130" t="s">
         <v>123</v>
       </c>
-      <c r="H1" s="125" t="s">
+      <c r="H1" s="130" t="s">
         <v>129</v>
       </c>
-      <c r="I1" s="125" t="s">
+      <c r="I1" s="130" t="s">
         <v>130</v>
       </c>
-      <c r="J1" s="125" t="s">
+      <c r="J1" s="130" t="s">
         <v>131</v>
       </c>
-      <c r="K1" s="125" t="s">
+      <c r="K1" s="130" t="s">
         <v>128</v>
       </c>
-      <c r="L1" s="127" t="s">
+      <c r="L1" s="132" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="130"/>
-      <c r="B2" s="126"/>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="135"/>
+      <c r="B2" s="131"/>
+      <c r="C2" s="131"/>
+      <c r="D2" s="131"/>
       <c r="E2" s="85" t="s">
         <v>124</v>
       </c>
       <c r="F2" s="85" t="s">
         <v>122</v>
       </c>
-      <c r="G2" s="126"/>
-      <c r="H2" s="126"/>
-      <c r="I2" s="126"/>
-      <c r="J2" s="126"/>
-      <c r="K2" s="126"/>
-      <c r="L2" s="128"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
+      <c r="K2" s="131"/>
+      <c r="L2" s="133"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="86" t="s">
         <v>98</v>
       </c>
@@ -6284,7 +6520,7 @@
       </c>
       <c r="L3" s="87"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="86" t="s">
         <v>132</v>
       </c>
@@ -6325,8 +6561,11 @@
       <c r="L4" s="87" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="86" t="s">
         <v>111</v>
       </c>
@@ -6367,10 +6606,13 @@
       <c r="L5" s="87" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="86" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B6" s="84">
         <f t="shared" si="0"/>
@@ -6409,10 +6651,13 @@
       <c r="L6" s="87" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="86" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="B7" s="84">
         <f>SQRT(C7*C7+D7*D7)</f>
@@ -6451,8 +6696,11 @@
       <c r="L7" s="87" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M7">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="86" t="s">
         <v>101</v>
       </c>
@@ -6491,8 +6739,11 @@
       <c r="L8" s="87" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M8" s="143">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="86" t="s">
         <v>100</v>
       </c>
@@ -6531,8 +6782,11 @@
       <c r="L9" s="87" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M9" s="143">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="86" t="s">
         <v>102</v>
       </c>
@@ -6571,8 +6825,11 @@
       <c r="L10" s="87" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M10" s="143">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="86" t="s">
         <v>99</v>
       </c>
@@ -6611,8 +6868,11 @@
       <c r="L11" s="87" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M11" s="143">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="86" t="s">
         <v>103</v>
       </c>
@@ -6651,8 +6911,11 @@
       <c r="L12" s="87" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M12" s="143">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="86" t="s">
         <v>104</v>
       </c>
@@ -6691,8 +6954,11 @@
       <c r="L13" s="87" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M13" s="143">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="86" t="s">
         <v>105</v>
       </c>
@@ -6731,8 +6997,11 @@
       <c r="L14" s="87" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="M14" s="143">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="88" t="s">
         <v>106</v>
       </c>
@@ -6770,6 +7039,9 @@
       <c r="K15" s="89"/>
       <c r="L15" s="90" t="s">
         <v>120</v>
+      </c>
+      <c r="M15" s="143">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -6807,208 +7079,208 @@
   <sheetData>
     <row r="1" spans="1:3" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="99" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B1" s="99" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C1" s="100" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="131">
+      <c r="A2" s="136">
         <v>1</v>
       </c>
       <c r="B2" s="101">
         <v>4</v>
       </c>
       <c r="C2" s="101" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="132"/>
+      <c r="A3" s="137"/>
       <c r="B3" s="102">
         <v>6</v>
       </c>
       <c r="C3" s="102" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="132"/>
+      <c r="A4" s="137"/>
       <c r="B4" s="102">
         <v>10</v>
       </c>
       <c r="C4" s="102" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="132"/>
+      <c r="A5" s="137"/>
       <c r="B5" s="102">
         <v>20</v>
       </c>
       <c r="C5" s="102" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="132"/>
+      <c r="A6" s="137"/>
       <c r="B6" s="102">
         <v>40</v>
       </c>
       <c r="C6" s="102" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="132"/>
+      <c r="A7" s="137"/>
       <c r="B7" s="102">
         <v>50</v>
       </c>
       <c r="C7" s="102" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="133"/>
+      <c r="A8" s="138"/>
       <c r="B8" s="103">
         <v>100</v>
       </c>
       <c r="C8" s="103" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="131">
+      <c r="A9" s="136">
         <v>2</v>
       </c>
       <c r="B9" s="101">
         <v>4</v>
       </c>
       <c r="C9" s="101" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="132"/>
+      <c r="A10" s="137"/>
       <c r="B10" s="102">
         <v>6</v>
       </c>
       <c r="C10" s="102" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="132"/>
+      <c r="A11" s="137"/>
       <c r="B11" s="102">
         <v>10</v>
       </c>
       <c r="C11" s="102" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="132"/>
+      <c r="A12" s="137"/>
       <c r="B12" s="102">
         <v>20</v>
       </c>
       <c r="C12" s="102" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="132"/>
+      <c r="A13" s="137"/>
       <c r="B13" s="102">
         <v>40</v>
       </c>
       <c r="C13" s="102" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="132"/>
+      <c r="A14" s="137"/>
       <c r="B14" s="102">
         <v>50</v>
       </c>
       <c r="C14" s="102" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="133"/>
+      <c r="A15" s="138"/>
       <c r="B15" s="103">
         <v>100</v>
       </c>
       <c r="C15" s="103" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="131">
+      <c r="A16" s="136">
         <v>3</v>
       </c>
       <c r="B16" s="101">
         <v>4</v>
       </c>
       <c r="C16" s="101" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="132"/>
+      <c r="A17" s="137"/>
       <c r="B17" s="102">
         <v>6</v>
       </c>
       <c r="C17" s="102" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="132"/>
+      <c r="A18" s="137"/>
       <c r="B18" s="102">
         <v>10</v>
       </c>
       <c r="C18" s="102" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="132"/>
+      <c r="A19" s="137"/>
       <c r="B19" s="102">
         <v>20</v>
       </c>
       <c r="C19" s="102" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="132"/>
+      <c r="A20" s="137"/>
       <c r="B20" s="102">
         <v>40</v>
       </c>
       <c r="C20" s="102" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="132"/>
+      <c r="A21" s="137"/>
       <c r="B21" s="102">
         <v>50</v>
       </c>
       <c r="C21" s="102" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="133"/>
+      <c r="A22" s="138"/>
       <c r="B22" s="103">
         <v>100</v>
       </c>
       <c r="C22" s="103" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
course project has finished. finally.
</commit_message>
<xml_diff>
--- a/курсач медведь.xlsx
+++ b/курсач медведь.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="135" windowWidth="27480" windowHeight="12600" activeTab="1"/>
+    <workbookView xWindow="720" yWindow="135" windowWidth="27480" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Ведомость электропотребителей" sheetId="1" r:id="rId1"/>
@@ -583,7 +583,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -605,16 +605,8 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -631,13 +623,8 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="57">
+  <borders count="62">
     <border>
       <left/>
       <right/>
@@ -1371,14 +1358,72 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1699,24 +1744,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="56" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1753,6 +1780,24 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="54" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1780,21 +1825,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="22" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="17" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="18" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="19" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="57" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Акцент2" xfId="3" builtinId="33"/>
+  <cellStyles count="3">
     <cellStyle name="Нейтральный" xfId="2" builtinId="28"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Плохой" xfId="1" builtinId="27"/>
@@ -2067,7 +2120,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2077,8 +2130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2115,7 +2168,7 @@
       <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="J1" s="143" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="10" t="s">
@@ -2149,14 +2202,14 @@
       <c r="H2" s="6">
         <v>0.3</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="19">
         <v>2.5</v>
       </c>
-      <c r="J2" s="143">
+      <c r="J2" s="149">
         <f>E2*I2</f>
         <v>51.177863196864337</v>
       </c>
-      <c r="K2" s="20">
+      <c r="K2" s="145">
         <f>H2+0.05</f>
         <v>0.35</v>
       </c>
@@ -2188,14 +2241,14 @@
       <c r="H3" s="105">
         <v>0.75</v>
       </c>
-      <c r="I3" s="105">
+      <c r="I3" s="15">
         <v>7</v>
       </c>
-      <c r="J3" s="144">
+      <c r="J3" s="150">
         <f t="shared" ref="J3:J21" si="2">E3*I3</f>
         <v>79.821473504859341</v>
       </c>
-      <c r="K3" s="17">
+      <c r="K3" s="146">
         <f>H3+0.05</f>
         <v>0.8</v>
       </c>
@@ -2227,14 +2280,14 @@
       <c r="H4" s="105">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I4" s="105">
+      <c r="I4" s="15">
         <v>7</v>
       </c>
-      <c r="J4" s="144">
+      <c r="J4" s="150">
         <f t="shared" si="2"/>
         <v>55.975787871570368</v>
       </c>
-      <c r="K4" s="17">
+      <c r="K4" s="146">
         <f>H4+0.05</f>
         <v>0.60000000000000009</v>
       </c>
@@ -2266,14 +2319,14 @@
       <c r="H5" s="105">
         <v>0.5</v>
       </c>
-      <c r="I5" s="105">
+      <c r="I5" s="15">
         <v>7</v>
       </c>
-      <c r="J5" s="144">
+      <c r="J5" s="150">
         <f t="shared" si="2"/>
         <v>44.780630297256295</v>
       </c>
-      <c r="K5" s="17">
+      <c r="K5" s="146">
         <f>H5+0.05</f>
         <v>0.55000000000000004</v>
       </c>
@@ -2305,14 +2358,14 @@
       <c r="H6" s="105">
         <v>0.46</v>
       </c>
-      <c r="I6" s="105">
+      <c r="I6" s="15">
         <v>7</v>
       </c>
-      <c r="J6" s="144">
+      <c r="J6" s="150">
         <f t="shared" si="2"/>
         <v>89.897115321742007</v>
       </c>
-      <c r="K6" s="17">
+      <c r="K6" s="146">
         <f t="shared" ref="K6:K21" si="3">H6+0.05</f>
         <v>0.51</v>
       </c>
@@ -2344,14 +2397,14 @@
       <c r="H7" s="105">
         <v>0.77</v>
       </c>
-      <c r="I7" s="105">
+      <c r="I7" s="15">
         <v>5</v>
       </c>
-      <c r="J7" s="144">
+      <c r="J7" s="150">
         <f t="shared" si="2"/>
         <v>88.76160648206158</v>
       </c>
-      <c r="K7" s="17">
+      <c r="K7" s="146">
         <f t="shared" si="3"/>
         <v>0.82000000000000006</v>
       </c>
@@ -2383,14 +2436,14 @@
       <c r="H8" s="105">
         <v>0.66</v>
       </c>
-      <c r="I8" s="105">
+      <c r="I8" s="15">
         <v>7</v>
       </c>
-      <c r="J8" s="144">
+      <c r="J8" s="150">
         <f t="shared" si="2"/>
         <v>98.853241381193271</v>
       </c>
-      <c r="K8" s="17">
+      <c r="K8" s="146">
         <f t="shared" si="3"/>
         <v>0.71000000000000008</v>
       </c>
@@ -2422,14 +2475,14 @@
       <c r="H9" s="105">
         <v>0.95</v>
       </c>
-      <c r="I9" s="105">
+      <c r="I9" s="15">
         <v>7</v>
       </c>
-      <c r="J9" s="144">
+      <c r="J9" s="150">
         <f>E9*I9</f>
         <v>111.95157574314074</v>
       </c>
-      <c r="K9" s="17">
+      <c r="K9" s="146">
         <f>0.98</f>
         <v>0.98</v>
       </c>
@@ -2461,14 +2514,14 @@
       <c r="H10" s="105">
         <v>0.78</v>
       </c>
-      <c r="I10" s="105">
+      <c r="I10" s="15">
         <v>7</v>
       </c>
-      <c r="J10" s="144">
+      <c r="J10" s="150">
         <f t="shared" si="2"/>
         <v>111.16791471293874</v>
       </c>
-      <c r="K10" s="17">
+      <c r="K10" s="146">
         <f t="shared" si="3"/>
         <v>0.83000000000000007</v>
       </c>
@@ -2500,14 +2553,14 @@
       <c r="H11" s="105">
         <v>0.4</v>
       </c>
-      <c r="I11" s="105">
+      <c r="I11" s="15">
         <v>7</v>
       </c>
-      <c r="J11" s="144">
+      <c r="J11" s="150">
         <f t="shared" si="2"/>
         <v>24.62934666349096</v>
       </c>
-      <c r="K11" s="17">
+      <c r="K11" s="146">
         <f t="shared" si="3"/>
         <v>0.45</v>
       </c>
@@ -2539,14 +2592,14 @@
       <c r="H12" s="105">
         <v>0.45</v>
       </c>
-      <c r="I12" s="105">
+      <c r="I12" s="15">
         <v>7</v>
       </c>
-      <c r="J12" s="144">
+      <c r="J12" s="150">
         <f t="shared" si="2"/>
         <v>79.821473504859341</v>
       </c>
-      <c r="K12" s="17">
+      <c r="K12" s="146">
         <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
@@ -2578,14 +2631,14 @@
       <c r="H13" s="105">
         <v>0.1</v>
       </c>
-      <c r="I13" s="105">
+      <c r="I13" s="15">
         <v>3.5</v>
       </c>
-      <c r="J13" s="144">
+      <c r="J13" s="150">
         <f>E13*I13</f>
         <v>66.051429688453027</v>
       </c>
-      <c r="K13" s="17">
+      <c r="K13" s="146">
         <f t="shared" si="3"/>
         <v>0.15000000000000002</v>
       </c>
@@ -2617,14 +2670,14 @@
       <c r="H14" s="105">
         <v>0.82</v>
       </c>
-      <c r="I14" s="105">
+      <c r="I14" s="15">
         <v>7</v>
       </c>
-      <c r="J14" s="144">
+      <c r="J14" s="150">
         <f t="shared" si="2"/>
         <v>81.724650292492726</v>
       </c>
-      <c r="K14" s="17">
+      <c r="K14" s="146">
         <f t="shared" si="3"/>
         <v>0.87</v>
       </c>
@@ -2656,14 +2709,14 @@
       <c r="H15" s="105">
         <v>0.3</v>
       </c>
-      <c r="I15" s="105">
+      <c r="I15" s="15">
         <v>2.5</v>
       </c>
-      <c r="J15" s="144">
+      <c r="J15" s="150">
         <f t="shared" si="2"/>
         <v>51.177863196864337</v>
       </c>
-      <c r="K15" s="17">
+      <c r="K15" s="146">
         <f t="shared" si="3"/>
         <v>0.35</v>
       </c>
@@ -2695,14 +2748,14 @@
       <c r="H16" s="105">
         <v>0.74</v>
       </c>
-      <c r="I16" s="105">
+      <c r="I16" s="15">
         <v>7</v>
       </c>
-      <c r="J16" s="144">
+      <c r="J16" s="150">
         <f t="shared" si="2"/>
         <v>46.236000781917127</v>
       </c>
-      <c r="K16" s="17">
+      <c r="K16" s="146">
         <f t="shared" si="3"/>
         <v>0.79</v>
       </c>
@@ -2734,14 +2787,14 @@
       <c r="H17" s="105">
         <v>0.81</v>
       </c>
-      <c r="I17" s="105">
+      <c r="I17" s="15">
         <v>7</v>
       </c>
-      <c r="J17" s="144">
+      <c r="J17" s="150">
         <f t="shared" si="2"/>
         <v>74.223894717702308</v>
       </c>
-      <c r="K17" s="17">
+      <c r="K17" s="146">
         <f t="shared" si="3"/>
         <v>0.8600000000000001</v>
       </c>
@@ -2773,14 +2826,14 @@
       <c r="H18" s="105">
         <v>0.76</v>
       </c>
-      <c r="I18" s="105">
+      <c r="I18" s="15">
         <v>7</v>
       </c>
-      <c r="J18" s="144">
+      <c r="J18" s="150">
         <f t="shared" si="2"/>
         <v>69.745831687976676</v>
       </c>
-      <c r="K18" s="17">
+      <c r="K18" s="146">
         <f t="shared" si="3"/>
         <v>0.81</v>
       </c>
@@ -2812,14 +2865,14 @@
       <c r="H19" s="105">
         <v>0.55000000000000004</v>
       </c>
-      <c r="I19" s="105">
+      <c r="I19" s="15">
         <v>7</v>
       </c>
-      <c r="J19" s="144">
+      <c r="J19" s="150">
         <f t="shared" si="2"/>
         <v>78.366103020198508</v>
       </c>
-      <c r="K19" s="17">
+      <c r="K19" s="146">
         <f t="shared" si="3"/>
         <v>0.60000000000000009</v>
       </c>
@@ -2851,14 +2904,14 @@
       <c r="H20" s="106">
         <v>0.4</v>
       </c>
-      <c r="I20" s="106">
+      <c r="I20" s="16">
         <v>7</v>
       </c>
-      <c r="J20" s="145">
+      <c r="J20" s="150">
         <f t="shared" si="2"/>
         <v>37.05597157097958</v>
       </c>
-      <c r="K20" s="18">
+      <c r="K20" s="147">
         <f t="shared" si="3"/>
         <v>0.45</v>
       </c>
@@ -2890,14 +2943,14 @@
       <c r="H21" s="13">
         <v>0.65</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="144">
         <v>7</v>
       </c>
-      <c r="J21" s="146">
+      <c r="J21" s="151">
         <f t="shared" si="2"/>
         <v>67.170945445884442</v>
       </c>
-      <c r="K21" s="14">
+      <c r="K21" s="148">
         <f t="shared" si="3"/>
         <v>0.70000000000000007</v>
       </c>
@@ -2915,7 +2968,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
@@ -2928,99 +2981,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="130" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="120" t="s">
+      <c r="B1" s="132" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="116" t="s">
+      <c r="C1" s="128" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="116" t="s">
+      <c r="D1" s="128" t="s">
         <v>33</v>
       </c>
-      <c r="E1" s="116"/>
-      <c r="F1" s="116" t="s">
+      <c r="E1" s="128"/>
+      <c r="F1" s="128" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="116" t="s">
+      <c r="G1" s="128" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="116" t="s">
+      <c r="H1" s="128" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="116" t="s">
+      <c r="I1" s="128" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="116" t="s">
+      <c r="J1" s="128" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="116" t="s">
+      <c r="K1" s="128" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="128" t="s">
+      <c r="L1" s="122" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="116" t="s">
+      <c r="M1" s="128" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="128" t="s">
+      <c r="N1" s="122" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="128" t="s">
+      <c r="O1" s="122" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="130" t="s">
+      <c r="P1" s="124" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="132" t="s">
+      <c r="Q1" s="126" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="119"/>
-      <c r="B2" s="121"/>
-      <c r="C2" s="117"/>
+      <c r="A2" s="131"/>
+      <c r="B2" s="133"/>
+      <c r="C2" s="129"/>
       <c r="D2" s="106" t="s">
         <v>34</v>
       </c>
       <c r="E2" s="106" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="117"/>
-      <c r="G2" s="117"/>
-      <c r="H2" s="117"/>
-      <c r="I2" s="117"/>
-      <c r="J2" s="117"/>
-      <c r="K2" s="117"/>
-      <c r="L2" s="129"/>
-      <c r="M2" s="117"/>
-      <c r="N2" s="129"/>
-      <c r="O2" s="129"/>
-      <c r="P2" s="131"/>
-      <c r="Q2" s="133"/>
+      <c r="F2" s="129"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="129"/>
+      <c r="I2" s="129"/>
+      <c r="J2" s="129"/>
+      <c r="K2" s="129"/>
+      <c r="L2" s="123"/>
+      <c r="M2" s="129"/>
+      <c r="N2" s="123"/>
+      <c r="O2" s="123"/>
+      <c r="P2" s="125"/>
+      <c r="Q2" s="127"/>
     </row>
     <row r="3" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="125" t="s">
+      <c r="A3" s="119" t="s">
         <v>134</v>
       </c>
-      <c r="B3" s="126"/>
-      <c r="C3" s="126"/>
-      <c r="D3" s="126"/>
-      <c r="E3" s="126"/>
-      <c r="F3" s="126"/>
-      <c r="G3" s="126"/>
-      <c r="H3" s="126"/>
-      <c r="I3" s="126"/>
-      <c r="J3" s="126"/>
-      <c r="K3" s="126"/>
-      <c r="L3" s="126"/>
-      <c r="M3" s="126"/>
-      <c r="N3" s="126"/>
-      <c r="O3" s="126"/>
-      <c r="P3" s="126"/>
-      <c r="Q3" s="127"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="120"/>
+      <c r="I3" s="120"/>
+      <c r="J3" s="120"/>
+      <c r="K3" s="120"/>
+      <c r="L3" s="120"/>
+      <c r="M3" s="120"/>
+      <c r="N3" s="120"/>
+      <c r="O3" s="120"/>
+      <c r="P3" s="120"/>
+      <c r="Q3" s="121"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="48">
@@ -3531,25 +3584,25 @@
       </c>
     </row>
     <row r="14" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="125" t="s">
+      <c r="A14" s="119" t="s">
         <v>135</v>
       </c>
-      <c r="B14" s="126"/>
-      <c r="C14" s="126"/>
-      <c r="D14" s="126"/>
-      <c r="E14" s="126"/>
-      <c r="F14" s="126"/>
-      <c r="G14" s="126"/>
-      <c r="H14" s="126"/>
-      <c r="I14" s="126"/>
-      <c r="J14" s="126"/>
-      <c r="K14" s="126"/>
-      <c r="L14" s="126"/>
-      <c r="M14" s="126"/>
-      <c r="N14" s="126"/>
-      <c r="O14" s="126"/>
-      <c r="P14" s="126"/>
-      <c r="Q14" s="127"/>
+      <c r="B14" s="120"/>
+      <c r="C14" s="120"/>
+      <c r="D14" s="120"/>
+      <c r="E14" s="120"/>
+      <c r="F14" s="120"/>
+      <c r="G14" s="120"/>
+      <c r="H14" s="120"/>
+      <c r="I14" s="120"/>
+      <c r="J14" s="120"/>
+      <c r="K14" s="120"/>
+      <c r="L14" s="120"/>
+      <c r="M14" s="120"/>
+      <c r="N14" s="120"/>
+      <c r="O14" s="120"/>
+      <c r="P14" s="120"/>
+      <c r="Q14" s="121"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="31">
@@ -4003,25 +4056,25 @@
       </c>
     </row>
     <row r="24" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="125" t="s">
+      <c r="A24" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="126"/>
-      <c r="C24" s="126"/>
-      <c r="D24" s="126"/>
-      <c r="E24" s="126"/>
-      <c r="F24" s="126"/>
-      <c r="G24" s="126"/>
-      <c r="H24" s="126"/>
-      <c r="I24" s="126"/>
-      <c r="J24" s="126"/>
-      <c r="K24" s="126"/>
-      <c r="L24" s="126"/>
-      <c r="M24" s="126"/>
-      <c r="N24" s="126"/>
-      <c r="O24" s="126"/>
-      <c r="P24" s="126"/>
-      <c r="Q24" s="127"/>
+      <c r="B24" s="120"/>
+      <c r="C24" s="120"/>
+      <c r="D24" s="120"/>
+      <c r="E24" s="120"/>
+      <c r="F24" s="120"/>
+      <c r="G24" s="120"/>
+      <c r="H24" s="120"/>
+      <c r="I24" s="120"/>
+      <c r="J24" s="120"/>
+      <c r="K24" s="120"/>
+      <c r="L24" s="120"/>
+      <c r="M24" s="120"/>
+      <c r="N24" s="120"/>
+      <c r="O24" s="120"/>
+      <c r="P24" s="120"/>
+      <c r="Q24" s="121"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="31">
@@ -4133,25 +4186,25 @@
       </c>
     </row>
     <row r="27" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="125" t="s">
+      <c r="A27" s="119" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="126"/>
-      <c r="C27" s="126"/>
-      <c r="D27" s="126"/>
-      <c r="E27" s="126"/>
-      <c r="F27" s="126"/>
-      <c r="G27" s="126"/>
-      <c r="H27" s="126"/>
-      <c r="I27" s="126"/>
-      <c r="J27" s="126"/>
-      <c r="K27" s="126"/>
-      <c r="L27" s="126"/>
-      <c r="M27" s="126"/>
-      <c r="N27" s="126"/>
-      <c r="O27" s="126"/>
-      <c r="P27" s="126"/>
-      <c r="Q27" s="127"/>
+      <c r="B27" s="120"/>
+      <c r="C27" s="120"/>
+      <c r="D27" s="120"/>
+      <c r="E27" s="120"/>
+      <c r="F27" s="120"/>
+      <c r="G27" s="120"/>
+      <c r="H27" s="120"/>
+      <c r="I27" s="120"/>
+      <c r="J27" s="120"/>
+      <c r="K27" s="120"/>
+      <c r="L27" s="120"/>
+      <c r="M27" s="120"/>
+      <c r="N27" s="120"/>
+      <c r="O27" s="120"/>
+      <c r="P27" s="120"/>
+      <c r="Q27" s="121"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="31">
@@ -4263,25 +4316,25 @@
       </c>
     </row>
     <row r="30" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="125" t="s">
+      <c r="A30" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="B30" s="126"/>
-      <c r="C30" s="126"/>
-      <c r="D30" s="126"/>
-      <c r="E30" s="126"/>
-      <c r="F30" s="126"/>
-      <c r="G30" s="126"/>
-      <c r="H30" s="126"/>
-      <c r="I30" s="126"/>
-      <c r="J30" s="126"/>
-      <c r="K30" s="126"/>
-      <c r="L30" s="126"/>
-      <c r="M30" s="126"/>
-      <c r="N30" s="126"/>
-      <c r="O30" s="126"/>
-      <c r="P30" s="126"/>
-      <c r="Q30" s="127"/>
+      <c r="B30" s="120"/>
+      <c r="C30" s="120"/>
+      <c r="D30" s="120"/>
+      <c r="E30" s="120"/>
+      <c r="F30" s="120"/>
+      <c r="G30" s="120"/>
+      <c r="H30" s="120"/>
+      <c r="I30" s="120"/>
+      <c r="J30" s="120"/>
+      <c r="K30" s="120"/>
+      <c r="L30" s="120"/>
+      <c r="M30" s="120"/>
+      <c r="N30" s="120"/>
+      <c r="O30" s="120"/>
+      <c r="P30" s="120"/>
+      <c r="Q30" s="121"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="31">
@@ -4462,25 +4515,25 @@
       </c>
     </row>
     <row r="34" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="122" t="s">
+      <c r="A34" s="116" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="123"/>
-      <c r="C34" s="123"/>
-      <c r="D34" s="123"/>
-      <c r="E34" s="123"/>
-      <c r="F34" s="123"/>
-      <c r="G34" s="123"/>
-      <c r="H34" s="123"/>
-      <c r="I34" s="123"/>
-      <c r="J34" s="123"/>
-      <c r="K34" s="123"/>
-      <c r="L34" s="123"/>
-      <c r="M34" s="123"/>
-      <c r="N34" s="123"/>
-      <c r="O34" s="123"/>
-      <c r="P34" s="123"/>
-      <c r="Q34" s="124"/>
+      <c r="B34" s="117"/>
+      <c r="C34" s="117"/>
+      <c r="D34" s="117"/>
+      <c r="E34" s="117"/>
+      <c r="F34" s="117"/>
+      <c r="G34" s="117"/>
+      <c r="H34" s="117"/>
+      <c r="I34" s="117"/>
+      <c r="J34" s="117"/>
+      <c r="K34" s="117"/>
+      <c r="L34" s="117"/>
+      <c r="M34" s="117"/>
+      <c r="N34" s="117"/>
+      <c r="O34" s="117"/>
+      <c r="P34" s="117"/>
+      <c r="Q34" s="118"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="4"/>
@@ -4756,6 +4809,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:F2"/>
     <mergeCell ref="A34:Q34"/>
     <mergeCell ref="A24:Q24"/>
     <mergeCell ref="A27:Q27"/>
@@ -4772,12 +4831,6 @@
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4988,22 +5041,22 @@
       <c r="O1" s="68"/>
     </row>
     <row r="2" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="116" t="s">
         <v>134</v>
       </c>
-      <c r="B2" s="123"/>
-      <c r="C2" s="123"/>
-      <c r="D2" s="123"/>
-      <c r="E2" s="123"/>
-      <c r="F2" s="123"/>
-      <c r="G2" s="123"/>
-      <c r="H2" s="123"/>
-      <c r="I2" s="123"/>
-      <c r="J2" s="123"/>
-      <c r="K2" s="123"/>
-      <c r="L2" s="123"/>
-      <c r="M2" s="123"/>
-      <c r="N2" s="124"/>
+      <c r="B2" s="117"/>
+      <c r="C2" s="117"/>
+      <c r="D2" s="117"/>
+      <c r="E2" s="117"/>
+      <c r="F2" s="117"/>
+      <c r="G2" s="117"/>
+      <c r="H2" s="117"/>
+      <c r="I2" s="117"/>
+      <c r="J2" s="117"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="117"/>
+      <c r="M2" s="117"/>
+      <c r="N2" s="118"/>
       <c r="O2" s="68"/>
       <c r="P2" t="s">
         <v>178</v>
@@ -5591,22 +5644,22 @@
       </c>
     </row>
     <row r="13" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="122" t="s">
+      <c r="A13" s="116" t="s">
         <v>135</v>
       </c>
-      <c r="B13" s="123"/>
-      <c r="C13" s="123"/>
-      <c r="D13" s="123"/>
-      <c r="E13" s="123"/>
-      <c r="F13" s="123"/>
-      <c r="G13" s="123"/>
-      <c r="H13" s="123"/>
-      <c r="I13" s="123"/>
-      <c r="J13" s="123"/>
-      <c r="K13" s="123"/>
-      <c r="L13" s="123"/>
-      <c r="M13" s="123"/>
-      <c r="N13" s="124"/>
+      <c r="B13" s="117"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117"/>
+      <c r="G13" s="117"/>
+      <c r="H13" s="117"/>
+      <c r="I13" s="117"/>
+      <c r="J13" s="117"/>
+      <c r="K13" s="117"/>
+      <c r="L13" s="117"/>
+      <c r="M13" s="117"/>
+      <c r="N13" s="118"/>
       <c r="O13" s="68"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
@@ -6131,22 +6184,22 @@
       </c>
     </row>
     <row r="23" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="122" t="s">
+      <c r="A23" s="116" t="s">
         <v>91</v>
       </c>
-      <c r="B23" s="123"/>
-      <c r="C23" s="123"/>
-      <c r="D23" s="123"/>
-      <c r="E23" s="123"/>
-      <c r="F23" s="123"/>
-      <c r="G23" s="123"/>
-      <c r="H23" s="123"/>
-      <c r="I23" s="123"/>
-      <c r="J23" s="123"/>
-      <c r="K23" s="123"/>
-      <c r="L23" s="123"/>
-      <c r="M23" s="123"/>
-      <c r="N23" s="124"/>
+      <c r="B23" s="117"/>
+      <c r="C23" s="117"/>
+      <c r="D23" s="117"/>
+      <c r="E23" s="117"/>
+      <c r="F23" s="117"/>
+      <c r="G23" s="117"/>
+      <c r="H23" s="117"/>
+      <c r="I23" s="117"/>
+      <c r="J23" s="117"/>
+      <c r="K23" s="117"/>
+      <c r="L23" s="117"/>
+      <c r="M23" s="117"/>
+      <c r="N23" s="118"/>
       <c r="O23" s="68"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
@@ -6344,22 +6397,22 @@
       </c>
     </row>
     <row r="27" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="122" t="s">
+      <c r="A27" s="116" t="s">
         <v>95</v>
       </c>
-      <c r="B27" s="123"/>
-      <c r="C27" s="123"/>
-      <c r="D27" s="123"/>
-      <c r="E27" s="123"/>
-      <c r="F27" s="123"/>
-      <c r="G27" s="123"/>
-      <c r="H27" s="123"/>
-      <c r="I27" s="123"/>
-      <c r="J27" s="123"/>
-      <c r="K27" s="123"/>
-      <c r="L27" s="123"/>
-      <c r="M27" s="123"/>
-      <c r="N27" s="124"/>
+      <c r="B27" s="117"/>
+      <c r="C27" s="117"/>
+      <c r="D27" s="117"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="117"/>
+      <c r="G27" s="117"/>
+      <c r="H27" s="117"/>
+      <c r="I27" s="117"/>
+      <c r="J27" s="117"/>
+      <c r="K27" s="117"/>
+      <c r="L27" s="117"/>
+      <c r="M27" s="117"/>
+      <c r="N27" s="118"/>
       <c r="O27" s="68"/>
     </row>
     <row r="28" spans="1:18" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>